<commit_message>
Create a table to store resource data
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB06A4F8-FFFB-4DB9-ADBC-1EEE5AF8B074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB491861-E494-411D-BEC7-05A7DD001E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
+    <sheet name="Create a table to storeResource" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
   <si>
     <t>構成</t>
   </si>
@@ -83,6 +84,45 @@
   </si>
   <si>
     <t>create_database.sql</t>
+  </si>
+  <si>
+    <t>Create a table to store resource data</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\create_database.sql</t>
+  </si>
+  <si>
+    <t>CREATE DATABASE api_db;</t>
+  </si>
+  <si>
+    <t>create_task_table.sql</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\create_task_table.sql</t>
+  </si>
+  <si>
+    <t>CREATE TABLE task (</t>
+  </si>
+  <si>
+    <t>    id INT NOT NULL AUTO_INCREMENT,</t>
+  </si>
+  <si>
+    <t>    name VARCHAR(128) NOT NULL,</t>
+  </si>
+  <si>
+    <t>    priority INT DEFAULT NULL,</t>
+  </si>
+  <si>
+    <t>    is_completed BOOLEAN NOT NULL DEFAULT FALSE,</t>
+  </si>
+  <si>
+    <t>    PRIMARY KEY (id),</t>
+  </si>
+  <si>
+    <t>    INDEX (name)</t>
+  </si>
+  <si>
+    <t>);</t>
   </si>
 </sst>
 </file>
@@ -205,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -216,8 +256,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -240,15 +281,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>608621</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>161436</xdr:rowOff>
+      <xdr:colOff>589571</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>180486</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -271,8 +312,57 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="704850" y="4819650"/>
+          <a:off x="685800" y="5600700"/>
           <a:ext cx="7828571" cy="3914286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>399086</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>37548</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7AA63D7-ACDC-1D37-5916-0292066F4E07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="7048500"/>
+          <a:ext cx="7714286" cy="4419048"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -547,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:J23"/>
+  <dimension ref="A4:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,7 +806,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B17" s="4"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -729,7 +819,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="4"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -742,7 +832,7 @@
       <c r="I18" s="9"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B19" s="4"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -755,12 +845,12 @@
       <c r="I19" s="9"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="11" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="9"/>
@@ -768,7 +858,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -781,7 +871,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -794,11 +884,11 @@
       <c r="I22" s="9"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F23" s="7"/>
@@ -807,9 +897,399 @@
       <c r="I23" s="7"/>
       <c r="J23" s="8"/>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6DC166-3C5B-44B6-AADB-1BB724337B91}">
+  <dimension ref="A2:J35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Connect to the database from PHP: add a Database class
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB491861-E494-411D-BEC7-05A7DD001E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5050583-D47E-4789-95C9-88B2E6E06D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
     <sheet name="Create a table to storeResource" sheetId="2" r:id="rId2"/>
+    <sheet name="Connect to the database fromPHP" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
   <si>
     <t>構成</t>
   </si>
@@ -123,6 +124,171 @@
   </si>
   <si>
     <t>);</t>
+  </si>
+  <si>
+    <t>Connect to the database from PHP: add a Database class</t>
+  </si>
+  <si>
+    <t>Database.php</t>
+  </si>
+  <si>
+    <t>→</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\src\Database.php</t>
+  </si>
+  <si>
+    <t>&lt;?php</t>
+  </si>
+  <si>
+    <t>class Database</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>    private $host;</t>
+  </si>
+  <si>
+    <t>    private $name;</t>
+  </si>
+  <si>
+    <t>    private $user;</t>
+  </si>
+  <si>
+    <t>    private $password;</t>
+  </si>
+  <si>
+    <t>    public function __construct(</t>
+  </si>
+  <si>
+    <t>        string $host,</t>
+  </si>
+  <si>
+    <t>        string $name,</t>
+  </si>
+  <si>
+    <t>        string $user,</t>
+  </si>
+  <si>
+    <t>        string $password</t>
+  </si>
+  <si>
+    <t>    ) {</t>
+  </si>
+  <si>
+    <t>        $this-&gt;host = $host;</t>
+  </si>
+  <si>
+    <t>        $this-&gt;name = $name;</t>
+  </si>
+  <si>
+    <t>        $this-&gt;user = $user;</t>
+  </si>
+  <si>
+    <t>        $this-&gt;password = $password;</t>
+  </si>
+  <si>
+    <t>    }</t>
+  </si>
+  <si>
+    <t>    public function getConnection(): PDO</t>
+  </si>
+  <si>
+    <t>    {</t>
+  </si>
+  <si>
+    <t>        $dsn = "mysql:host={$this-&gt;host};dbname={$this-&gt;name};charset=utf8";</t>
+  </si>
+  <si>
+    <t>        return new PDO($dsn, $this-&gt;user, $this-&gt;password, [</t>
+  </si>
+  <si>
+    <t>            PDO::ATTR_ERRMODE =&gt; PDO::ERRMODE_EXCEPTION</t>
+  </si>
+  <si>
+    <t>        ]);</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\api\index.php</t>
+  </si>
+  <si>
+    <t>declare(strict_types=1);</t>
+  </si>
+  <si>
+    <t>ini_set("display_errors", "On");</t>
+  </si>
+  <si>
+    <t>require dirname(__DIR__) . "/vendor/autoload.php";</t>
+  </si>
+  <si>
+    <t>set_exception_handler("ErrorHandler::handleException");</t>
+  </si>
+  <si>
+    <t>$path = parse_url($_SERVER["REQUEST_URI"], PHP_URL_PATH);</t>
+  </si>
+  <si>
+    <t>$parts = explode("/", $path);</t>
+  </si>
+  <si>
+    <t>$resource = $parts[2];</t>
+  </si>
+  <si>
+    <t>$id = $parts[3] ?? null;</t>
+  </si>
+  <si>
+    <t>if ($resource != "tasks") {</t>
+  </si>
+  <si>
+    <t>    http_response_code(404);</t>
+  </si>
+  <si>
+    <t>    exit;</t>
+  </si>
+  <si>
+    <t>header("Content-type: application/json; charset=UTF-8");</t>
+  </si>
+  <si>
+    <t>$database = new Database("localhost", "api_db", "root", "");</t>
+  </si>
+  <si>
+    <t>$database-&gt;getConnection();</t>
+  </si>
+  <si>
+    <t>$controller = new TaskController;</t>
+  </si>
+  <si>
+    <t>$controller-&gt;processRequest($_SERVER['REQUEST_METHOD'], $id);</t>
+  </si>
+  <si>
+    <t>Sử dụng PDO, ngoài ra có thể dùng mysqli</t>
+  </si>
+  <si>
+    <t>Khi connect DB bị lỗi thì trả về exception</t>
+  </si>
+  <si>
+    <t>Kết nối với DB</t>
+  </si>
+  <si>
+    <t>Check by call api</t>
+  </si>
+  <si>
+    <t>http://localhost/api/tasks</t>
+  </si>
+  <si>
+    <t>Vẫn gọi được api bình thường, ko có thông báo lỗi kết nối DB</t>
+  </si>
+  <si>
+    <t>Trường hợp ko kết nối được DB thì sẽ có thông báo lỗi trả về, ở đây mình check trường hợp nhập pwd sai thì sẽ ko kết nối được DB</t>
   </si>
 </sst>
 </file>
@@ -145,15 +311,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -241,11 +413,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -259,6 +511,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,6 +633,205 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{276483B9-2C6B-0C87-B5AE-7CE6657974BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1038225" y="5867400"/>
+          <a:ext cx="723900" cy="10791825"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>379745</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>94913</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2316052F-839A-4485-C621-948F31A32859}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="18926175"/>
+          <a:ext cx="10038095" cy="2695238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>494040</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>123415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4412BD2A-800E-D946-6B9F-11D1A93A5ED9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="22564725"/>
+          <a:ext cx="10076190" cy="3276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB5B4F5F-B8FB-9B87-A344-8EEBB7B6BFF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2857500" y="22440900"/>
+          <a:ext cx="5010150" cy="2447925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -927,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6DC166-3C5B-44B6-AADB-1BB724337B91}">
   <dimension ref="A2:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="R57" sqref="R57"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,4 +1755,1994 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0807E891-05D4-4189-A4AB-FEA17BF4CE1C}">
+  <dimension ref="A2:T138"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="L94" sqref="L94"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="5"/>
+      <c r="K17" t="s">
+        <v>34</v>
+      </c>
+      <c r="L17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="5"/>
+      <c r="K19" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="5"/>
+      <c r="J54" t="s">
+        <v>34</v>
+      </c>
+      <c r="K54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="5"/>
+      <c r="J55" t="s">
+        <v>34</v>
+      </c>
+      <c r="K55" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="I58" s="8"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="3"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B87" s="4"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B88" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B89" s="15"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B90" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="5"/>
+      <c r="J90" t="s">
+        <v>34</v>
+      </c>
+      <c r="K90" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B94" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="8"/>
+    </row>
+    <row r="96" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A97" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="18"/>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="18"/>
+      <c r="I97" s="18"/>
+      <c r="J97" s="18"/>
+      <c r="K97" s="18"/>
+      <c r="L97" s="18"/>
+      <c r="M97" s="18"/>
+      <c r="N97" s="18"/>
+      <c r="O97" s="18"/>
+      <c r="P97" s="18"/>
+      <c r="Q97" s="18"/>
+      <c r="R97" s="18"/>
+      <c r="S97" s="18"/>
+      <c r="T97" s="19"/>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A98" s="20"/>
+      <c r="B98" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
+      <c r="L98" s="2"/>
+      <c r="M98" s="2"/>
+      <c r="N98" s="2"/>
+      <c r="O98" s="2"/>
+      <c r="P98" s="2"/>
+      <c r="Q98" s="2"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="9"/>
+      <c r="T98" s="21"/>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A99" s="20"/>
+      <c r="B99" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="9"/>
+      <c r="O99" s="9"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="9"/>
+      <c r="R99" s="5"/>
+      <c r="S99" s="9"/>
+      <c r="T99" s="21"/>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A100" s="20"/>
+      <c r="B100" s="4"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="9"/>
+      <c r="J100" s="9"/>
+      <c r="K100" s="9"/>
+      <c r="L100" s="9"/>
+      <c r="M100" s="9"/>
+      <c r="N100" s="9"/>
+      <c r="O100" s="9"/>
+      <c r="P100" s="9"/>
+      <c r="Q100" s="9"/>
+      <c r="R100" s="5"/>
+      <c r="S100" s="9"/>
+      <c r="T100" s="21"/>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A101" s="20"/>
+      <c r="B101" s="4"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
+      <c r="L101" s="9"/>
+      <c r="M101" s="9"/>
+      <c r="N101" s="9"/>
+      <c r="O101" s="9"/>
+      <c r="P101" s="9"/>
+      <c r="Q101" s="9"/>
+      <c r="R101" s="5"/>
+      <c r="S101" s="9"/>
+      <c r="T101" s="21"/>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A102" s="20"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="9"/>
+      <c r="M102" s="9"/>
+      <c r="N102" s="9"/>
+      <c r="O102" s="9"/>
+      <c r="P102" s="9"/>
+      <c r="Q102" s="9"/>
+      <c r="R102" s="5"/>
+      <c r="S102" s="9"/>
+      <c r="T102" s="21"/>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A103" s="20"/>
+      <c r="B103" s="4"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
+      <c r="M103" s="9"/>
+      <c r="N103" s="9"/>
+      <c r="O103" s="9"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="9"/>
+      <c r="R103" s="5"/>
+      <c r="S103" s="9"/>
+      <c r="T103" s="21"/>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A104" s="20"/>
+      <c r="B104" s="4"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
+      <c r="L104" s="9"/>
+      <c r="M104" s="9"/>
+      <c r="N104" s="9"/>
+      <c r="O104" s="9"/>
+      <c r="P104" s="9"/>
+      <c r="Q104" s="9"/>
+      <c r="R104" s="5"/>
+      <c r="S104" s="9"/>
+      <c r="T104" s="21"/>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A105" s="20"/>
+      <c r="B105" s="4"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="9"/>
+      <c r="M105" s="9"/>
+      <c r="N105" s="9"/>
+      <c r="O105" s="9"/>
+      <c r="P105" s="9"/>
+      <c r="Q105" s="9"/>
+      <c r="R105" s="5"/>
+      <c r="S105" s="9"/>
+      <c r="T105" s="21"/>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A106" s="20"/>
+      <c r="B106" s="4"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
+      <c r="L106" s="9"/>
+      <c r="M106" s="9"/>
+      <c r="N106" s="9"/>
+      <c r="O106" s="9"/>
+      <c r="P106" s="9"/>
+      <c r="Q106" s="9"/>
+      <c r="R106" s="5"/>
+      <c r="S106" s="9"/>
+      <c r="T106" s="21"/>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A107" s="20"/>
+      <c r="B107" s="4"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
+      <c r="L107" s="9"/>
+      <c r="M107" s="9"/>
+      <c r="N107" s="9"/>
+      <c r="O107" s="9"/>
+      <c r="P107" s="9"/>
+      <c r="Q107" s="9"/>
+      <c r="R107" s="5"/>
+      <c r="S107" s="9"/>
+      <c r="T107" s="21"/>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A108" s="20"/>
+      <c r="B108" s="4"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
+      <c r="L108" s="9"/>
+      <c r="M108" s="9"/>
+      <c r="N108" s="9"/>
+      <c r="O108" s="9"/>
+      <c r="P108" s="9"/>
+      <c r="Q108" s="9"/>
+      <c r="R108" s="5"/>
+      <c r="S108" s="9"/>
+      <c r="T108" s="21"/>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A109" s="20"/>
+      <c r="B109" s="4"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="9"/>
+      <c r="H109" s="9"/>
+      <c r="I109" s="9"/>
+      <c r="J109" s="9"/>
+      <c r="K109" s="9"/>
+      <c r="L109" s="9"/>
+      <c r="M109" s="9"/>
+      <c r="N109" s="9"/>
+      <c r="O109" s="9"/>
+      <c r="P109" s="9"/>
+      <c r="Q109" s="9"/>
+      <c r="R109" s="5"/>
+      <c r="S109" s="9"/>
+      <c r="T109" s="21"/>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A110" s="20"/>
+      <c r="B110" s="4"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="9"/>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
+      <c r="L110" s="9"/>
+      <c r="M110" s="9"/>
+      <c r="N110" s="9"/>
+      <c r="O110" s="9"/>
+      <c r="P110" s="9"/>
+      <c r="Q110" s="9"/>
+      <c r="R110" s="5"/>
+      <c r="S110" s="9"/>
+      <c r="T110" s="21"/>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A111" s="20"/>
+      <c r="B111" s="4"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
+      <c r="I111" s="9"/>
+      <c r="J111" s="9"/>
+      <c r="K111" s="9"/>
+      <c r="L111" s="9"/>
+      <c r="M111" s="9"/>
+      <c r="N111" s="9"/>
+      <c r="O111" s="9"/>
+      <c r="P111" s="9"/>
+      <c r="Q111" s="9"/>
+      <c r="R111" s="5"/>
+      <c r="S111" s="9"/>
+      <c r="T111" s="21"/>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A112" s="20"/>
+      <c r="B112" s="4"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="9"/>
+      <c r="J112" s="9"/>
+      <c r="K112" s="9"/>
+      <c r="L112" s="9"/>
+      <c r="M112" s="9"/>
+      <c r="N112" s="9"/>
+      <c r="O112" s="9"/>
+      <c r="P112" s="9"/>
+      <c r="Q112" s="9"/>
+      <c r="R112" s="5"/>
+      <c r="S112" s="9"/>
+      <c r="T112" s="21"/>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A113" s="20"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="9"/>
+      <c r="H113" s="9"/>
+      <c r="I113" s="9"/>
+      <c r="J113" s="9"/>
+      <c r="K113" s="9"/>
+      <c r="L113" s="9"/>
+      <c r="M113" s="9"/>
+      <c r="N113" s="9"/>
+      <c r="O113" s="9"/>
+      <c r="P113" s="9"/>
+      <c r="Q113" s="9"/>
+      <c r="R113" s="5"/>
+      <c r="S113" s="9"/>
+      <c r="T113" s="21"/>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A114" s="20"/>
+      <c r="B114" s="4"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="9"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="9"/>
+      <c r="J114" s="9"/>
+      <c r="K114" s="9"/>
+      <c r="L114" s="9"/>
+      <c r="M114" s="9"/>
+      <c r="N114" s="9"/>
+      <c r="O114" s="9"/>
+      <c r="P114" s="9"/>
+      <c r="Q114" s="9"/>
+      <c r="R114" s="5"/>
+      <c r="S114" s="9"/>
+      <c r="T114" s="21"/>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A115" s="20"/>
+      <c r="B115" s="6"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7"/>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="7"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="7"/>
+      <c r="P115" s="7"/>
+      <c r="Q115" s="7"/>
+      <c r="R115" s="8"/>
+      <c r="S115" s="9"/>
+      <c r="T115" s="21"/>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A116" s="20"/>
+      <c r="B116" s="9"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="9"/>
+      <c r="K116" s="9"/>
+      <c r="L116" s="9"/>
+      <c r="M116" s="9"/>
+      <c r="N116" s="9"/>
+      <c r="O116" s="9"/>
+      <c r="P116" s="9"/>
+      <c r="Q116" s="9"/>
+      <c r="R116" s="9"/>
+      <c r="S116" s="9"/>
+      <c r="T116" s="21"/>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A117" s="20"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="9"/>
+      <c r="K117" s="9"/>
+      <c r="L117" s="9"/>
+      <c r="M117" s="9"/>
+      <c r="N117" s="9"/>
+      <c r="O117" s="9"/>
+      <c r="P117" s="9"/>
+      <c r="Q117" s="9"/>
+      <c r="R117" s="9"/>
+      <c r="S117" s="9"/>
+      <c r="T117" s="21"/>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A118" s="20"/>
+      <c r="B118" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2"/>
+      <c r="I118" s="2"/>
+      <c r="J118" s="2"/>
+      <c r="K118" s="2"/>
+      <c r="L118" s="2"/>
+      <c r="M118" s="2"/>
+      <c r="N118" s="2"/>
+      <c r="O118" s="2"/>
+      <c r="P118" s="2"/>
+      <c r="Q118" s="2"/>
+      <c r="R118" s="2"/>
+      <c r="S118" s="3"/>
+      <c r="T118" s="21"/>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A119" s="20"/>
+      <c r="B119" s="4"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="9"/>
+      <c r="K119" s="9"/>
+      <c r="L119" s="9"/>
+      <c r="M119" s="9"/>
+      <c r="N119" s="9"/>
+      <c r="O119" s="9"/>
+      <c r="P119" s="9"/>
+      <c r="Q119" s="9"/>
+      <c r="R119" s="9"/>
+      <c r="S119" s="5"/>
+      <c r="T119" s="21"/>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" s="20"/>
+      <c r="B120" s="4"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="9"/>
+      <c r="K120" s="9"/>
+      <c r="L120" s="9"/>
+      <c r="M120" s="9"/>
+      <c r="N120" s="9"/>
+      <c r="O120" s="9"/>
+      <c r="P120" s="9"/>
+      <c r="Q120" s="9"/>
+      <c r="R120" s="9"/>
+      <c r="S120" s="5"/>
+      <c r="T120" s="21"/>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A121" s="20"/>
+      <c r="B121" s="4"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
+      <c r="H121" s="9"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="9"/>
+      <c r="K121" s="9"/>
+      <c r="L121" s="9"/>
+      <c r="M121" s="9"/>
+      <c r="N121" s="9"/>
+      <c r="O121" s="9"/>
+      <c r="P121" s="9"/>
+      <c r="Q121" s="9"/>
+      <c r="R121" s="9"/>
+      <c r="S121" s="5"/>
+      <c r="T121" s="21"/>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A122" s="20"/>
+      <c r="B122" s="4"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="9"/>
+      <c r="H122" s="9"/>
+      <c r="I122" s="9"/>
+      <c r="J122" s="9"/>
+      <c r="K122" s="9"/>
+      <c r="L122" s="9"/>
+      <c r="M122" s="9"/>
+      <c r="N122" s="9"/>
+      <c r="O122" s="9"/>
+      <c r="P122" s="9"/>
+      <c r="Q122" s="9"/>
+      <c r="R122" s="9"/>
+      <c r="S122" s="5"/>
+      <c r="T122" s="21"/>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A123" s="20"/>
+      <c r="B123" s="4"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="9"/>
+      <c r="J123" s="9"/>
+      <c r="K123" s="9"/>
+      <c r="L123" s="9"/>
+      <c r="M123" s="9"/>
+      <c r="N123" s="9"/>
+      <c r="O123" s="9"/>
+      <c r="P123" s="9"/>
+      <c r="Q123" s="9"/>
+      <c r="R123" s="9"/>
+      <c r="S123" s="5"/>
+      <c r="T123" s="21"/>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A124" s="20"/>
+      <c r="B124" s="4"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="H124" s="9"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="9"/>
+      <c r="K124" s="9"/>
+      <c r="L124" s="9"/>
+      <c r="M124" s="9"/>
+      <c r="N124" s="9"/>
+      <c r="O124" s="9"/>
+      <c r="P124" s="9"/>
+      <c r="Q124" s="9"/>
+      <c r="R124" s="9"/>
+      <c r="S124" s="5"/>
+      <c r="T124" s="21"/>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A125" s="20"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="9"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="9"/>
+      <c r="J125" s="9"/>
+      <c r="K125" s="9"/>
+      <c r="L125" s="9"/>
+      <c r="M125" s="9"/>
+      <c r="N125" s="9"/>
+      <c r="O125" s="9"/>
+      <c r="P125" s="9"/>
+      <c r="Q125" s="9"/>
+      <c r="R125" s="9"/>
+      <c r="S125" s="5"/>
+      <c r="T125" s="21"/>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A126" s="20"/>
+      <c r="B126" s="4"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="9"/>
+      <c r="H126" s="9"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
+      <c r="L126" s="9"/>
+      <c r="M126" s="9"/>
+      <c r="N126" s="9"/>
+      <c r="O126" s="9"/>
+      <c r="P126" s="9"/>
+      <c r="Q126" s="9"/>
+      <c r="R126" s="9"/>
+      <c r="S126" s="5"/>
+      <c r="T126" s="21"/>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A127" s="20"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+      <c r="H127" s="9"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="9"/>
+      <c r="K127" s="9"/>
+      <c r="L127" s="9"/>
+      <c r="M127" s="9"/>
+      <c r="N127" s="9"/>
+      <c r="O127" s="9"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="9"/>
+      <c r="R127" s="9"/>
+      <c r="S127" s="5"/>
+      <c r="T127" s="21"/>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A128" s="20"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="9"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="9"/>
+      <c r="K128" s="9"/>
+      <c r="L128" s="9"/>
+      <c r="M128" s="9"/>
+      <c r="N128" s="9"/>
+      <c r="O128" s="9"/>
+      <c r="P128" s="9"/>
+      <c r="Q128" s="9"/>
+      <c r="R128" s="9"/>
+      <c r="S128" s="5"/>
+      <c r="T128" s="21"/>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+      <c r="H129" s="9"/>
+      <c r="I129" s="9"/>
+      <c r="J129" s="9"/>
+      <c r="K129" s="9"/>
+      <c r="L129" s="9"/>
+      <c r="M129" s="9"/>
+      <c r="N129" s="9"/>
+      <c r="O129" s="9"/>
+      <c r="P129" s="9"/>
+      <c r="Q129" s="9"/>
+      <c r="R129" s="9"/>
+      <c r="S129" s="5"/>
+      <c r="T129" s="21"/>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A130" s="20"/>
+      <c r="B130" s="4"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9"/>
+      <c r="H130" s="9"/>
+      <c r="I130" s="9"/>
+      <c r="J130" s="9"/>
+      <c r="K130" s="9"/>
+      <c r="L130" s="9"/>
+      <c r="M130" s="9"/>
+      <c r="N130" s="9"/>
+      <c r="O130" s="9"/>
+      <c r="P130" s="9"/>
+      <c r="Q130" s="9"/>
+      <c r="R130" s="9"/>
+      <c r="S130" s="5"/>
+      <c r="T130" s="21"/>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A131" s="20"/>
+      <c r="B131" s="4"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="9"/>
+      <c r="K131" s="9"/>
+      <c r="L131" s="9"/>
+      <c r="M131" s="9"/>
+      <c r="N131" s="9"/>
+      <c r="O131" s="9"/>
+      <c r="P131" s="9"/>
+      <c r="Q131" s="9"/>
+      <c r="R131" s="9"/>
+      <c r="S131" s="5"/>
+      <c r="T131" s="21"/>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A132" s="20"/>
+      <c r="B132" s="4"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="9"/>
+      <c r="K132" s="9"/>
+      <c r="L132" s="9"/>
+      <c r="M132" s="9"/>
+      <c r="N132" s="9"/>
+      <c r="O132" s="9"/>
+      <c r="P132" s="9"/>
+      <c r="Q132" s="9"/>
+      <c r="R132" s="9"/>
+      <c r="S132" s="5"/>
+      <c r="T132" s="21"/>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A133" s="20"/>
+      <c r="B133" s="4"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="9"/>
+      <c r="K133" s="9"/>
+      <c r="L133" s="9"/>
+      <c r="M133" s="9"/>
+      <c r="N133" s="9"/>
+      <c r="O133" s="9"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="9"/>
+      <c r="R133" s="9"/>
+      <c r="S133" s="5"/>
+      <c r="T133" s="21"/>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A134" s="20"/>
+      <c r="B134" s="4"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="9"/>
+      <c r="K134" s="9"/>
+      <c r="L134" s="9"/>
+      <c r="M134" s="9"/>
+      <c r="N134" s="9"/>
+      <c r="O134" s="9"/>
+      <c r="P134" s="9"/>
+      <c r="Q134" s="9"/>
+      <c r="R134" s="9"/>
+      <c r="S134" s="5"/>
+      <c r="T134" s="21"/>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A135" s="20"/>
+      <c r="B135" s="4"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="9"/>
+      <c r="N135" s="9"/>
+      <c r="O135" s="9"/>
+      <c r="P135" s="9"/>
+      <c r="Q135" s="9"/>
+      <c r="R135" s="9"/>
+      <c r="S135" s="5"/>
+      <c r="T135" s="21"/>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A136" s="20"/>
+      <c r="B136" s="4"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="9"/>
+      <c r="K136" s="9"/>
+      <c r="L136" s="9"/>
+      <c r="M136" s="9"/>
+      <c r="N136" s="9"/>
+      <c r="O136" s="9"/>
+      <c r="P136" s="9"/>
+      <c r="Q136" s="9"/>
+      <c r="R136" s="9"/>
+      <c r="S136" s="5"/>
+      <c r="T136" s="21"/>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A137" s="20"/>
+      <c r="B137" s="6"/>
+      <c r="C137" s="7"/>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7"/>
+      <c r="G137" s="7"/>
+      <c r="H137" s="7"/>
+      <c r="I137" s="7"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
+      <c r="L137" s="7"/>
+      <c r="M137" s="7"/>
+      <c r="N137" s="7"/>
+      <c r="O137" s="7"/>
+      <c r="P137" s="7"/>
+      <c r="Q137" s="7"/>
+      <c r="R137" s="7"/>
+      <c r="S137" s="8"/>
+      <c r="T137" s="21"/>
+    </row>
+    <row r="138" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="22"/>
+      <c r="B138" s="23"/>
+      <c r="C138" s="23"/>
+      <c r="D138" s="23"/>
+      <c r="E138" s="23"/>
+      <c r="F138" s="23"/>
+      <c r="G138" s="23"/>
+      <c r="H138" s="23"/>
+      <c r="I138" s="23"/>
+      <c r="J138" s="23"/>
+      <c r="K138" s="23"/>
+      <c r="L138" s="23"/>
+      <c r="M138" s="23"/>
+      <c r="N138" s="23"/>
+      <c r="O138" s="23"/>
+      <c r="P138" s="23"/>
+      <c r="Q138" s="23"/>
+      <c r="R138" s="23"/>
+      <c r="S138" s="23"/>
+      <c r="T138" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Move the database connection data to a separate .env file
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5050583-D47E-4789-95C9-88B2E6E06D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D6704D-95CB-44CC-8236-E277A6072DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
     <sheet name="Create a table to storeResource" sheetId="2" r:id="rId2"/>
     <sheet name="Connect to the database fromPHP" sheetId="3" r:id="rId3"/>
+    <sheet name=".env file" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
   <si>
     <t>構成</t>
   </si>
@@ -289,13 +290,85 @@
   </si>
   <si>
     <t>Trường hợp ko kết nối được DB thì sẽ có thông báo lỗi trả về, ở đây mình check trường hợp nhập pwd sai thì sẽ ko kết nối được DB</t>
+  </si>
+  <si>
+    <t>Move the database connection data to a separate .env file</t>
+  </si>
+  <si>
+    <t>Các thông tin liên quan đến Database thì sẽ lưu trong file .env để lưu các biến môi trường</t>
+  </si>
+  <si>
+    <t>vlucas/phpdotenv</t>
+  </si>
+  <si>
+    <t>https://packagist.org/packages/vlucas/phpdotenv</t>
+  </si>
+  <si>
+    <t>Load các biến môi trường trong file .env bằng vlucas/phpdotenv</t>
+  </si>
+  <si>
+    <t>Installation</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>composer require vlucas/phpdotenv</t>
+  </si>
+  <si>
+    <t>.env</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\.env</t>
+  </si>
+  <si>
+    <t>DB_HOST="localhost"</t>
+  </si>
+  <si>
+    <t>DB_NAME="api_db"</t>
+  </si>
+  <si>
+    <t>DB_USER="root"</t>
+  </si>
+  <si>
+    <t>DB_PASS=""</t>
+  </si>
+  <si>
+    <t>$dotenv = Dotenv\Dotenv::createImmutable(dirname(__DIR__));</t>
+  </si>
+  <si>
+    <t>$dotenv-&gt;load();</t>
+  </si>
+  <si>
+    <t>$database = new Database($_ENV["DB_HOST"], $_ENV["DB_NAME"], $_ENV["DB_USER"], $_ENV["DB_PASS"]);</t>
+  </si>
+  <si>
+    <t>Tham số truyền vào của phương thức createImmutable() là path của folder chứa file .env</t>
+  </si>
+  <si>
+    <t>Load các giá trị trong file .env vào biến môi trường của PHP $_ENV</t>
+  </si>
+  <si>
+    <t>Check call api</t>
+  </si>
+  <si>
+    <t>api vẫn gọi được bình thường và ko có thông báo lỗi có nghĩa là việc kết nối với DB ko có vấn đề gì</t>
+  </si>
+  <si>
+    <t>Trường hợp ko kết nối được DB thì sẽ có thông báo lỗi trả về, ở đây mình check trường hợp nhập pwd trong .env sai thì sẽ ko kết nối được DB</t>
+  </si>
+  <si>
+    <t>Sau khi check kết nối DB thành công bằng cách gọi api thì có thể bỏ dòng này</t>
+  </si>
+  <si>
+    <t>Đến đây thì việc kiểm tra kết nối DB đã hoàn tất</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -310,8 +383,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +400,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -497,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -523,6 +608,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,6 +927,593 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>51795</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2004ECBC-2B5D-6D6F-79CA-DE42E315FBA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723900" y="1428751"/>
+          <a:ext cx="11268075" cy="3957044"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>218380</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>161717</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{817B08E1-361E-495B-48E8-A2B480CDCF7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="5924550"/>
+          <a:ext cx="5561905" cy="1666667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>236736</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>170796</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3CB11662-5C04-BACE-4BFC-E15899A9CBB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="8086725"/>
+          <a:ext cx="11114286" cy="5228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD6C76FC-5943-4DFC-0B66-78F9515FAC4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="514350" y="6915150"/>
+          <a:ext cx="981075" cy="7410450"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>160851</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>65837</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B09FE24-A545-A304-FD5C-A4D0790F1365}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="14525625"/>
+          <a:ext cx="8590476" cy="6704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{682096BE-8C9D-4D04-9CDD-A150B6F2A2AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2543175" y="30099000"/>
+          <a:ext cx="9067800" cy="3286125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Arrow Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{221447AF-1F0D-1879-42A3-D009B174D8D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2162175" y="33909000"/>
+          <a:ext cx="2276475" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>417842</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>132959</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8466422A-CC5F-4C43-CDE9-AF9DEFD96D9D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="35699700"/>
+          <a:ext cx="10066667" cy="3123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>208</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>494040</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>123415</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0651D6E-54A3-44DB-82DA-1F59AB03C7D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="22574250"/>
+          <a:ext cx="10076190" cy="3276190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD0A15A9-6EA1-4AE2-A611-62EE0F8820DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2857500" y="22450425"/>
+          <a:ext cx="5010150" cy="2447925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>177</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>227</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6C73CE7-E2DA-8EF2-D554-00BF2E1EC6B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3419475" y="33918525"/>
+          <a:ext cx="4533900" cy="9439275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54FE1C15-4C27-8F17-9A0F-FDFA14439E91}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="476250" y="14497050"/>
+          <a:ext cx="457200" cy="15268575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1761,8 +2438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0807E891-05D4-4189-A4AB-FEA17BF4CE1C}">
   <dimension ref="A2:T138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="L94" sqref="L94"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B118" sqref="B118:R136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3745,4 +4422,3441 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C56BAC-8DE4-497E-995C-01E4CC964831}">
+  <dimension ref="A2:U229"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="L157" sqref="L157"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="19"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="21"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="21"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="21"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="21"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="21"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="21"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="21"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="21"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="21"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="21"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="21"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="21"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="21"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="21"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="21"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="21"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="21"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="21"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="21"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="21"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="21"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="21"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="21"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="21"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="21"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="21"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="21"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="21"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="21"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="21"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="21"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="21"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="21"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="21"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="21"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="21"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+      <c r="B43" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="21"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="21"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A45" s="20"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
+      <c r="S45" s="9"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="21"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A46" s="20"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="21"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="21"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="4"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="21"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="5"/>
+      <c r="U49" s="21"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="21"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A51" s="20"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="5"/>
+      <c r="U51" s="21"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="20"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="9"/>
+      <c r="S52" s="9"/>
+      <c r="T52" s="5"/>
+      <c r="U52" s="21"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="20"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
+      <c r="T53" s="5"/>
+      <c r="U53" s="21"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="9"/>
+      <c r="S54" s="9"/>
+      <c r="T54" s="5"/>
+      <c r="U54" s="21"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A55" s="20"/>
+      <c r="B55" s="4"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="9"/>
+      <c r="S55" s="9"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="21"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="9"/>
+      <c r="S56" s="9"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="21"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="20"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="9"/>
+      <c r="R57" s="9"/>
+      <c r="S57" s="9"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="21"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="20"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
+      <c r="Q58" s="9"/>
+      <c r="R58" s="9"/>
+      <c r="S58" s="9"/>
+      <c r="T58" s="5"/>
+      <c r="U58" s="21"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="20"/>
+      <c r="B59" s="4"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="O59" s="9"/>
+      <c r="P59" s="9"/>
+      <c r="Q59" s="9"/>
+      <c r="R59" s="9"/>
+      <c r="S59" s="9"/>
+      <c r="T59" s="5"/>
+      <c r="U59" s="21"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="20"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
+      <c r="R60" s="9"/>
+      <c r="S60" s="9"/>
+      <c r="T60" s="5"/>
+      <c r="U60" s="21"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A61" s="20"/>
+      <c r="B61" s="4"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+      <c r="O61" s="9"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="9"/>
+      <c r="R61" s="9"/>
+      <c r="S61" s="9"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="21"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A62" s="20"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+      <c r="O62" s="9"/>
+      <c r="P62" s="9"/>
+      <c r="Q62" s="9"/>
+      <c r="R62" s="9"/>
+      <c r="S62" s="9"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="21"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A63" s="20"/>
+      <c r="B63" s="4"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+      <c r="O63" s="9"/>
+      <c r="P63" s="9"/>
+      <c r="Q63" s="9"/>
+      <c r="R63" s="9"/>
+      <c r="S63" s="9"/>
+      <c r="T63" s="5"/>
+      <c r="U63" s="21"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A64" s="20"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="9"/>
+      <c r="S64" s="9"/>
+      <c r="T64" s="5"/>
+      <c r="U64" s="21"/>
+    </row>
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A65" s="20"/>
+      <c r="B65" s="4"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="9"/>
+      <c r="S65" s="9"/>
+      <c r="T65" s="5"/>
+      <c r="U65" s="21"/>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A66" s="20"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+      <c r="O66" s="9"/>
+      <c r="P66" s="9"/>
+      <c r="Q66" s="9"/>
+      <c r="R66" s="9"/>
+      <c r="S66" s="9"/>
+      <c r="T66" s="5"/>
+      <c r="U66" s="21"/>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="O67" s="9"/>
+      <c r="P67" s="9"/>
+      <c r="Q67" s="9"/>
+      <c r="R67" s="9"/>
+      <c r="S67" s="9"/>
+      <c r="T67" s="5"/>
+      <c r="U67" s="21"/>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A68" s="20"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="9"/>
+      <c r="S68" s="9"/>
+      <c r="T68" s="5"/>
+      <c r="U68" s="21"/>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A69" s="20"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="9"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="9"/>
+      <c r="R69" s="9"/>
+      <c r="S69" s="9"/>
+      <c r="T69" s="5"/>
+      <c r="U69" s="21"/>
+    </row>
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A70" s="20"/>
+      <c r="B70" s="4"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+      <c r="O70" s="9"/>
+      <c r="P70" s="9"/>
+      <c r="Q70" s="9"/>
+      <c r="R70" s="9"/>
+      <c r="S70" s="9"/>
+      <c r="T70" s="5"/>
+      <c r="U70" s="21"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A71" s="20"/>
+      <c r="B71" s="4"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="9"/>
+      <c r="R71" s="9"/>
+      <c r="S71" s="9"/>
+      <c r="T71" s="5"/>
+      <c r="U71" s="21"/>
+    </row>
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A72" s="20"/>
+      <c r="B72" s="6"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="7"/>
+      <c r="R72" s="7"/>
+      <c r="S72" s="7"/>
+      <c r="T72" s="8"/>
+      <c r="U72" s="21"/>
+    </row>
+    <row r="73" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="22"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="23"/>
+      <c r="H73" s="23"/>
+      <c r="I73" s="23"/>
+      <c r="J73" s="23"/>
+      <c r="K73" s="23"/>
+      <c r="L73" s="23"/>
+      <c r="M73" s="23"/>
+      <c r="N73" s="23"/>
+      <c r="O73" s="23"/>
+      <c r="P73" s="23"/>
+      <c r="Q73" s="23"/>
+      <c r="R73" s="23"/>
+      <c r="S73" s="23"/>
+      <c r="T73" s="23"/>
+      <c r="U73" s="24"/>
+    </row>
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2"/>
+      <c r="I115" s="2"/>
+      <c r="J115" s="3"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+      <c r="C116" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="5"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B117" s="4"/>
+      <c r="C117" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="5"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+      <c r="C118" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="5"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B119" s="4"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="5"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="5"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B121" s="4"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
+      <c r="H121" s="9"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="5"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="9"/>
+      <c r="H122" s="9"/>
+      <c r="I122" s="9"/>
+      <c r="J122" s="5"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="4"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="9"/>
+      <c r="J123" s="5"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="H124" s="9"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="5"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B125" s="4"/>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" s="9"/>
+      <c r="G125" s="9"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="9"/>
+      <c r="J125" s="5"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B126" s="4"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G126" s="9"/>
+      <c r="H126" s="9"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="5"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B127" s="4"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G127" s="9"/>
+      <c r="H127" s="9"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="5"/>
+      <c r="K127" t="s">
+        <v>34</v>
+      </c>
+      <c r="L127" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B128" s="4"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="9"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="5"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B129" s="4"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G129" s="9"/>
+      <c r="H129" s="9"/>
+      <c r="I129" s="9"/>
+      <c r="J129" s="5"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B130" s="4"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G130" s="9"/>
+      <c r="H130" s="9"/>
+      <c r="I130" s="9"/>
+      <c r="J130" s="5"/>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B131" s="4"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="5"/>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="5"/>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B133" s="4"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="5"/>
+      <c r="K133" t="s">
+        <v>34</v>
+      </c>
+      <c r="L133" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B134" s="4"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="5"/>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B135" s="4"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="5"/>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B136" s="6"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F136" s="7"/>
+      <c r="G136" s="7"/>
+      <c r="H136" s="7"/>
+      <c r="I136" s="7"/>
+      <c r="J136" s="8"/>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B140" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="5"/>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="5"/>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B143" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C143" s="7"/>
+      <c r="D143" s="7"/>
+      <c r="E143" s="8"/>
+    </row>
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B147" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+      <c r="H147" s="2"/>
+      <c r="I147" s="2"/>
+      <c r="J147" s="2"/>
+      <c r="K147" s="2"/>
+      <c r="L147" s="3"/>
+    </row>
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B148" s="4"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="9"/>
+      <c r="K148" s="9"/>
+      <c r="L148" s="5"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="9"/>
+      <c r="I149" s="9"/>
+      <c r="J149" s="9"/>
+      <c r="K149" s="9"/>
+      <c r="L149" s="5"/>
+    </row>
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B150" s="4"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="9"/>
+      <c r="L150" s="5"/>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+      <c r="H151" s="9"/>
+      <c r="I151" s="9"/>
+      <c r="J151" s="9"/>
+      <c r="K151" s="9"/>
+      <c r="L151" s="5"/>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B152" s="4"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+      <c r="H152" s="9"/>
+      <c r="I152" s="9"/>
+      <c r="J152" s="9"/>
+      <c r="K152" s="9"/>
+      <c r="L152" s="5"/>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9"/>
+      <c r="L153" s="5"/>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B154" s="4"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="9"/>
+      <c r="J154" s="9"/>
+      <c r="K154" s="9"/>
+      <c r="L154" s="5"/>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+      <c r="H155" s="9"/>
+      <c r="I155" s="9"/>
+      <c r="J155" s="9"/>
+      <c r="K155" s="9"/>
+      <c r="L155" s="5"/>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="9"/>
+      <c r="J156" s="9"/>
+      <c r="K156" s="9"/>
+      <c r="L156" s="5"/>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B157" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
+      <c r="G157" s="9"/>
+      <c r="H157" s="9"/>
+      <c r="I157" s="9"/>
+      <c r="J157" s="9"/>
+      <c r="K157" s="9"/>
+      <c r="L157" s="5"/>
+      <c r="M157" t="s">
+        <v>34</v>
+      </c>
+      <c r="N157" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B158" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9"/>
+      <c r="G158" s="9"/>
+      <c r="H158" s="9"/>
+      <c r="I158" s="9"/>
+      <c r="J158" s="9"/>
+      <c r="K158" s="9"/>
+      <c r="L158" s="5"/>
+      <c r="M158" t="s">
+        <v>34</v>
+      </c>
+      <c r="N158" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B159" s="4"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="9"/>
+      <c r="H159" s="9"/>
+      <c r="I159" s="9"/>
+      <c r="J159" s="9"/>
+      <c r="K159" s="9"/>
+      <c r="L159" s="5"/>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B160" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
+      <c r="G160" s="9"/>
+      <c r="H160" s="9"/>
+      <c r="I160" s="9"/>
+      <c r="J160" s="9"/>
+      <c r="K160" s="9"/>
+      <c r="L160" s="5"/>
+    </row>
+    <row r="161" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B161" s="4"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="9"/>
+      <c r="H161" s="9"/>
+      <c r="I161" s="9"/>
+      <c r="J161" s="9"/>
+      <c r="K161" s="9"/>
+      <c r="L161" s="5"/>
+    </row>
+    <row r="162" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="9"/>
+      <c r="J162" s="9"/>
+      <c r="K162" s="9"/>
+      <c r="L162" s="5"/>
+    </row>
+    <row r="163" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B163" s="4"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
+      <c r="H163" s="9"/>
+      <c r="I163" s="9"/>
+      <c r="J163" s="9"/>
+      <c r="K163" s="9"/>
+      <c r="L163" s="5"/>
+    </row>
+    <row r="164" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B164" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
+      <c r="G164" s="9"/>
+      <c r="H164" s="9"/>
+      <c r="I164" s="9"/>
+      <c r="J164" s="9"/>
+      <c r="K164" s="9"/>
+      <c r="L164" s="5"/>
+    </row>
+    <row r="165" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B165" s="4"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
+      <c r="G165" s="9"/>
+      <c r="H165" s="9"/>
+      <c r="I165" s="9"/>
+      <c r="J165" s="9"/>
+      <c r="K165" s="9"/>
+      <c r="L165" s="5"/>
+    </row>
+    <row r="166" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B166" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C166" s="9"/>
+      <c r="D166" s="9"/>
+      <c r="E166" s="9"/>
+      <c r="F166" s="9"/>
+      <c r="G166" s="9"/>
+      <c r="H166" s="9"/>
+      <c r="I166" s="9"/>
+      <c r="J166" s="9"/>
+      <c r="K166" s="9"/>
+      <c r="L166" s="5"/>
+    </row>
+    <row r="167" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B167" s="4"/>
+      <c r="C167" s="9"/>
+      <c r="D167" s="9"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
+      <c r="G167" s="9"/>
+      <c r="H167" s="9"/>
+      <c r="I167" s="9"/>
+      <c r="J167" s="9"/>
+      <c r="K167" s="9"/>
+      <c r="L167" s="5"/>
+    </row>
+    <row r="168" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B168" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C168" s="9"/>
+      <c r="D168" s="9"/>
+      <c r="E168" s="9"/>
+      <c r="F168" s="9"/>
+      <c r="G168" s="9"/>
+      <c r="H168" s="9"/>
+      <c r="I168" s="9"/>
+      <c r="J168" s="9"/>
+      <c r="K168" s="9"/>
+      <c r="L168" s="5"/>
+    </row>
+    <row r="169" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B169" s="4"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="9"/>
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
+      <c r="G169" s="9"/>
+      <c r="H169" s="9"/>
+      <c r="I169" s="9"/>
+      <c r="J169" s="9"/>
+      <c r="K169" s="9"/>
+      <c r="L169" s="5"/>
+    </row>
+    <row r="170" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B170" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
+      <c r="G170" s="9"/>
+      <c r="H170" s="9"/>
+      <c r="I170" s="9"/>
+      <c r="J170" s="9"/>
+      <c r="K170" s="9"/>
+      <c r="L170" s="5"/>
+    </row>
+    <row r="171" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B171" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C171" s="9"/>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
+      <c r="G171" s="9"/>
+      <c r="H171" s="9"/>
+      <c r="I171" s="9"/>
+      <c r="J171" s="9"/>
+      <c r="K171" s="9"/>
+      <c r="L171" s="5"/>
+    </row>
+    <row r="172" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B172" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
+      <c r="G172" s="9"/>
+      <c r="H172" s="9"/>
+      <c r="I172" s="9"/>
+      <c r="J172" s="9"/>
+      <c r="K172" s="9"/>
+      <c r="L172" s="5"/>
+    </row>
+    <row r="173" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B173" s="4"/>
+      <c r="C173" s="9"/>
+      <c r="D173" s="9"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="9"/>
+      <c r="G173" s="9"/>
+      <c r="H173" s="9"/>
+      <c r="I173" s="9"/>
+      <c r="J173" s="9"/>
+      <c r="K173" s="9"/>
+      <c r="L173" s="5"/>
+    </row>
+    <row r="174" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B174" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C174" s="9"/>
+      <c r="D174" s="9"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="9"/>
+      <c r="H174" s="9"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="9"/>
+      <c r="K174" s="9"/>
+      <c r="L174" s="5"/>
+    </row>
+    <row r="175" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B175" s="4"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="9"/>
+      <c r="H175" s="9"/>
+      <c r="I175" s="9"/>
+      <c r="J175" s="9"/>
+      <c r="K175" s="9"/>
+      <c r="L175" s="5"/>
+    </row>
+    <row r="176" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B176" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C176" s="9"/>
+      <c r="D176" s="9"/>
+      <c r="E176" s="9"/>
+      <c r="F176" s="9"/>
+      <c r="G176" s="9"/>
+      <c r="H176" s="9"/>
+      <c r="I176" s="9"/>
+      <c r="J176" s="9"/>
+      <c r="K176" s="9"/>
+      <c r="L176" s="5"/>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B177" s="4"/>
+      <c r="C177" s="9"/>
+      <c r="D177" s="9"/>
+      <c r="E177" s="9"/>
+      <c r="F177" s="9"/>
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+      <c r="I177" s="9"/>
+      <c r="J177" s="9"/>
+      <c r="K177" s="9"/>
+      <c r="L177" s="5"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B178" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C178" s="29"/>
+      <c r="D178" s="29"/>
+      <c r="E178" s="9"/>
+      <c r="F178" s="9"/>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="9"/>
+      <c r="K178" s="9"/>
+      <c r="L178" s="5"/>
+      <c r="M178" t="s">
+        <v>34</v>
+      </c>
+      <c r="N178" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B179" s="4"/>
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+      <c r="I179" s="9"/>
+      <c r="J179" s="9"/>
+      <c r="K179" s="9"/>
+      <c r="L179" s="5"/>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B180" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C180" s="9"/>
+      <c r="D180" s="9"/>
+      <c r="E180" s="9"/>
+      <c r="F180" s="9"/>
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+      <c r="I180" s="9"/>
+      <c r="J180" s="9"/>
+      <c r="K180" s="9"/>
+      <c r="L180" s="5"/>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B181" s="4"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="9"/>
+      <c r="E181" s="9"/>
+      <c r="F181" s="9"/>
+      <c r="G181" s="9"/>
+      <c r="H181" s="9"/>
+      <c r="I181" s="9"/>
+      <c r="J181" s="9"/>
+      <c r="K181" s="9"/>
+      <c r="L181" s="5"/>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B182" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C182" s="7"/>
+      <c r="D182" s="7"/>
+      <c r="E182" s="7"/>
+      <c r="F182" s="7"/>
+      <c r="G182" s="7"/>
+      <c r="H182" s="7"/>
+      <c r="I182" s="7"/>
+      <c r="J182" s="7"/>
+      <c r="K182" s="7"/>
+      <c r="L182" s="8"/>
+    </row>
+    <row r="184" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A185" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B185" s="18"/>
+      <c r="C185" s="18"/>
+      <c r="D185" s="18"/>
+      <c r="E185" s="18"/>
+      <c r="F185" s="18"/>
+      <c r="G185" s="18"/>
+      <c r="H185" s="18"/>
+      <c r="I185" s="18"/>
+      <c r="J185" s="18"/>
+      <c r="K185" s="18"/>
+      <c r="L185" s="18"/>
+      <c r="M185" s="18"/>
+      <c r="N185" s="18"/>
+      <c r="O185" s="18"/>
+      <c r="P185" s="18"/>
+      <c r="Q185" s="18"/>
+      <c r="R185" s="18"/>
+      <c r="S185" s="19"/>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A186" s="20"/>
+      <c r="B186" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
+      <c r="E186" s="2"/>
+      <c r="F186" s="2"/>
+      <c r="G186" s="2"/>
+      <c r="H186" s="2"/>
+      <c r="I186" s="2"/>
+      <c r="J186" s="2"/>
+      <c r="K186" s="2"/>
+      <c r="L186" s="2"/>
+      <c r="M186" s="2"/>
+      <c r="N186" s="2"/>
+      <c r="O186" s="2"/>
+      <c r="P186" s="2"/>
+      <c r="Q186" s="2"/>
+      <c r="R186" s="3"/>
+      <c r="S186" s="21"/>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A187" s="20"/>
+      <c r="B187" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C187" s="9"/>
+      <c r="D187" s="9"/>
+      <c r="E187" s="9"/>
+      <c r="F187" s="9"/>
+      <c r="G187" s="9"/>
+      <c r="H187" s="9"/>
+      <c r="I187" s="9"/>
+      <c r="J187" s="9"/>
+      <c r="K187" s="9"/>
+      <c r="L187" s="9"/>
+      <c r="M187" s="9"/>
+      <c r="N187" s="9"/>
+      <c r="O187" s="9"/>
+      <c r="P187" s="9"/>
+      <c r="Q187" s="9"/>
+      <c r="R187" s="5"/>
+      <c r="S187" s="21"/>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A188" s="20"/>
+      <c r="B188" s="4"/>
+      <c r="C188" s="9"/>
+      <c r="D188" s="9"/>
+      <c r="E188" s="9"/>
+      <c r="F188" s="9"/>
+      <c r="G188" s="9"/>
+      <c r="H188" s="9"/>
+      <c r="I188" s="9"/>
+      <c r="J188" s="9"/>
+      <c r="K188" s="9"/>
+      <c r="L188" s="9"/>
+      <c r="M188" s="9"/>
+      <c r="N188" s="9"/>
+      <c r="O188" s="9"/>
+      <c r="P188" s="9"/>
+      <c r="Q188" s="9"/>
+      <c r="R188" s="5"/>
+      <c r="S188" s="21"/>
+    </row>
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A189" s="20"/>
+      <c r="B189" s="4"/>
+      <c r="C189" s="9"/>
+      <c r="D189" s="9"/>
+      <c r="E189" s="9"/>
+      <c r="F189" s="9"/>
+      <c r="G189" s="9"/>
+      <c r="H189" s="9"/>
+      <c r="I189" s="9"/>
+      <c r="J189" s="9"/>
+      <c r="K189" s="9"/>
+      <c r="L189" s="9"/>
+      <c r="M189" s="9"/>
+      <c r="N189" s="9"/>
+      <c r="O189" s="9"/>
+      <c r="P189" s="9"/>
+      <c r="Q189" s="9"/>
+      <c r="R189" s="5"/>
+      <c r="S189" s="21"/>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A190" s="20"/>
+      <c r="B190" s="4"/>
+      <c r="C190" s="9"/>
+      <c r="D190" s="9"/>
+      <c r="E190" s="9"/>
+      <c r="F190" s="9"/>
+      <c r="G190" s="9"/>
+      <c r="H190" s="9"/>
+      <c r="I190" s="9"/>
+      <c r="J190" s="9"/>
+      <c r="K190" s="9"/>
+      <c r="L190" s="9"/>
+      <c r="M190" s="9"/>
+      <c r="N190" s="9"/>
+      <c r="O190" s="9"/>
+      <c r="P190" s="9"/>
+      <c r="Q190" s="9"/>
+      <c r="R190" s="5"/>
+      <c r="S190" s="21"/>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A191" s="20"/>
+      <c r="B191" s="4"/>
+      <c r="C191" s="9"/>
+      <c r="D191" s="9"/>
+      <c r="E191" s="9"/>
+      <c r="F191" s="9"/>
+      <c r="G191" s="9"/>
+      <c r="H191" s="9"/>
+      <c r="I191" s="9"/>
+      <c r="J191" s="9"/>
+      <c r="K191" s="9"/>
+      <c r="L191" s="9"/>
+      <c r="M191" s="9"/>
+      <c r="N191" s="9"/>
+      <c r="O191" s="9"/>
+      <c r="P191" s="9"/>
+      <c r="Q191" s="9"/>
+      <c r="R191" s="5"/>
+      <c r="S191" s="21"/>
+    </row>
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A192" s="20"/>
+      <c r="B192" s="4"/>
+      <c r="C192" s="9"/>
+      <c r="D192" s="9"/>
+      <c r="E192" s="9"/>
+      <c r="F192" s="9"/>
+      <c r="G192" s="9"/>
+      <c r="H192" s="9"/>
+      <c r="I192" s="9"/>
+      <c r="J192" s="9"/>
+      <c r="K192" s="9"/>
+      <c r="L192" s="9"/>
+      <c r="M192" s="9"/>
+      <c r="N192" s="9"/>
+      <c r="O192" s="9"/>
+      <c r="P192" s="9"/>
+      <c r="Q192" s="9"/>
+      <c r="R192" s="5"/>
+      <c r="S192" s="21"/>
+    </row>
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A193" s="20"/>
+      <c r="B193" s="4"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="9"/>
+      <c r="E193" s="9"/>
+      <c r="F193" s="9"/>
+      <c r="G193" s="9"/>
+      <c r="H193" s="9"/>
+      <c r="I193" s="9"/>
+      <c r="J193" s="9"/>
+      <c r="K193" s="9"/>
+      <c r="L193" s="9"/>
+      <c r="M193" s="9"/>
+      <c r="N193" s="9"/>
+      <c r="O193" s="9"/>
+      <c r="P193" s="9"/>
+      <c r="Q193" s="9"/>
+      <c r="R193" s="5"/>
+      <c r="S193" s="21"/>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A194" s="20"/>
+      <c r="B194" s="4"/>
+      <c r="C194" s="9"/>
+      <c r="D194" s="9"/>
+      <c r="E194" s="9"/>
+      <c r="F194" s="9"/>
+      <c r="G194" s="9"/>
+      <c r="H194" s="9"/>
+      <c r="I194" s="9"/>
+      <c r="J194" s="9"/>
+      <c r="K194" s="9"/>
+      <c r="L194" s="9"/>
+      <c r="M194" s="9"/>
+      <c r="N194" s="9"/>
+      <c r="O194" s="9"/>
+      <c r="P194" s="9"/>
+      <c r="Q194" s="9"/>
+      <c r="R194" s="5"/>
+      <c r="S194" s="21"/>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A195" s="20"/>
+      <c r="B195" s="4"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="9"/>
+      <c r="E195" s="9"/>
+      <c r="F195" s="9"/>
+      <c r="G195" s="9"/>
+      <c r="H195" s="9"/>
+      <c r="I195" s="9"/>
+      <c r="J195" s="9"/>
+      <c r="K195" s="9"/>
+      <c r="L195" s="9"/>
+      <c r="M195" s="9"/>
+      <c r="N195" s="9"/>
+      <c r="O195" s="9"/>
+      <c r="P195" s="9"/>
+      <c r="Q195" s="9"/>
+      <c r="R195" s="5"/>
+      <c r="S195" s="21"/>
+    </row>
+    <row r="196" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A196" s="20"/>
+      <c r="B196" s="4"/>
+      <c r="C196" s="9"/>
+      <c r="D196" s="9"/>
+      <c r="E196" s="9"/>
+      <c r="F196" s="9"/>
+      <c r="G196" s="9"/>
+      <c r="H196" s="9"/>
+      <c r="I196" s="9"/>
+      <c r="J196" s="9"/>
+      <c r="K196" s="9"/>
+      <c r="L196" s="9"/>
+      <c r="M196" s="9"/>
+      <c r="N196" s="9"/>
+      <c r="O196" s="9"/>
+      <c r="P196" s="9"/>
+      <c r="Q196" s="9"/>
+      <c r="R196" s="5"/>
+      <c r="S196" s="21"/>
+    </row>
+    <row r="197" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A197" s="20"/>
+      <c r="B197" s="4"/>
+      <c r="C197" s="9"/>
+      <c r="D197" s="9"/>
+      <c r="E197" s="9"/>
+      <c r="F197" s="9"/>
+      <c r="G197" s="9"/>
+      <c r="H197" s="9"/>
+      <c r="I197" s="9"/>
+      <c r="J197" s="9"/>
+      <c r="K197" s="9"/>
+      <c r="L197" s="9"/>
+      <c r="M197" s="9"/>
+      <c r="N197" s="9"/>
+      <c r="O197" s="9"/>
+      <c r="P197" s="9"/>
+      <c r="Q197" s="9"/>
+      <c r="R197" s="5"/>
+      <c r="S197" s="21"/>
+    </row>
+    <row r="198" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A198" s="20"/>
+      <c r="B198" s="4"/>
+      <c r="C198" s="9"/>
+      <c r="D198" s="9"/>
+      <c r="E198" s="9"/>
+      <c r="F198" s="9"/>
+      <c r="G198" s="9"/>
+      <c r="H198" s="9"/>
+      <c r="I198" s="9"/>
+      <c r="J198" s="9"/>
+      <c r="K198" s="9"/>
+      <c r="L198" s="9"/>
+      <c r="M198" s="9"/>
+      <c r="N198" s="9"/>
+      <c r="O198" s="9"/>
+      <c r="P198" s="9"/>
+      <c r="Q198" s="9"/>
+      <c r="R198" s="5"/>
+      <c r="S198" s="21"/>
+    </row>
+    <row r="199" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A199" s="20"/>
+      <c r="B199" s="4"/>
+      <c r="C199" s="9"/>
+      <c r="D199" s="9"/>
+      <c r="E199" s="9"/>
+      <c r="F199" s="9"/>
+      <c r="G199" s="9"/>
+      <c r="H199" s="9"/>
+      <c r="I199" s="9"/>
+      <c r="J199" s="9"/>
+      <c r="K199" s="9"/>
+      <c r="L199" s="9"/>
+      <c r="M199" s="9"/>
+      <c r="N199" s="9"/>
+      <c r="O199" s="9"/>
+      <c r="P199" s="9"/>
+      <c r="Q199" s="9"/>
+      <c r="R199" s="5"/>
+      <c r="S199" s="21"/>
+    </row>
+    <row r="200" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A200" s="20"/>
+      <c r="B200" s="4"/>
+      <c r="C200" s="9"/>
+      <c r="D200" s="9"/>
+      <c r="E200" s="9"/>
+      <c r="F200" s="9"/>
+      <c r="G200" s="9"/>
+      <c r="H200" s="9"/>
+      <c r="I200" s="9"/>
+      <c r="J200" s="9"/>
+      <c r="K200" s="9"/>
+      <c r="L200" s="9"/>
+      <c r="M200" s="9"/>
+      <c r="N200" s="9"/>
+      <c r="O200" s="9"/>
+      <c r="P200" s="9"/>
+      <c r="Q200" s="9"/>
+      <c r="R200" s="5"/>
+      <c r="S200" s="21"/>
+    </row>
+    <row r="201" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A201" s="20"/>
+      <c r="B201" s="4"/>
+      <c r="C201" s="9"/>
+      <c r="D201" s="9"/>
+      <c r="E201" s="9"/>
+      <c r="F201" s="9"/>
+      <c r="G201" s="9"/>
+      <c r="H201" s="9"/>
+      <c r="I201" s="9"/>
+      <c r="J201" s="9"/>
+      <c r="K201" s="9"/>
+      <c r="L201" s="9"/>
+      <c r="M201" s="9"/>
+      <c r="N201" s="9"/>
+      <c r="O201" s="9"/>
+      <c r="P201" s="9"/>
+      <c r="Q201" s="9"/>
+      <c r="R201" s="5"/>
+      <c r="S201" s="21"/>
+    </row>
+    <row r="202" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A202" s="20"/>
+      <c r="B202" s="4"/>
+      <c r="C202" s="9"/>
+      <c r="D202" s="9"/>
+      <c r="E202" s="9"/>
+      <c r="F202" s="9"/>
+      <c r="G202" s="9"/>
+      <c r="H202" s="9"/>
+      <c r="I202" s="9"/>
+      <c r="J202" s="9"/>
+      <c r="K202" s="9"/>
+      <c r="L202" s="9"/>
+      <c r="M202" s="9"/>
+      <c r="N202" s="9"/>
+      <c r="O202" s="9"/>
+      <c r="P202" s="9"/>
+      <c r="Q202" s="9"/>
+      <c r="R202" s="5"/>
+      <c r="S202" s="21"/>
+    </row>
+    <row r="203" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A203" s="20"/>
+      <c r="B203" s="4"/>
+      <c r="C203" s="9"/>
+      <c r="D203" s="9"/>
+      <c r="E203" s="9"/>
+      <c r="F203" s="9"/>
+      <c r="G203" s="9"/>
+      <c r="H203" s="9"/>
+      <c r="I203" s="9"/>
+      <c r="J203" s="9"/>
+      <c r="K203" s="9"/>
+      <c r="L203" s="9"/>
+      <c r="M203" s="9"/>
+      <c r="N203" s="9"/>
+      <c r="O203" s="9"/>
+      <c r="P203" s="9"/>
+      <c r="Q203" s="9"/>
+      <c r="R203" s="5"/>
+      <c r="S203" s="21"/>
+    </row>
+    <row r="204" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A204" s="20"/>
+      <c r="B204" s="4"/>
+      <c r="C204" s="9"/>
+      <c r="D204" s="9"/>
+      <c r="E204" s="9"/>
+      <c r="F204" s="9"/>
+      <c r="G204" s="9"/>
+      <c r="H204" s="9"/>
+      <c r="I204" s="9"/>
+      <c r="J204" s="9"/>
+      <c r="K204" s="9"/>
+      <c r="L204" s="9"/>
+      <c r="M204" s="9"/>
+      <c r="N204" s="9"/>
+      <c r="O204" s="9"/>
+      <c r="P204" s="9"/>
+      <c r="Q204" s="9"/>
+      <c r="R204" s="5"/>
+      <c r="S204" s="21"/>
+    </row>
+    <row r="205" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A205" s="20"/>
+      <c r="B205" s="6"/>
+      <c r="C205" s="7"/>
+      <c r="D205" s="7"/>
+      <c r="E205" s="7"/>
+      <c r="F205" s="7"/>
+      <c r="G205" s="7"/>
+      <c r="H205" s="7"/>
+      <c r="I205" s="7"/>
+      <c r="J205" s="7"/>
+      <c r="K205" s="7"/>
+      <c r="L205" s="7"/>
+      <c r="M205" s="7"/>
+      <c r="N205" s="7"/>
+      <c r="O205" s="7"/>
+      <c r="P205" s="7"/>
+      <c r="Q205" s="7"/>
+      <c r="R205" s="8"/>
+      <c r="S205" s="21"/>
+    </row>
+    <row r="206" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A206" s="20"/>
+      <c r="B206" s="9"/>
+      <c r="C206" s="9"/>
+      <c r="D206" s="9"/>
+      <c r="E206" s="9"/>
+      <c r="F206" s="9"/>
+      <c r="G206" s="9"/>
+      <c r="H206" s="9"/>
+      <c r="I206" s="9"/>
+      <c r="J206" s="9"/>
+      <c r="K206" s="9"/>
+      <c r="L206" s="9"/>
+      <c r="M206" s="9"/>
+      <c r="N206" s="9"/>
+      <c r="O206" s="9"/>
+      <c r="P206" s="9"/>
+      <c r="Q206" s="9"/>
+      <c r="R206" s="9"/>
+      <c r="S206" s="21"/>
+    </row>
+    <row r="207" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A207" s="20"/>
+      <c r="B207" s="9"/>
+      <c r="C207" s="9"/>
+      <c r="D207" s="9"/>
+      <c r="E207" s="9"/>
+      <c r="F207" s="9"/>
+      <c r="G207" s="9"/>
+      <c r="H207" s="9"/>
+      <c r="I207" s="9"/>
+      <c r="J207" s="9"/>
+      <c r="K207" s="9"/>
+      <c r="L207" s="9"/>
+      <c r="M207" s="9"/>
+      <c r="N207" s="9"/>
+      <c r="O207" s="9"/>
+      <c r="P207" s="9"/>
+      <c r="Q207" s="9"/>
+      <c r="R207" s="9"/>
+      <c r="S207" s="21"/>
+    </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A208" s="20"/>
+      <c r="B208" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C208" s="2"/>
+      <c r="D208" s="2"/>
+      <c r="E208" s="2"/>
+      <c r="F208" s="2"/>
+      <c r="G208" s="2"/>
+      <c r="H208" s="2"/>
+      <c r="I208" s="2"/>
+      <c r="J208" s="2"/>
+      <c r="K208" s="2"/>
+      <c r="L208" s="2"/>
+      <c r="M208" s="2"/>
+      <c r="N208" s="2"/>
+      <c r="O208" s="2"/>
+      <c r="P208" s="2"/>
+      <c r="Q208" s="2"/>
+      <c r="R208" s="3"/>
+      <c r="S208" s="21"/>
+    </row>
+    <row r="209" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A209" s="20"/>
+      <c r="B209" s="4"/>
+      <c r="C209" s="9"/>
+      <c r="D209" s="9"/>
+      <c r="E209" s="9"/>
+      <c r="F209" s="9"/>
+      <c r="G209" s="9"/>
+      <c r="H209" s="9"/>
+      <c r="I209" s="9"/>
+      <c r="J209" s="9"/>
+      <c r="K209" s="9"/>
+      <c r="L209" s="9"/>
+      <c r="M209" s="9"/>
+      <c r="N209" s="9"/>
+      <c r="O209" s="9"/>
+      <c r="P209" s="9"/>
+      <c r="Q209" s="9"/>
+      <c r="R209" s="5"/>
+      <c r="S209" s="21"/>
+    </row>
+    <row r="210" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A210" s="20"/>
+      <c r="B210" s="4"/>
+      <c r="C210" s="9"/>
+      <c r="D210" s="9"/>
+      <c r="E210" s="9"/>
+      <c r="F210" s="9"/>
+      <c r="G210" s="9"/>
+      <c r="H210" s="9"/>
+      <c r="I210" s="9"/>
+      <c r="J210" s="9"/>
+      <c r="K210" s="9"/>
+      <c r="L210" s="9"/>
+      <c r="M210" s="9"/>
+      <c r="N210" s="9"/>
+      <c r="O210" s="9"/>
+      <c r="P210" s="9"/>
+      <c r="Q210" s="9"/>
+      <c r="R210" s="5"/>
+      <c r="S210" s="21"/>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A211" s="20"/>
+      <c r="B211" s="4"/>
+      <c r="C211" s="9"/>
+      <c r="D211" s="9"/>
+      <c r="E211" s="9"/>
+      <c r="F211" s="9"/>
+      <c r="G211" s="9"/>
+      <c r="H211" s="9"/>
+      <c r="I211" s="9"/>
+      <c r="J211" s="9"/>
+      <c r="K211" s="9"/>
+      <c r="L211" s="9"/>
+      <c r="M211" s="9"/>
+      <c r="N211" s="9"/>
+      <c r="O211" s="9"/>
+      <c r="P211" s="9"/>
+      <c r="Q211" s="9"/>
+      <c r="R211" s="5"/>
+      <c r="S211" s="21"/>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A212" s="20"/>
+      <c r="B212" s="4"/>
+      <c r="C212" s="9"/>
+      <c r="D212" s="9"/>
+      <c r="E212" s="9"/>
+      <c r="F212" s="9"/>
+      <c r="G212" s="9"/>
+      <c r="H212" s="9"/>
+      <c r="I212" s="9"/>
+      <c r="J212" s="9"/>
+      <c r="K212" s="9"/>
+      <c r="L212" s="9"/>
+      <c r="M212" s="9"/>
+      <c r="N212" s="9"/>
+      <c r="O212" s="9"/>
+      <c r="P212" s="9"/>
+      <c r="Q212" s="9"/>
+      <c r="R212" s="5"/>
+      <c r="S212" s="21"/>
+    </row>
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A213" s="20"/>
+      <c r="B213" s="4"/>
+      <c r="C213" s="9"/>
+      <c r="D213" s="9"/>
+      <c r="E213" s="9"/>
+      <c r="F213" s="9"/>
+      <c r="G213" s="9"/>
+      <c r="H213" s="9"/>
+      <c r="I213" s="9"/>
+      <c r="J213" s="9"/>
+      <c r="K213" s="9"/>
+      <c r="L213" s="9"/>
+      <c r="M213" s="9"/>
+      <c r="N213" s="9"/>
+      <c r="O213" s="9"/>
+      <c r="P213" s="9"/>
+      <c r="Q213" s="9"/>
+      <c r="R213" s="5"/>
+      <c r="S213" s="21"/>
+    </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A214" s="20"/>
+      <c r="B214" s="4"/>
+      <c r="C214" s="9"/>
+      <c r="D214" s="9"/>
+      <c r="E214" s="9"/>
+      <c r="F214" s="9"/>
+      <c r="G214" s="9"/>
+      <c r="H214" s="9"/>
+      <c r="I214" s="9"/>
+      <c r="J214" s="9"/>
+      <c r="K214" s="9"/>
+      <c r="L214" s="9"/>
+      <c r="M214" s="9"/>
+      <c r="N214" s="9"/>
+      <c r="O214" s="9"/>
+      <c r="P214" s="9"/>
+      <c r="Q214" s="9"/>
+      <c r="R214" s="5"/>
+      <c r="S214" s="21"/>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A215" s="20"/>
+      <c r="B215" s="4"/>
+      <c r="C215" s="9"/>
+      <c r="D215" s="9"/>
+      <c r="E215" s="9"/>
+      <c r="F215" s="9"/>
+      <c r="G215" s="9"/>
+      <c r="H215" s="9"/>
+      <c r="I215" s="9"/>
+      <c r="J215" s="9"/>
+      <c r="K215" s="9"/>
+      <c r="L215" s="9"/>
+      <c r="M215" s="9"/>
+      <c r="N215" s="9"/>
+      <c r="O215" s="9"/>
+      <c r="P215" s="9"/>
+      <c r="Q215" s="9"/>
+      <c r="R215" s="5"/>
+      <c r="S215" s="21"/>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A216" s="20"/>
+      <c r="B216" s="4"/>
+      <c r="C216" s="9"/>
+      <c r="D216" s="9"/>
+      <c r="E216" s="9"/>
+      <c r="F216" s="9"/>
+      <c r="G216" s="9"/>
+      <c r="H216" s="9"/>
+      <c r="I216" s="9"/>
+      <c r="J216" s="9"/>
+      <c r="K216" s="9"/>
+      <c r="L216" s="9"/>
+      <c r="M216" s="9"/>
+      <c r="N216" s="9"/>
+      <c r="O216" s="9"/>
+      <c r="P216" s="9"/>
+      <c r="Q216" s="9"/>
+      <c r="R216" s="5"/>
+      <c r="S216" s="21"/>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A217" s="20"/>
+      <c r="B217" s="4"/>
+      <c r="C217" s="9"/>
+      <c r="D217" s="9"/>
+      <c r="E217" s="9"/>
+      <c r="F217" s="9"/>
+      <c r="G217" s="9"/>
+      <c r="H217" s="9"/>
+      <c r="I217" s="9"/>
+      <c r="J217" s="9"/>
+      <c r="K217" s="9"/>
+      <c r="L217" s="9"/>
+      <c r="M217" s="9"/>
+      <c r="N217" s="9"/>
+      <c r="O217" s="9"/>
+      <c r="P217" s="9"/>
+      <c r="Q217" s="9"/>
+      <c r="R217" s="5"/>
+      <c r="S217" s="21"/>
+    </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A218" s="20"/>
+      <c r="B218" s="4"/>
+      <c r="C218" s="9"/>
+      <c r="D218" s="9"/>
+      <c r="E218" s="9"/>
+      <c r="F218" s="9"/>
+      <c r="G218" s="9"/>
+      <c r="H218" s="9"/>
+      <c r="I218" s="9"/>
+      <c r="J218" s="9"/>
+      <c r="K218" s="9"/>
+      <c r="L218" s="9"/>
+      <c r="M218" s="9"/>
+      <c r="N218" s="9"/>
+      <c r="O218" s="9"/>
+      <c r="P218" s="9"/>
+      <c r="Q218" s="9"/>
+      <c r="R218" s="5"/>
+      <c r="S218" s="21"/>
+    </row>
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A219" s="20"/>
+      <c r="B219" s="4"/>
+      <c r="C219" s="9"/>
+      <c r="D219" s="9"/>
+      <c r="E219" s="9"/>
+      <c r="F219" s="9"/>
+      <c r="G219" s="9"/>
+      <c r="H219" s="9"/>
+      <c r="I219" s="9"/>
+      <c r="J219" s="9"/>
+      <c r="K219" s="9"/>
+      <c r="L219" s="9"/>
+      <c r="M219" s="9"/>
+      <c r="N219" s="9"/>
+      <c r="O219" s="9"/>
+      <c r="P219" s="9"/>
+      <c r="Q219" s="9"/>
+      <c r="R219" s="5"/>
+      <c r="S219" s="21"/>
+    </row>
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A220" s="20"/>
+      <c r="B220" s="4"/>
+      <c r="C220" s="9"/>
+      <c r="D220" s="9"/>
+      <c r="E220" s="9"/>
+      <c r="F220" s="9"/>
+      <c r="G220" s="9"/>
+      <c r="H220" s="9"/>
+      <c r="I220" s="9"/>
+      <c r="J220" s="9"/>
+      <c r="K220" s="9"/>
+      <c r="L220" s="9"/>
+      <c r="M220" s="9"/>
+      <c r="N220" s="9"/>
+      <c r="O220" s="9"/>
+      <c r="P220" s="9"/>
+      <c r="Q220" s="9"/>
+      <c r="R220" s="5"/>
+      <c r="S220" s="21"/>
+    </row>
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A221" s="20"/>
+      <c r="B221" s="4"/>
+      <c r="C221" s="9"/>
+      <c r="D221" s="9"/>
+      <c r="E221" s="9"/>
+      <c r="F221" s="9"/>
+      <c r="G221" s="9"/>
+      <c r="H221" s="9"/>
+      <c r="I221" s="9"/>
+      <c r="J221" s="9"/>
+      <c r="K221" s="9"/>
+      <c r="L221" s="9"/>
+      <c r="M221" s="9"/>
+      <c r="N221" s="9"/>
+      <c r="O221" s="9"/>
+      <c r="P221" s="9"/>
+      <c r="Q221" s="9"/>
+      <c r="R221" s="5"/>
+      <c r="S221" s="21"/>
+    </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A222" s="20"/>
+      <c r="B222" s="4"/>
+      <c r="C222" s="9"/>
+      <c r="D222" s="9"/>
+      <c r="E222" s="9"/>
+      <c r="F222" s="9"/>
+      <c r="G222" s="9"/>
+      <c r="H222" s="9"/>
+      <c r="I222" s="9"/>
+      <c r="J222" s="9"/>
+      <c r="K222" s="9"/>
+      <c r="L222" s="9"/>
+      <c r="M222" s="9"/>
+      <c r="N222" s="9"/>
+      <c r="O222" s="9"/>
+      <c r="P222" s="9"/>
+      <c r="Q222" s="9"/>
+      <c r="R222" s="5"/>
+      <c r="S222" s="21"/>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A223" s="20"/>
+      <c r="B223" s="4"/>
+      <c r="C223" s="9"/>
+      <c r="D223" s="9"/>
+      <c r="E223" s="9"/>
+      <c r="F223" s="9"/>
+      <c r="G223" s="9"/>
+      <c r="H223" s="9"/>
+      <c r="I223" s="9"/>
+      <c r="J223" s="9"/>
+      <c r="K223" s="9"/>
+      <c r="L223" s="9"/>
+      <c r="M223" s="9"/>
+      <c r="N223" s="9"/>
+      <c r="O223" s="9"/>
+      <c r="P223" s="9"/>
+      <c r="Q223" s="9"/>
+      <c r="R223" s="5"/>
+      <c r="S223" s="21"/>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A224" s="20"/>
+      <c r="B224" s="4"/>
+      <c r="C224" s="9"/>
+      <c r="D224" s="9"/>
+      <c r="E224" s="9"/>
+      <c r="F224" s="9"/>
+      <c r="G224" s="9"/>
+      <c r="H224" s="9"/>
+      <c r="I224" s="9"/>
+      <c r="J224" s="9"/>
+      <c r="K224" s="9"/>
+      <c r="L224" s="9"/>
+      <c r="M224" s="9"/>
+      <c r="N224" s="9"/>
+      <c r="O224" s="9"/>
+      <c r="P224" s="9"/>
+      <c r="Q224" s="9"/>
+      <c r="R224" s="5"/>
+      <c r="S224" s="21"/>
+    </row>
+    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A225" s="20"/>
+      <c r="B225" s="4"/>
+      <c r="C225" s="9"/>
+      <c r="D225" s="9"/>
+      <c r="E225" s="9"/>
+      <c r="F225" s="9"/>
+      <c r="G225" s="9"/>
+      <c r="H225" s="9"/>
+      <c r="I225" s="9"/>
+      <c r="J225" s="9"/>
+      <c r="K225" s="9"/>
+      <c r="L225" s="9"/>
+      <c r="M225" s="9"/>
+      <c r="N225" s="9"/>
+      <c r="O225" s="9"/>
+      <c r="P225" s="9"/>
+      <c r="Q225" s="9"/>
+      <c r="R225" s="5"/>
+      <c r="S225" s="21"/>
+    </row>
+    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A226" s="20"/>
+      <c r="B226" s="6"/>
+      <c r="C226" s="7"/>
+      <c r="D226" s="7"/>
+      <c r="E226" s="7"/>
+      <c r="F226" s="7"/>
+      <c r="G226" s="7"/>
+      <c r="H226" s="7"/>
+      <c r="I226" s="7"/>
+      <c r="J226" s="7"/>
+      <c r="K226" s="7"/>
+      <c r="L226" s="7"/>
+      <c r="M226" s="7"/>
+      <c r="N226" s="7"/>
+      <c r="O226" s="7"/>
+      <c r="P226" s="7"/>
+      <c r="Q226" s="7"/>
+      <c r="R226" s="8"/>
+      <c r="S226" s="21"/>
+    </row>
+    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A227" s="20"/>
+      <c r="B227" s="9"/>
+      <c r="C227" s="9"/>
+      <c r="D227" s="9"/>
+      <c r="E227" s="9"/>
+      <c r="F227" s="9"/>
+      <c r="G227" s="9"/>
+      <c r="H227" s="9"/>
+      <c r="I227" s="9"/>
+      <c r="J227" s="9"/>
+      <c r="K227" s="9"/>
+      <c r="L227" s="9"/>
+      <c r="M227" s="9"/>
+      <c r="N227" s="9"/>
+      <c r="O227" s="9"/>
+      <c r="P227" s="9"/>
+      <c r="Q227" s="9"/>
+      <c r="R227" s="9"/>
+      <c r="S227" s="21"/>
+    </row>
+    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A228" s="20"/>
+      <c r="B228" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C228" s="9"/>
+      <c r="D228" s="9"/>
+      <c r="E228" s="9"/>
+      <c r="F228" s="9"/>
+      <c r="G228" s="9"/>
+      <c r="H228" s="9"/>
+      <c r="I228" s="9"/>
+      <c r="J228" s="9"/>
+      <c r="K228" s="9"/>
+      <c r="L228" s="9"/>
+      <c r="M228" s="9"/>
+      <c r="N228" s="9"/>
+      <c r="O228" s="9"/>
+      <c r="P228" s="9"/>
+      <c r="Q228" s="9"/>
+      <c r="R228" s="9"/>
+      <c r="S228" s="21"/>
+    </row>
+    <row r="229" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="22"/>
+      <c r="B229" s="23"/>
+      <c r="C229" s="23"/>
+      <c r="D229" s="23"/>
+      <c r="E229" s="23"/>
+      <c r="F229" s="23"/>
+      <c r="G229" s="23"/>
+      <c r="H229" s="23"/>
+      <c r="I229" s="23"/>
+      <c r="J229" s="23"/>
+      <c r="K229" s="23"/>
+      <c r="L229" s="23"/>
+      <c r="M229" s="23"/>
+      <c r="N229" s="23"/>
+      <c r="O229" s="23"/>
+      <c r="P229" s="23"/>
+      <c r="Q229" s="23"/>
+      <c r="R229" s="23"/>
+      <c r="S229" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create a table data gateway class for the resource table
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D6704D-95CB-44CC-8236-E277A6072DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C523A7-2FA6-4361-A1DA-9D6A97E9AEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
     <sheet name="Create a table to storeResource" sheetId="2" r:id="rId2"/>
     <sheet name="Connect to the database fromPHP" sheetId="3" r:id="rId3"/>
     <sheet name=".env file" sheetId="4" r:id="rId4"/>
+    <sheet name="table data gateway class" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="152">
   <si>
     <t>構成</t>
   </si>
@@ -362,6 +363,129 @@
   </si>
   <si>
     <t>Đến đây thì việc kiểm tra kết nối DB đã hoàn tất</t>
+  </si>
+  <si>
+    <t>Create a table data gateway class for the resource table</t>
+  </si>
+  <si>
+    <t>Trong TaskController có các hành động xử lý khi gọi api, thay cho việc xử lý DB trực tiếp ở đây thì tạo thêm class TaskGateway để xử lý với database của bảng task</t>
+  </si>
+  <si>
+    <t>TaskGateway.php</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\src\TaskGateway.php</t>
+  </si>
+  <si>
+    <t>class TaskGateway</t>
+  </si>
+  <si>
+    <t>    private $conn;</t>
+  </si>
+  <si>
+    <t>    public function __construct(Database $database)</t>
+  </si>
+  <si>
+    <t>        $this-&gt;conn = $database-&gt;getConnection();</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\src\TaskController.php</t>
+  </si>
+  <si>
+    <t>class TaskController</t>
+  </si>
+  <si>
+    <t>    private $gateway;</t>
+  </si>
+  <si>
+    <t>    public function __construct(TaskGateway $gateway)</t>
+  </si>
+  <si>
+    <t>        $this-&gt;gateway = $gateway;</t>
+  </si>
+  <si>
+    <t>    public function processRequest(string $method, ?string $id): void</t>
+  </si>
+  <si>
+    <t>        if ($id === null) {</t>
+  </si>
+  <si>
+    <t>            if ($method == "GET") {</t>
+  </si>
+  <si>
+    <t>                echo json_encode("index");</t>
+  </si>
+  <si>
+    <t>            } elseif ($method == "POST") {</t>
+  </si>
+  <si>
+    <t>                echo json_encode("create");</t>
+  </si>
+  <si>
+    <t>            } else {</t>
+  </si>
+  <si>
+    <t>                $this-&gt;respondMethodNotAllowed("GET, POST");</t>
+  </si>
+  <si>
+    <t>            }</t>
+  </si>
+  <si>
+    <t>        } else {</t>
+  </si>
+  <si>
+    <t>            switch ($method) {</t>
+  </si>
+  <si>
+    <t>                case "GET":</t>
+  </si>
+  <si>
+    <t>                    echo json_encode("show $id");</t>
+  </si>
+  <si>
+    <t>                    break;</t>
+  </si>
+  <si>
+    <t>                case "PATCH":</t>
+  </si>
+  <si>
+    <t>                    echo json_encode("update $id");</t>
+  </si>
+  <si>
+    <t>                case "DELETE":</t>
+  </si>
+  <si>
+    <t>                    echo json_encode("delete $id");</t>
+  </si>
+  <si>
+    <t>                default:</t>
+  </si>
+  <si>
+    <t>                    $this-&gt;respondMethodNotAllowed("GET, PATCH, DELETE");</t>
+  </si>
+  <si>
+    <t>        }</t>
+  </si>
+  <si>
+    <t>    private function respondMethodNotAllowed(string $allowed_methods): void</t>
+  </si>
+  <si>
+    <t>        http_response_code(405);</t>
+  </si>
+  <si>
+    <t>        header("Allow: $allowed_methods");</t>
+  </si>
+  <si>
+    <t>$task_gateway = new TaskGateway($database);</t>
+  </si>
+  <si>
+    <t>$controller = new TaskController($task_gateway);</t>
+  </si>
+  <si>
+    <t>Class này sẽ sử lý các thao tác với database</t>
+  </si>
+  <si>
+    <t>Gọi api và thấy vẫn hoạt động bình thường</t>
   </si>
 </sst>
 </file>
@@ -582,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -613,6 +737,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1514,6 +1640,320 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE6F1618-17AF-7D5A-FC47-62501137ED73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1257300" y="6457950"/>
+          <a:ext cx="1352550" cy="3333750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9402853-B475-9AA0-E4BD-FF5B589CB1F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2667000" y="9877425"/>
+          <a:ext cx="247650" cy="15716250"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFE1EB14-07AD-6B9E-FFE1-17EE05F63A52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3381375" y="6448425"/>
+          <a:ext cx="3629025" cy="695325"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>427370</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>85394</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E8AC6D3-5B9B-D37E-0BA6-50F1F1C1ADDC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="27155775"/>
+          <a:ext cx="10038095" cy="2647619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Straight Arrow Connector 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FB8ADDE-E0C7-1D60-F237-7A468AFBF5ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1628775" y="26841450"/>
+          <a:ext cx="1266825" cy="2667000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="16" name="Straight Arrow Connector 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04F6E700-4D66-56C1-2C4C-1095EC1F79CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2905125" y="26831925"/>
+          <a:ext cx="6581775" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4428,8 +4868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8C56BAC-8DE4-497E-995C-01E4CC964831}">
   <dimension ref="A2:U229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="L157" sqref="L157"/>
+    <sheetView topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114:L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7859,4 +8299,1983 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA190C99-A3E9-4F93-9540-3F02D2357A9D}">
+  <dimension ref="A2:R158"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="5"/>
+      <c r="K18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="5"/>
+      <c r="K22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="5"/>
+      <c r="K23" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="5"/>
+      <c r="H34" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="15"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B54" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B63" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="4"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B98" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7"/>
+      <c r="I98" s="8"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B102" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="2"/>
+      <c r="J102" s="2"/>
+      <c r="K102" s="2"/>
+      <c r="L102" s="3"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B103" s="4"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="5"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B104" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
+      <c r="L104" s="5"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B105" s="4"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="5"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
+      <c r="L106" s="5"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B107" s="4"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
+      <c r="L107" s="5"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
+      <c r="L108" s="5"/>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B109" s="4"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="9"/>
+      <c r="H109" s="9"/>
+      <c r="I109" s="9"/>
+      <c r="J109" s="9"/>
+      <c r="K109" s="9"/>
+      <c r="L109" s="5"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="9"/>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
+      <c r="L110" s="5"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B111" s="4"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
+      <c r="I111" s="9"/>
+      <c r="J111" s="9"/>
+      <c r="K111" s="9"/>
+      <c r="L111" s="5"/>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="9"/>
+      <c r="J112" s="9"/>
+      <c r="K112" s="9"/>
+      <c r="L112" s="5"/>
+    </row>
+    <row r="113" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="9"/>
+      <c r="H113" s="9"/>
+      <c r="I113" s="9"/>
+      <c r="J113" s="9"/>
+      <c r="K113" s="9"/>
+      <c r="L113" s="5"/>
+    </row>
+    <row r="114" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B114" s="4"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="9"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="9"/>
+      <c r="J114" s="9"/>
+      <c r="K114" s="9"/>
+      <c r="L114" s="5"/>
+    </row>
+    <row r="115" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="9"/>
+      <c r="K115" s="9"/>
+      <c r="L115" s="5"/>
+    </row>
+    <row r="116" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="9"/>
+      <c r="K116" s="9"/>
+      <c r="L116" s="5"/>
+    </row>
+    <row r="117" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="9"/>
+      <c r="K117" s="9"/>
+      <c r="L117" s="5"/>
+    </row>
+    <row r="118" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="9"/>
+      <c r="K118" s="9"/>
+      <c r="L118" s="5"/>
+    </row>
+    <row r="119" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="9"/>
+      <c r="K119" s="9"/>
+      <c r="L119" s="5"/>
+    </row>
+    <row r="120" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B120" s="4"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="9"/>
+      <c r="K120" s="9"/>
+      <c r="L120" s="5"/>
+    </row>
+    <row r="121" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
+      <c r="H121" s="9"/>
+      <c r="I121" s="9"/>
+      <c r="J121" s="9"/>
+      <c r="K121" s="9"/>
+      <c r="L121" s="5"/>
+    </row>
+    <row r="122" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="9"/>
+      <c r="H122" s="9"/>
+      <c r="I122" s="9"/>
+      <c r="J122" s="9"/>
+      <c r="K122" s="9"/>
+      <c r="L122" s="5"/>
+    </row>
+    <row r="123" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="9"/>
+      <c r="J123" s="9"/>
+      <c r="K123" s="9"/>
+      <c r="L123" s="5"/>
+    </row>
+    <row r="124" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B124" s="4"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="H124" s="9"/>
+      <c r="I124" s="9"/>
+      <c r="J124" s="9"/>
+      <c r="K124" s="9"/>
+      <c r="L124" s="5"/>
+    </row>
+    <row r="125" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="9"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="9"/>
+      <c r="J125" s="9"/>
+      <c r="K125" s="9"/>
+      <c r="L125" s="5"/>
+    </row>
+    <row r="126" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B126" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="9"/>
+      <c r="H126" s="9"/>
+      <c r="I126" s="9"/>
+      <c r="J126" s="9"/>
+      <c r="K126" s="9"/>
+      <c r="L126" s="5"/>
+    </row>
+    <row r="127" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+      <c r="H127" s="9"/>
+      <c r="I127" s="9"/>
+      <c r="J127" s="9"/>
+      <c r="K127" s="9"/>
+      <c r="L127" s="5"/>
+    </row>
+    <row r="128" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B128" s="4"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="9"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="9"/>
+      <c r="K128" s="9"/>
+      <c r="L128" s="5"/>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+      <c r="H129" s="9"/>
+      <c r="I129" s="9"/>
+      <c r="J129" s="9"/>
+      <c r="K129" s="9"/>
+      <c r="L129" s="5"/>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B130" s="4"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9"/>
+      <c r="H130" s="9"/>
+      <c r="I130" s="9"/>
+      <c r="J130" s="9"/>
+      <c r="K130" s="9"/>
+      <c r="L130" s="5"/>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="9"/>
+      <c r="K131" s="9"/>
+      <c r="L131" s="5"/>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B132" s="4"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="9"/>
+      <c r="K132" s="9"/>
+      <c r="L132" s="5"/>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B133" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="9"/>
+      <c r="K133" s="9"/>
+      <c r="L133" s="5"/>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B134" s="15"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="9"/>
+      <c r="K134" s="9"/>
+      <c r="L134" s="5"/>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B135" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="5"/>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B136" s="4"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="9"/>
+      <c r="K136" s="9"/>
+      <c r="L136" s="5"/>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B137" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C137" s="7"/>
+      <c r="D137" s="7"/>
+      <c r="E137" s="7"/>
+      <c r="F137" s="7"/>
+      <c r="G137" s="7"/>
+      <c r="H137" s="7"/>
+      <c r="I137" s="7"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="7"/>
+      <c r="L137" s="8"/>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A140" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B140" s="2"/>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+      <c r="E140" s="2"/>
+      <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
+      <c r="H140" s="2"/>
+      <c r="I140" s="2"/>
+      <c r="J140" s="2"/>
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2"/>
+      <c r="O140" s="2"/>
+      <c r="P140" s="2"/>
+      <c r="Q140" s="2"/>
+      <c r="R140" s="3"/>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A141" s="4"/>
+      <c r="B141" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+      <c r="I141" s="9"/>
+      <c r="J141" s="9"/>
+      <c r="K141" s="9"/>
+      <c r="L141" s="9"/>
+      <c r="M141" s="9"/>
+      <c r="N141" s="9"/>
+      <c r="O141" s="9"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="9"/>
+      <c r="R141" s="5"/>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A142" s="4"/>
+      <c r="B142" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+      <c r="H142" s="9"/>
+      <c r="I142" s="9"/>
+      <c r="J142" s="9"/>
+      <c r="K142" s="9"/>
+      <c r="L142" s="9"/>
+      <c r="M142" s="9"/>
+      <c r="N142" s="9"/>
+      <c r="O142" s="9"/>
+      <c r="P142" s="9"/>
+      <c r="Q142" s="9"/>
+      <c r="R142" s="5"/>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A143" s="4"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+      <c r="H143" s="9"/>
+      <c r="I143" s="9"/>
+      <c r="J143" s="9"/>
+      <c r="K143" s="9"/>
+      <c r="L143" s="9"/>
+      <c r="M143" s="9"/>
+      <c r="N143" s="9"/>
+      <c r="O143" s="9"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="9"/>
+      <c r="R143" s="5"/>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A144" s="4"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+      <c r="H144" s="9"/>
+      <c r="I144" s="9"/>
+      <c r="J144" s="9"/>
+      <c r="K144" s="9"/>
+      <c r="L144" s="9"/>
+      <c r="M144" s="9"/>
+      <c r="N144" s="9"/>
+      <c r="O144" s="9"/>
+      <c r="P144" s="9"/>
+      <c r="Q144" s="9"/>
+      <c r="R144" s="5"/>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A145" s="4"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+      <c r="H145" s="9"/>
+      <c r="I145" s="9"/>
+      <c r="J145" s="9"/>
+      <c r="K145" s="9"/>
+      <c r="L145" s="9"/>
+      <c r="M145" s="9"/>
+      <c r="N145" s="9"/>
+      <c r="O145" s="9"/>
+      <c r="P145" s="9"/>
+      <c r="Q145" s="9"/>
+      <c r="R145" s="5"/>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A146" s="4"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="9"/>
+      <c r="H146" s="9"/>
+      <c r="I146" s="9"/>
+      <c r="J146" s="9"/>
+      <c r="K146" s="9"/>
+      <c r="L146" s="9"/>
+      <c r="M146" s="9"/>
+      <c r="N146" s="9"/>
+      <c r="O146" s="9"/>
+      <c r="P146" s="9"/>
+      <c r="Q146" s="9"/>
+      <c r="R146" s="5"/>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A147" s="4"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="9"/>
+      <c r="K147" s="9"/>
+      <c r="L147" s="9"/>
+      <c r="M147" s="9"/>
+      <c r="N147" s="9"/>
+      <c r="O147" s="9"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="9"/>
+      <c r="R147" s="5"/>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A148" s="4"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="9"/>
+      <c r="K148" s="9"/>
+      <c r="L148" s="9"/>
+      <c r="M148" s="9"/>
+      <c r="N148" s="9"/>
+      <c r="O148" s="9"/>
+      <c r="P148" s="9"/>
+      <c r="Q148" s="9"/>
+      <c r="R148" s="5"/>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A149" s="4"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="9"/>
+      <c r="I149" s="9"/>
+      <c r="J149" s="9"/>
+      <c r="K149" s="9"/>
+      <c r="L149" s="9"/>
+      <c r="M149" s="9"/>
+      <c r="N149" s="9"/>
+      <c r="O149" s="9"/>
+      <c r="P149" s="9"/>
+      <c r="Q149" s="9"/>
+      <c r="R149" s="5"/>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A150" s="4"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="9"/>
+      <c r="L150" s="9"/>
+      <c r="M150" s="9"/>
+      <c r="N150" s="9"/>
+      <c r="O150" s="9"/>
+      <c r="P150" s="9"/>
+      <c r="Q150" s="9"/>
+      <c r="R150" s="5"/>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A151" s="4"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+      <c r="H151" s="9"/>
+      <c r="I151" s="9"/>
+      <c r="J151" s="9"/>
+      <c r="K151" s="9"/>
+      <c r="L151" s="9"/>
+      <c r="M151" s="9"/>
+      <c r="N151" s="9"/>
+      <c r="O151" s="9"/>
+      <c r="P151" s="9"/>
+      <c r="Q151" s="9"/>
+      <c r="R151" s="5"/>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A152" s="4"/>
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+      <c r="H152" s="9"/>
+      <c r="I152" s="9"/>
+      <c r="J152" s="9"/>
+      <c r="K152" s="9"/>
+      <c r="L152" s="9"/>
+      <c r="M152" s="9"/>
+      <c r="N152" s="9"/>
+      <c r="O152" s="9"/>
+      <c r="P152" s="9"/>
+      <c r="Q152" s="9"/>
+      <c r="R152" s="5"/>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A153" s="4"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9"/>
+      <c r="L153" s="9"/>
+      <c r="M153" s="9"/>
+      <c r="N153" s="9"/>
+      <c r="O153" s="9"/>
+      <c r="P153" s="9"/>
+      <c r="Q153" s="9"/>
+      <c r="R153" s="5"/>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A154" s="4"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="9"/>
+      <c r="J154" s="9"/>
+      <c r="K154" s="9"/>
+      <c r="L154" s="9"/>
+      <c r="M154" s="9"/>
+      <c r="N154" s="9"/>
+      <c r="O154" s="9"/>
+      <c r="P154" s="9"/>
+      <c r="Q154" s="9"/>
+      <c r="R154" s="5"/>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A155" s="4"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+      <c r="H155" s="9"/>
+      <c r="I155" s="9"/>
+      <c r="J155" s="9"/>
+      <c r="K155" s="9"/>
+      <c r="L155" s="9"/>
+      <c r="M155" s="9"/>
+      <c r="N155" s="9"/>
+      <c r="O155" s="9"/>
+      <c r="P155" s="9"/>
+      <c r="Q155" s="9"/>
+      <c r="R155" s="5"/>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A156" s="4"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="9"/>
+      <c r="J156" s="9"/>
+      <c r="K156" s="9"/>
+      <c r="L156" s="9"/>
+      <c r="M156" s="9"/>
+      <c r="N156" s="9"/>
+      <c r="O156" s="9"/>
+      <c r="P156" s="9"/>
+      <c r="Q156" s="9"/>
+      <c r="R156" s="5"/>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A157" s="4"/>
+      <c r="B157" s="9"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
+      <c r="G157" s="9"/>
+      <c r="H157" s="9"/>
+      <c r="I157" s="9"/>
+      <c r="J157" s="9"/>
+      <c r="K157" s="9"/>
+      <c r="L157" s="9"/>
+      <c r="M157" s="9"/>
+      <c r="N157" s="9"/>
+      <c r="O157" s="9"/>
+      <c r="P157" s="9"/>
+      <c r="Q157" s="9"/>
+      <c r="R157" s="5"/>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A158" s="6"/>
+      <c r="B158" s="7"/>
+      <c r="C158" s="7"/>
+      <c r="D158" s="7"/>
+      <c r="E158" s="7"/>
+      <c r="F158" s="7"/>
+      <c r="G158" s="7"/>
+      <c r="H158" s="7"/>
+      <c r="I158" s="7"/>
+      <c r="J158" s="7"/>
+      <c r="K158" s="7"/>
+      <c r="L158" s="7"/>
+      <c r="M158" s="7"/>
+      <c r="N158" s="7"/>
+      <c r="O158" s="7"/>
+      <c r="P158" s="7"/>
+      <c r="Q158" s="7"/>
+      <c r="R158" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Show a list of all records
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C523A7-2FA6-4361-A1DA-9D6A97E9AEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7785651C-392E-474E-B6ED-FDEBE38AE415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Connect to the database fromPHP" sheetId="3" r:id="rId3"/>
     <sheet name=".env file" sheetId="4" r:id="rId4"/>
     <sheet name="table data gateway class" sheetId="5" r:id="rId5"/>
+    <sheet name="Show a list of all records" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="166">
   <si>
     <t>構成</t>
   </si>
@@ -486,6 +487,48 @@
   </si>
   <si>
     <t>Gọi api và thấy vẫn hoạt động bình thường</t>
+  </si>
+  <si>
+    <t>insert_task_table.sql</t>
+  </si>
+  <si>
+    <t>rest-api-php\4.create-a-restful-api\insert_task_table.sql</t>
+  </si>
+  <si>
+    <t>INSERT INTO task (name, priority, is_completed) VALUES</t>
+  </si>
+  <si>
+    <t>    ('Buy new shoes', 1, true),</t>
+  </si>
+  <si>
+    <t>    ('Renew passport', 2, false),</t>
+  </si>
+  <si>
+    <t>    ('Paint wall', NULL, true);</t>
+  </si>
+  <si>
+    <t>    public function getAll(): array</t>
+  </si>
+  <si>
+    <t>        $sql = "SELECT *</t>
+  </si>
+  <si>
+    <t>                FROM task</t>
+  </si>
+  <si>
+    <t>                ORDER BY name";</t>
+  </si>
+  <si>
+    <t>        $stmt = $this-&gt;conn-&gt;query($sql);</t>
+  </si>
+  <si>
+    <t>        return $stmt-&gt;fetchAll(PDO::FETCH_ASSOC);</t>
+  </si>
+  <si>
+    <t>                echo json_encode($this-&gt;gateway-&gt;getAll());</t>
+  </si>
+  <si>
+    <t>Kết quả trả về dạng mảng</t>
   </si>
 </sst>
 </file>
@@ -1954,6 +1997,249 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>532663</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66464</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E2E2395-808D-F97D-9BA1-E9895D644163}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8048625" y="3333750"/>
+          <a:ext cx="5895238" cy="1685714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>542109</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>94887</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{890F2FAA-C5FD-36C6-DF3E-9F05DC389E0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8039100" y="5381625"/>
+          <a:ext cx="6523809" cy="2904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D01B97B-0E09-7C46-C417-AECFC3A448D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3371850" y="5467350"/>
+          <a:ext cx="4543425" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBE44394-EE63-FFAB-3B9C-3B274227C2B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1809750" y="11039475"/>
+          <a:ext cx="1524000" cy="5781675"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>408321</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>37459</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86FBF3BC-73A6-BD87-80AD-B5E0EF5731D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="742950" y="24441150"/>
+          <a:ext cx="10028571" cy="5123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8305,8 +8591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA190C99-A3E9-4F93-9540-3F02D2357A9D}">
   <dimension ref="A2:R158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10278,4 +10564,2193 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF5B913-A637-422C-8D40-BE71A2590EEF}">
+  <dimension ref="A4:X157"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="C159" sqref="C159"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="5"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="3"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="5"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="5"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="5"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="5"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="5"/>
+      <c r="K21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" t="s">
+        <v>36</v>
+      </c>
+      <c r="N21" s="4"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="5"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="5"/>
+      <c r="K22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+      <c r="N22" s="4"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="5"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="5"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="5"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="5"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="5"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="5"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="5"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="5"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="9"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="5"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="5"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="5"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="8"/>
+      <c r="K28" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" s="4"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="5"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N29" s="4"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="5"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N30" s="4"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="5"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+      <c r="N31" s="4"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="5"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="5"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="5"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="9"/>
+      <c r="U33" s="9"/>
+      <c r="V33" s="9"/>
+      <c r="W33" s="9"/>
+      <c r="X33" s="5"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="5"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="9"/>
+      <c r="U34" s="9"/>
+      <c r="V34" s="9"/>
+      <c r="W34" s="9"/>
+      <c r="X34" s="5"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="5"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N36" s="4"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="5"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N37" s="4"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="9"/>
+      <c r="U37" s="9"/>
+      <c r="V37" s="9"/>
+      <c r="W37" s="9"/>
+      <c r="X37" s="5"/>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N38" s="4"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="5"/>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N39" s="4"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="9"/>
+      <c r="U39" s="9"/>
+      <c r="V39" s="9"/>
+      <c r="W39" s="9"/>
+      <c r="X39" s="5"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N40" s="4"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="9"/>
+      <c r="X40" s="5"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N41" s="4"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="9"/>
+      <c r="W41" s="9"/>
+      <c r="X41" s="5"/>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N42" s="4"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="9"/>
+      <c r="U42" s="9"/>
+      <c r="V42" s="9"/>
+      <c r="W42" s="9"/>
+      <c r="X42" s="5"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N43" s="4"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="5"/>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N44" s="4"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
+      <c r="W44" s="9"/>
+      <c r="X44" s="5"/>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="N45" s="6"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
+      <c r="S45" s="7"/>
+      <c r="T45" s="7"/>
+      <c r="U45" s="7"/>
+      <c r="V45" s="7"/>
+      <c r="W45" s="7"/>
+      <c r="X45" s="8"/>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="15"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="15"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B66" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="5"/>
+      <c r="H66" t="s">
+        <v>34</v>
+      </c>
+      <c r="I66" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B67" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="5"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="8"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+      <c r="H72" s="2"/>
+      <c r="I72" s="3"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="4"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="4"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="4"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="4"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="9"/>
+      <c r="H109" s="9"/>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="4"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="9"/>
+      <c r="H113" s="9"/>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="9"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="5"/>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="5"/>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B120" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="5"/>
+    </row>
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
+      <c r="H121" s="9"/>
+      <c r="I121" s="5"/>
+    </row>
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B122" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="9"/>
+      <c r="H122" s="9"/>
+      <c r="I122" s="5"/>
+    </row>
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="5"/>
+    </row>
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B124" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C124" s="7"/>
+      <c r="D124" s="7"/>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
+      <c r="G124" s="7"/>
+      <c r="H124" s="7"/>
+      <c r="I124" s="8"/>
+    </row>
+    <row r="126" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A127" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B127" s="18"/>
+      <c r="C127" s="18"/>
+      <c r="D127" s="18"/>
+      <c r="E127" s="18"/>
+      <c r="F127" s="18"/>
+      <c r="G127" s="18"/>
+      <c r="H127" s="18"/>
+      <c r="I127" s="18"/>
+      <c r="J127" s="18"/>
+      <c r="K127" s="18"/>
+      <c r="L127" s="18"/>
+      <c r="M127" s="18"/>
+      <c r="N127" s="18"/>
+      <c r="O127" s="18"/>
+      <c r="P127" s="18"/>
+      <c r="Q127" s="18"/>
+      <c r="R127" s="19"/>
+    </row>
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A128" s="20"/>
+      <c r="B128" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="9"/>
+      <c r="I128" s="9"/>
+      <c r="J128" s="9"/>
+      <c r="K128" s="9"/>
+      <c r="L128" s="9"/>
+      <c r="M128" s="9"/>
+      <c r="N128" s="9"/>
+      <c r="O128" s="9"/>
+      <c r="P128" s="9"/>
+      <c r="Q128" s="9"/>
+      <c r="R128" s="21"/>
+    </row>
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A129" s="20"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+      <c r="H129" s="9"/>
+      <c r="I129" s="9"/>
+      <c r="J129" s="9"/>
+      <c r="K129" s="9"/>
+      <c r="L129" s="9"/>
+      <c r="M129" s="9"/>
+      <c r="N129" s="9"/>
+      <c r="O129" s="9"/>
+      <c r="P129" s="9"/>
+      <c r="Q129" s="9"/>
+      <c r="R129" s="21"/>
+    </row>
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A130" s="20"/>
+      <c r="B130" s="9"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9"/>
+      <c r="H130" s="9"/>
+      <c r="I130" s="9"/>
+      <c r="J130" s="9"/>
+      <c r="K130" s="9"/>
+      <c r="L130" s="9"/>
+      <c r="M130" s="9"/>
+      <c r="N130" s="9"/>
+      <c r="O130" s="9"/>
+      <c r="P130" s="9"/>
+      <c r="Q130" s="9"/>
+      <c r="R130" s="21"/>
+    </row>
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A131" s="20"/>
+      <c r="B131" s="9"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="9"/>
+      <c r="J131" s="9"/>
+      <c r="K131" s="9"/>
+      <c r="L131" s="9"/>
+      <c r="M131" s="9"/>
+      <c r="N131" s="9"/>
+      <c r="O131" s="9"/>
+      <c r="P131" s="9"/>
+      <c r="Q131" s="9"/>
+      <c r="R131" s="21"/>
+    </row>
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A132" s="20"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="9"/>
+      <c r="J132" s="9"/>
+      <c r="K132" s="9"/>
+      <c r="L132" s="9"/>
+      <c r="M132" s="9"/>
+      <c r="N132" s="9"/>
+      <c r="O132" s="9"/>
+      <c r="P132" s="9"/>
+      <c r="Q132" s="9"/>
+      <c r="R132" s="21"/>
+    </row>
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A133" s="20"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="9"/>
+      <c r="K133" s="9"/>
+      <c r="L133" s="9"/>
+      <c r="M133" s="9"/>
+      <c r="N133" s="9"/>
+      <c r="O133" s="9"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="9"/>
+      <c r="R133" s="21"/>
+    </row>
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A134" s="20"/>
+      <c r="B134" s="9"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="9"/>
+      <c r="J134" s="9"/>
+      <c r="K134" s="9"/>
+      <c r="L134" s="9"/>
+      <c r="M134" s="9"/>
+      <c r="N134" s="9"/>
+      <c r="O134" s="9"/>
+      <c r="P134" s="9"/>
+      <c r="Q134" s="9"/>
+      <c r="R134" s="21"/>
+    </row>
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A135" s="20"/>
+      <c r="B135" s="9"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="9"/>
+      <c r="J135" s="9"/>
+      <c r="K135" s="9"/>
+      <c r="L135" s="9"/>
+      <c r="M135" s="9"/>
+      <c r="N135" s="9"/>
+      <c r="O135" s="9"/>
+      <c r="P135" s="9"/>
+      <c r="Q135" s="9"/>
+      <c r="R135" s="21"/>
+    </row>
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A136" s="20"/>
+      <c r="B136" s="9"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="9"/>
+      <c r="J136" s="9"/>
+      <c r="K136" s="9"/>
+      <c r="L136" s="9"/>
+      <c r="M136" s="9"/>
+      <c r="N136" s="9"/>
+      <c r="O136" s="9"/>
+      <c r="P136" s="9"/>
+      <c r="Q136" s="9"/>
+      <c r="R136" s="21"/>
+    </row>
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A137" s="20"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="9"/>
+      <c r="J137" s="9"/>
+      <c r="K137" s="9"/>
+      <c r="L137" s="9"/>
+      <c r="M137" s="9"/>
+      <c r="N137" s="9"/>
+      <c r="O137" s="9"/>
+      <c r="P137" s="9"/>
+      <c r="Q137" s="9"/>
+      <c r="R137" s="21"/>
+    </row>
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A138" s="20"/>
+      <c r="B138" s="9"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="9"/>
+      <c r="H138" s="9"/>
+      <c r="I138" s="9"/>
+      <c r="J138" s="9"/>
+      <c r="K138" s="9"/>
+      <c r="L138" s="9"/>
+      <c r="M138" s="9"/>
+      <c r="N138" s="9"/>
+      <c r="O138" s="9"/>
+      <c r="P138" s="9"/>
+      <c r="Q138" s="9"/>
+      <c r="R138" s="21"/>
+    </row>
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A139" s="20"/>
+      <c r="B139" s="9"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+      <c r="H139" s="9"/>
+      <c r="I139" s="9"/>
+      <c r="J139" s="9"/>
+      <c r="K139" s="9"/>
+      <c r="L139" s="9"/>
+      <c r="M139" s="9"/>
+      <c r="N139" s="9"/>
+      <c r="O139" s="9"/>
+      <c r="P139" s="9"/>
+      <c r="Q139" s="9"/>
+      <c r="R139" s="21"/>
+    </row>
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A140" s="20"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="9"/>
+      <c r="K140" s="9"/>
+      <c r="L140" s="9"/>
+      <c r="M140" s="9"/>
+      <c r="N140" s="9"/>
+      <c r="O140" s="9"/>
+      <c r="P140" s="9"/>
+      <c r="Q140" s="9"/>
+      <c r="R140" s="21"/>
+    </row>
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A141" s="20"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+      <c r="I141" s="9"/>
+      <c r="J141" s="9"/>
+      <c r="K141" s="9"/>
+      <c r="L141" s="9"/>
+      <c r="M141" s="9"/>
+      <c r="N141" s="9"/>
+      <c r="O141" s="9"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="9"/>
+      <c r="R141" s="21"/>
+    </row>
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A142" s="20"/>
+      <c r="B142" s="9"/>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+      <c r="H142" s="9"/>
+      <c r="I142" s="9"/>
+      <c r="J142" s="9"/>
+      <c r="K142" s="9"/>
+      <c r="L142" s="9"/>
+      <c r="M142" s="9"/>
+      <c r="N142" s="9"/>
+      <c r="O142" s="9"/>
+      <c r="P142" s="9"/>
+      <c r="Q142" s="9"/>
+      <c r="R142" s="21"/>
+    </row>
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A143" s="20"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+      <c r="H143" s="9"/>
+      <c r="I143" s="9"/>
+      <c r="J143" s="9"/>
+      <c r="K143" s="9"/>
+      <c r="L143" s="9"/>
+      <c r="M143" s="9"/>
+      <c r="N143" s="9"/>
+      <c r="O143" s="9"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="9"/>
+      <c r="R143" s="21"/>
+    </row>
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A144" s="20"/>
+      <c r="B144" s="9"/>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+      <c r="H144" s="9"/>
+      <c r="I144" s="9"/>
+      <c r="J144" s="9"/>
+      <c r="K144" s="9"/>
+      <c r="L144" s="9"/>
+      <c r="M144" s="9"/>
+      <c r="N144" s="9"/>
+      <c r="O144" s="9"/>
+      <c r="P144" s="9"/>
+      <c r="Q144" s="9"/>
+      <c r="R144" s="21"/>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A145" s="20"/>
+      <c r="B145" s="9"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+      <c r="H145" s="9"/>
+      <c r="I145" s="9"/>
+      <c r="J145" s="9"/>
+      <c r="K145" s="9"/>
+      <c r="L145" s="9"/>
+      <c r="M145" s="9"/>
+      <c r="N145" s="9"/>
+      <c r="O145" s="9"/>
+      <c r="P145" s="9"/>
+      <c r="Q145" s="9"/>
+      <c r="R145" s="21"/>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A146" s="20"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="9"/>
+      <c r="H146" s="9"/>
+      <c r="I146" s="9"/>
+      <c r="J146" s="9"/>
+      <c r="K146" s="9"/>
+      <c r="L146" s="9"/>
+      <c r="M146" s="9"/>
+      <c r="N146" s="9"/>
+      <c r="O146" s="9"/>
+      <c r="P146" s="9"/>
+      <c r="Q146" s="9"/>
+      <c r="R146" s="21"/>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A147" s="20"/>
+      <c r="B147" s="9"/>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="9"/>
+      <c r="K147" s="9"/>
+      <c r="L147" s="9"/>
+      <c r="M147" s="9"/>
+      <c r="N147" s="9"/>
+      <c r="O147" s="9"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="9"/>
+      <c r="R147" s="21"/>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A148" s="20"/>
+      <c r="B148" s="9"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="9"/>
+      <c r="K148" s="9"/>
+      <c r="L148" s="9"/>
+      <c r="M148" s="9"/>
+      <c r="N148" s="9"/>
+      <c r="O148" s="9"/>
+      <c r="P148" s="9"/>
+      <c r="Q148" s="9"/>
+      <c r="R148" s="21"/>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A149" s="20"/>
+      <c r="B149" s="9"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="9"/>
+      <c r="I149" s="9"/>
+      <c r="J149" s="9"/>
+      <c r="K149" s="9"/>
+      <c r="L149" s="9"/>
+      <c r="M149" s="9"/>
+      <c r="N149" s="9"/>
+      <c r="O149" s="9"/>
+      <c r="P149" s="9"/>
+      <c r="Q149" s="9"/>
+      <c r="R149" s="21"/>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A150" s="20"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="9"/>
+      <c r="L150" s="9"/>
+      <c r="M150" s="9"/>
+      <c r="N150" s="9"/>
+      <c r="O150" s="9"/>
+      <c r="P150" s="9"/>
+      <c r="Q150" s="9"/>
+      <c r="R150" s="21"/>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A151" s="20"/>
+      <c r="B151" s="9"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+      <c r="H151" s="9"/>
+      <c r="I151" s="9"/>
+      <c r="J151" s="9"/>
+      <c r="K151" s="9"/>
+      <c r="L151" s="9"/>
+      <c r="M151" s="9"/>
+      <c r="N151" s="9"/>
+      <c r="O151" s="9"/>
+      <c r="P151" s="9"/>
+      <c r="Q151" s="9"/>
+      <c r="R151" s="21"/>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A152" s="20"/>
+      <c r="B152" s="9"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+      <c r="H152" s="9"/>
+      <c r="I152" s="9"/>
+      <c r="J152" s="9"/>
+      <c r="K152" s="9"/>
+      <c r="L152" s="9"/>
+      <c r="M152" s="9"/>
+      <c r="N152" s="9"/>
+      <c r="O152" s="9"/>
+      <c r="P152" s="9"/>
+      <c r="Q152" s="9"/>
+      <c r="R152" s="21"/>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A153" s="20"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9"/>
+      <c r="L153" s="9"/>
+      <c r="M153" s="9"/>
+      <c r="N153" s="9"/>
+      <c r="O153" s="9"/>
+      <c r="P153" s="9"/>
+      <c r="Q153" s="9"/>
+      <c r="R153" s="21"/>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A154" s="20"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="9"/>
+      <c r="J154" s="9"/>
+      <c r="K154" s="9"/>
+      <c r="L154" s="9"/>
+      <c r="M154" s="9"/>
+      <c r="N154" s="9"/>
+      <c r="O154" s="9"/>
+      <c r="P154" s="9"/>
+      <c r="Q154" s="9"/>
+      <c r="R154" s="21"/>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A155" s="20"/>
+      <c r="B155" s="9"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+      <c r="H155" s="9"/>
+      <c r="I155" s="9"/>
+      <c r="J155" s="9"/>
+      <c r="K155" s="9"/>
+      <c r="L155" s="9"/>
+      <c r="M155" s="9"/>
+      <c r="N155" s="9"/>
+      <c r="O155" s="9"/>
+      <c r="P155" s="9"/>
+      <c r="Q155" s="9"/>
+      <c r="R155" s="21"/>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A156" s="20"/>
+      <c r="B156" s="9"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="9"/>
+      <c r="J156" s="9"/>
+      <c r="K156" s="9"/>
+      <c r="L156" s="9"/>
+      <c r="M156" s="9"/>
+      <c r="N156" s="9"/>
+      <c r="O156" s="9"/>
+      <c r="P156" s="9"/>
+      <c r="Q156" s="9"/>
+      <c r="R156" s="21"/>
+    </row>
+    <row r="157" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A157" s="22"/>
+      <c r="B157" s="23"/>
+      <c r="C157" s="23"/>
+      <c r="D157" s="23"/>
+      <c r="E157" s="23"/>
+      <c r="F157" s="23"/>
+      <c r="G157" s="23"/>
+      <c r="H157" s="23"/>
+      <c r="I157" s="23"/>
+      <c r="J157" s="23"/>
+      <c r="K157" s="23"/>
+      <c r="L157" s="23"/>
+      <c r="M157" s="23"/>
+      <c r="N157" s="23"/>
+      <c r="O157" s="23"/>
+      <c r="P157" s="23"/>
+      <c r="Q157" s="23"/>
+      <c r="R157" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Configure PDO to prevent numeric values from being converted to strings
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7785651C-392E-474E-B6ED-FDEBE38AE415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392439E2-B7FC-4132-BDFC-F26707EED9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name=".env file" sheetId="4" r:id="rId4"/>
     <sheet name="table data gateway class" sheetId="5" r:id="rId5"/>
     <sheet name="Show a list of all records" sheetId="6" r:id="rId6"/>
+    <sheet name="prevent numeric converted toStr" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="193">
   <si>
     <t>構成</t>
   </si>
@@ -529,6 +530,221 @@
   </si>
   <si>
     <t>Kết quả trả về dạng mảng</t>
+  </si>
+  <si>
+    <t>Configure PDO to prevent numeric values from being converted to strings</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "Buy new shoes",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    },</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "Paint wall",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "priority": null,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        "name": "Renew passport",</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "id": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "priority": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "is_completed": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"1"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "id": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"3"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "id": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"2"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "priority": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"2"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">        "is_completed": </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"0"</t>
+    </r>
+  </si>
+  <si>
+    <t>Hiện tại các giá trị api trả về đang có dạng string bất kể kiểu dữ liệu trong Database là kiểu số hoặc boolean</t>
+  </si>
+  <si>
+    <t>Tuy nhiên thì các giá trị json thì có thể là string, number, boolean, object, array hoặc null</t>
+  </si>
+  <si>
+    <t>https://www.json.org/json-en.html</t>
+  </si>
+  <si>
+    <t>            PDO::ATTR_ERRMODE =&gt; PDO::ERRMODE_EXCEPTION,</t>
+  </si>
+  <si>
+    <t>            PDO::ATTR_EMULATE_PREPARES =&gt; false,</t>
+  </si>
+  <si>
+    <t>            PDO::ATTR_STRINGIFY_FETCHES =&gt; false</t>
+  </si>
+  <si>
+    <t>Nếu ATTR_EMULATE_PREPARES được set true thì có thể ảnh hưởng đến kiểu dữ liệu trả về sau khi query data từ DB ra</t>
+  </si>
+  <si>
+    <t>Nếu ATTR_STRINGIFY_FETCHES được set true thì sẽ thực hiện convert tất cả các giá trị về kiểu string</t>
+  </si>
+  <si>
+    <t>setattribute</t>
+  </si>
+  <si>
+    <t>https://www.php.net/manual/en/pdo.setattribute.php</t>
   </si>
 </sst>
 </file>
@@ -749,7 +965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -782,6 +998,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2240,6 +2465,346 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>236973</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>170631</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAC0BD3-BB98-760C-3085-27ACFFB230E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="5619750"/>
+          <a:ext cx="9219048" cy="6552381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>17918</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>18317</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FC98C0E-0B0F-0EEF-009F-AD45AD917453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="13201650"/>
+          <a:ext cx="9057143" cy="5866667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>436889</xdr:colOff>
+      <xdr:row>194</xdr:row>
+      <xdr:rowOff>46984</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{287F449D-D974-1884-F99F-C91793B2BE41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="714375" y="31880175"/>
+          <a:ext cx="10085714" cy="5123809"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>188700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E356FC6E-697C-425F-AECC-C3EB433B6FBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4448175" y="866775"/>
+          <a:ext cx="7248525" cy="3703425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{933F7D98-DBDA-6E95-EA5A-B04F3679C7F9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2019300" y="533400"/>
+          <a:ext cx="3943350" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B12132C1-F28D-8C7D-C74B-73C80898399E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2657475" y="561975"/>
+          <a:ext cx="3924300" cy="1257300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>180</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85DD2651-6FA9-E672-C59A-5B356884A61F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2181225" y="2828925"/>
+          <a:ext cx="3362325" cy="31623000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -10570,8 +11135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF5B913-A637-422C-8D40-BE71A2590EEF}">
   <dimension ref="A4:X157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" workbookViewId="0">
-      <selection activeCell="C159" sqref="C159"/>
+    <sheetView topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12753,4 +13318,3299 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E626A40E-2901-4376-94B0-2A64A7359002}">
+  <dimension ref="A2:T196"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="G203" sqref="G203"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+      <c r="T10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="5"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+      <c r="T13" s="5"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="5"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="8"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="5"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="5"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="5"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="5"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="5"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="5"/>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="5"/>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="5"/>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="5"/>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="5"/>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="5"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="5"/>
+    </row>
+    <row r="51" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="5"/>
+    </row>
+    <row r="52" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="5"/>
+    </row>
+    <row r="53" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="5"/>
+    </row>
+    <row r="54" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="5"/>
+    </row>
+    <row r="55" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="5"/>
+    </row>
+    <row r="56" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="5"/>
+    </row>
+    <row r="57" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="5"/>
+    </row>
+    <row r="58" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B58" s="4"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
+      <c r="Q58" s="5"/>
+    </row>
+    <row r="59" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="O59" s="9"/>
+      <c r="P59" s="9"/>
+      <c r="Q59" s="5"/>
+    </row>
+    <row r="60" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="5"/>
+    </row>
+    <row r="61" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B61" s="4"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
+      <c r="L61" s="9"/>
+      <c r="M61" s="9"/>
+      <c r="N61" s="9"/>
+      <c r="O61" s="9"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="5"/>
+    </row>
+    <row r="62" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+      <c r="O62" s="9"/>
+      <c r="P62" s="9"/>
+      <c r="Q62" s="5"/>
+    </row>
+    <row r="63" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+      <c r="O63" s="9"/>
+      <c r="P63" s="9"/>
+      <c r="Q63" s="5"/>
+    </row>
+    <row r="64" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="5"/>
+    </row>
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B65" s="6"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="8"/>
+    </row>
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B68" s="25" t="s">
+        <v>191</v>
+      </c>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="3"/>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B69" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="9"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="5"/>
+    </row>
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B70" s="27"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+      <c r="O70" s="9"/>
+      <c r="P70" s="9"/>
+      <c r="Q70" s="5"/>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B71" s="27"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="5"/>
+    </row>
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B72" s="27"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+      <c r="O72" s="9"/>
+      <c r="P72" s="9"/>
+      <c r="Q72" s="5"/>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B73" s="27"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="5"/>
+    </row>
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B74" s="27"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
+      <c r="O74" s="9"/>
+      <c r="P74" s="9"/>
+      <c r="Q74" s="5"/>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B75" s="27"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
+      <c r="O75" s="9"/>
+      <c r="P75" s="9"/>
+      <c r="Q75" s="5"/>
+    </row>
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B76" s="27"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="5"/>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B77" s="27"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+      <c r="O77" s="9"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="5"/>
+    </row>
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B78" s="27"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="5"/>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B79" s="27"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
+      <c r="O79" s="9"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="5"/>
+    </row>
+    <row r="80" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B80" s="27"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
+      <c r="O80" s="9"/>
+      <c r="P80" s="9"/>
+      <c r="Q80" s="5"/>
+    </row>
+    <row r="81" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B81" s="27"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="9"/>
+      <c r="O81" s="9"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="5"/>
+    </row>
+    <row r="82" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B82" s="27"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="5"/>
+    </row>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B83" s="27"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="9"/>
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="9"/>
+      <c r="O83" s="9"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="5"/>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B84" s="27"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
+      <c r="O84" s="9"/>
+      <c r="P84" s="9"/>
+      <c r="Q84" s="5"/>
+    </row>
+    <row r="85" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B85" s="27"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
+      <c r="O85" s="9"/>
+      <c r="P85" s="9"/>
+      <c r="Q85" s="5"/>
+    </row>
+    <row r="86" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B86" s="27"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="9"/>
+      <c r="O86" s="9"/>
+      <c r="P86" s="9"/>
+      <c r="Q86" s="5"/>
+    </row>
+    <row r="87" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B87" s="27"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
+      <c r="O87" s="9"/>
+      <c r="P87" s="9"/>
+      <c r="Q87" s="5"/>
+    </row>
+    <row r="88" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B88" s="27"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
+      <c r="O88" s="9"/>
+      <c r="P88" s="9"/>
+      <c r="Q88" s="5"/>
+    </row>
+    <row r="89" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B89" s="27"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
+      <c r="O89" s="9"/>
+      <c r="P89" s="9"/>
+      <c r="Q89" s="5"/>
+    </row>
+    <row r="90" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B90" s="27"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="9"/>
+      <c r="P90" s="9"/>
+      <c r="Q90" s="5"/>
+    </row>
+    <row r="91" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B91" s="27"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="9"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="5"/>
+    </row>
+    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B92" s="27"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="9"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="9"/>
+      <c r="P92" s="9"/>
+      <c r="Q92" s="5"/>
+    </row>
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B93" s="27"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="9"/>
+      <c r="O93" s="9"/>
+      <c r="P93" s="9"/>
+      <c r="Q93" s="5"/>
+    </row>
+    <row r="94" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B94" s="27"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="9"/>
+      <c r="K94" s="9"/>
+      <c r="L94" s="9"/>
+      <c r="M94" s="9"/>
+      <c r="N94" s="9"/>
+      <c r="O94" s="9"/>
+      <c r="P94" s="9"/>
+      <c r="Q94" s="5"/>
+    </row>
+    <row r="95" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B95" s="27"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="9"/>
+      <c r="M95" s="9"/>
+      <c r="N95" s="9"/>
+      <c r="O95" s="9"/>
+      <c r="P95" s="9"/>
+      <c r="Q95" s="5"/>
+    </row>
+    <row r="96" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B96" s="27"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="9"/>
+      <c r="K96" s="9"/>
+      <c r="L96" s="9"/>
+      <c r="M96" s="9"/>
+      <c r="N96" s="9"/>
+      <c r="O96" s="9"/>
+      <c r="P96" s="9"/>
+      <c r="Q96" s="5"/>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B97" s="27"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="9"/>
+      <c r="K97" s="9"/>
+      <c r="L97" s="9"/>
+      <c r="M97" s="9"/>
+      <c r="N97" s="9"/>
+      <c r="O97" s="9"/>
+      <c r="P97" s="9"/>
+      <c r="Q97" s="5"/>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B98" s="27"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="9"/>
+      <c r="L98" s="9"/>
+      <c r="M98" s="9"/>
+      <c r="N98" s="9"/>
+      <c r="O98" s="9"/>
+      <c r="P98" s="9"/>
+      <c r="Q98" s="5"/>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B99" s="27"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="9"/>
+      <c r="O99" s="9"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="5"/>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B100" s="4"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="9"/>
+      <c r="J100" s="9"/>
+      <c r="K100" s="9"/>
+      <c r="L100" s="9"/>
+      <c r="M100" s="9"/>
+      <c r="N100" s="9"/>
+      <c r="O100" s="9"/>
+      <c r="P100" s="9"/>
+      <c r="Q100" s="5"/>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B101" s="6"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="7"/>
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="7"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="7"/>
+      <c r="P101" s="7"/>
+      <c r="Q101" s="8"/>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B102" s="9"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="9"/>
+      <c r="M102" s="9"/>
+      <c r="N102" s="9"/>
+      <c r="O102" s="9"/>
+      <c r="P102" s="9"/>
+      <c r="Q102" s="9"/>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="32"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="32"/>
+      <c r="J104" s="32"/>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" s="32"/>
+      <c r="B105" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="34"/>
+      <c r="D105" s="34"/>
+      <c r="E105" s="34"/>
+      <c r="F105" s="34"/>
+      <c r="G105" s="34"/>
+      <c r="H105" s="34"/>
+      <c r="I105" s="34"/>
+      <c r="J105" s="35"/>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" s="32"/>
+      <c r="B106" s="36"/>
+      <c r="C106" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" s="11"/>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="11"/>
+      <c r="I106" s="11"/>
+      <c r="J106" s="37"/>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" s="32"/>
+      <c r="B107" s="36"/>
+      <c r="C107" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" s="11"/>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="37"/>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108" s="32"/>
+      <c r="B108" s="36"/>
+      <c r="C108" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11"/>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="37"/>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
+      <c r="B109" s="36"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11"/>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="37"/>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A110" s="32"/>
+      <c r="B110" s="36"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F110" s="11"/>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="37"/>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A111" s="32"/>
+      <c r="B111" s="36"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F111" s="11"/>
+      <c r="G111" s="11"/>
+      <c r="H111" s="11"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="37"/>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A112" s="32"/>
+      <c r="B112" s="36"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11"/>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
+      <c r="I112" s="11"/>
+      <c r="J112" s="37"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="32"/>
+      <c r="B113" s="36"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11"/>
+      <c r="G113" s="11"/>
+      <c r="H113" s="11"/>
+      <c r="I113" s="11"/>
+      <c r="J113" s="37"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="32"/>
+      <c r="B114" s="36"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11"/>
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="37"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="32"/>
+      <c r="B115" s="36"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" s="11"/>
+      <c r="G115" s="11"/>
+      <c r="H115" s="11"/>
+      <c r="I115" s="11"/>
+      <c r="J115" s="37"/>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="32"/>
+      <c r="B116" s="36"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="11"/>
+      <c r="F116" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G116" s="11"/>
+      <c r="H116" s="11"/>
+      <c r="I116" s="11"/>
+      <c r="J116" s="37"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="32"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="11"/>
+      <c r="F117" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G117" s="11"/>
+      <c r="H117" s="11"/>
+      <c r="I117" s="11"/>
+      <c r="J117" s="37"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="32"/>
+      <c r="B118" s="36"/>
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F118" s="11"/>
+      <c r="G118" s="11"/>
+      <c r="H118" s="11"/>
+      <c r="I118" s="11"/>
+      <c r="J118" s="37"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="32"/>
+      <c r="B119" s="36"/>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="11"/>
+      <c r="F119" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G119" s="11"/>
+      <c r="H119" s="11"/>
+      <c r="I119" s="11"/>
+      <c r="J119" s="37"/>
+      <c r="K119" t="s">
+        <v>34</v>
+      </c>
+      <c r="L119" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
+      <c r="B120" s="36"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="11"/>
+      <c r="F120" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G120" s="11"/>
+      <c r="H120" s="11"/>
+      <c r="I120" s="11"/>
+      <c r="J120" s="37"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" s="32"/>
+      <c r="B121" s="36"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="11"/>
+      <c r="E121" s="11"/>
+      <c r="F121" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G121" s="11"/>
+      <c r="H121" s="11"/>
+      <c r="I121" s="11"/>
+      <c r="J121" s="37"/>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" s="32"/>
+      <c r="B122" s="36"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="11"/>
+      <c r="E122" s="11"/>
+      <c r="F122" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G122" s="11"/>
+      <c r="H122" s="11"/>
+      <c r="I122" s="11"/>
+      <c r="J122" s="37"/>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" s="32"/>
+      <c r="B123" s="36"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F123" s="11"/>
+      <c r="G123" s="11"/>
+      <c r="H123" s="11"/>
+      <c r="I123" s="11"/>
+      <c r="J123" s="37"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" s="32"/>
+      <c r="B124" s="36"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="11"/>
+      <c r="E124" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F124" s="11"/>
+      <c r="G124" s="11"/>
+      <c r="H124" s="11"/>
+      <c r="I124" s="11"/>
+      <c r="J124" s="37"/>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" s="32"/>
+      <c r="B125" s="36"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="11"/>
+      <c r="E125" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F125" s="11"/>
+      <c r="G125" s="11"/>
+      <c r="H125" s="11"/>
+      <c r="I125" s="11"/>
+      <c r="J125" s="37"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" s="32"/>
+      <c r="B126" s="36"/>
+      <c r="C126" s="11"/>
+      <c r="D126" s="11"/>
+      <c r="E126" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F126" s="11"/>
+      <c r="G126" s="11"/>
+      <c r="H126" s="11"/>
+      <c r="I126" s="11"/>
+      <c r="J126" s="37"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" s="32"/>
+      <c r="B127" s="36"/>
+      <c r="C127" s="11"/>
+      <c r="D127" s="11"/>
+      <c r="E127" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F127" s="11"/>
+      <c r="G127" s="11"/>
+      <c r="H127" s="11"/>
+      <c r="I127" s="11"/>
+      <c r="J127" s="37"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" s="32"/>
+      <c r="B128" s="38"/>
+      <c r="C128" s="39"/>
+      <c r="D128" s="39"/>
+      <c r="E128" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F128" s="39"/>
+      <c r="G128" s="39"/>
+      <c r="H128" s="39"/>
+      <c r="I128" s="39"/>
+      <c r="J128" s="40"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B132" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
+      <c r="E132" s="2"/>
+      <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
+      <c r="H132" s="2"/>
+      <c r="I132" s="3"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B133" s="4"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="5"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="5"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="5"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="5"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="5"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="9"/>
+      <c r="H138" s="9"/>
+      <c r="I138" s="5"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+      <c r="H139" s="9"/>
+      <c r="I139" s="5"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="4"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="5"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+      <c r="I141" s="5"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+      <c r="H142" s="9"/>
+      <c r="I142" s="5"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+      <c r="H143" s="9"/>
+      <c r="I143" s="5"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B144" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+      <c r="H144" s="9"/>
+      <c r="I144" s="5"/>
+    </row>
+    <row r="145" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+      <c r="H145" s="9"/>
+      <c r="I145" s="5"/>
+    </row>
+    <row r="146" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B146" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="9"/>
+      <c r="H146" s="9"/>
+      <c r="I146" s="5"/>
+    </row>
+    <row r="147" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B147" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="5"/>
+    </row>
+    <row r="148" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="5"/>
+    </row>
+    <row r="149" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="9"/>
+      <c r="I149" s="5"/>
+    </row>
+    <row r="150" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="5"/>
+    </row>
+    <row r="151" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+      <c r="H151" s="9"/>
+      <c r="I151" s="5"/>
+    </row>
+    <row r="152" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B152" s="4"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+      <c r="H152" s="9"/>
+      <c r="I152" s="5"/>
+    </row>
+    <row r="153" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="5"/>
+    </row>
+    <row r="154" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B154" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="5"/>
+    </row>
+    <row r="155" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B155" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+      <c r="H155" s="9"/>
+      <c r="I155" s="5"/>
+    </row>
+    <row r="156" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="5"/>
+    </row>
+    <row r="157" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B157" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
+      <c r="G157" s="9"/>
+      <c r="H157" s="9"/>
+      <c r="I157" s="5"/>
+    </row>
+    <row r="158" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B158" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9"/>
+      <c r="G158" s="9"/>
+      <c r="H158" s="9"/>
+      <c r="I158" s="5"/>
+    </row>
+    <row r="159" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B159" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="9"/>
+      <c r="H159" s="9"/>
+      <c r="I159" s="5"/>
+      <c r="J159" t="s">
+        <v>34</v>
+      </c>
+      <c r="K159" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="160" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B160" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
+      <c r="G160" s="9"/>
+      <c r="H160" s="9"/>
+      <c r="I160" s="5"/>
+      <c r="J160" t="s">
+        <v>34</v>
+      </c>
+      <c r="K160" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="161" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B161" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="9"/>
+      <c r="H161" s="9"/>
+      <c r="I161" s="5"/>
+    </row>
+    <row r="162" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B162" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="5"/>
+    </row>
+    <row r="163" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B163" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C163" s="7"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7"/>
+      <c r="F163" s="7"/>
+      <c r="G163" s="7"/>
+      <c r="H163" s="7"/>
+      <c r="I163" s="8"/>
+    </row>
+    <row r="165" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="166" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A166" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B166" s="18"/>
+      <c r="C166" s="18"/>
+      <c r="D166" s="18"/>
+      <c r="E166" s="18"/>
+      <c r="F166" s="18"/>
+      <c r="G166" s="18"/>
+      <c r="H166" s="18"/>
+      <c r="I166" s="18"/>
+      <c r="J166" s="18"/>
+      <c r="K166" s="18"/>
+      <c r="L166" s="18"/>
+      <c r="M166" s="18"/>
+      <c r="N166" s="18"/>
+      <c r="O166" s="18"/>
+      <c r="P166" s="18"/>
+      <c r="Q166" s="18"/>
+      <c r="R166" s="18"/>
+      <c r="S166" s="19"/>
+    </row>
+    <row r="167" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A167" s="20"/>
+      <c r="B167" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C167" s="9"/>
+      <c r="D167" s="9"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
+      <c r="G167" s="9"/>
+      <c r="H167" s="9"/>
+      <c r="I167" s="9"/>
+      <c r="J167" s="9"/>
+      <c r="K167" s="9"/>
+      <c r="L167" s="9"/>
+      <c r="M167" s="9"/>
+      <c r="N167" s="9"/>
+      <c r="O167" s="9"/>
+      <c r="P167" s="9"/>
+      <c r="Q167" s="9"/>
+      <c r="R167" s="9"/>
+      <c r="S167" s="21"/>
+    </row>
+    <row r="168" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A168" s="20"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="9"/>
+      <c r="D168" s="9"/>
+      <c r="E168" s="9"/>
+      <c r="F168" s="9"/>
+      <c r="G168" s="9"/>
+      <c r="H168" s="9"/>
+      <c r="I168" s="9"/>
+      <c r="J168" s="9"/>
+      <c r="K168" s="9"/>
+      <c r="L168" s="9"/>
+      <c r="M168" s="9"/>
+      <c r="N168" s="9"/>
+      <c r="O168" s="9"/>
+      <c r="P168" s="9"/>
+      <c r="Q168" s="9"/>
+      <c r="R168" s="9"/>
+      <c r="S168" s="21"/>
+    </row>
+    <row r="169" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A169" s="20"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="9"/>
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
+      <c r="G169" s="9"/>
+      <c r="H169" s="9"/>
+      <c r="I169" s="9"/>
+      <c r="J169" s="9"/>
+      <c r="K169" s="9"/>
+      <c r="L169" s="9"/>
+      <c r="M169" s="9"/>
+      <c r="N169" s="9"/>
+      <c r="O169" s="9"/>
+      <c r="P169" s="9"/>
+      <c r="Q169" s="9"/>
+      <c r="R169" s="9"/>
+      <c r="S169" s="21"/>
+    </row>
+    <row r="170" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A170" s="20"/>
+      <c r="B170" s="9"/>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
+      <c r="G170" s="9"/>
+      <c r="H170" s="9"/>
+      <c r="I170" s="9"/>
+      <c r="J170" s="9"/>
+      <c r="K170" s="9"/>
+      <c r="L170" s="9"/>
+      <c r="M170" s="9"/>
+      <c r="N170" s="9"/>
+      <c r="O170" s="9"/>
+      <c r="P170" s="9"/>
+      <c r="Q170" s="9"/>
+      <c r="R170" s="9"/>
+      <c r="S170" s="21"/>
+    </row>
+    <row r="171" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A171" s="20"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
+      <c r="G171" s="9"/>
+      <c r="H171" s="9"/>
+      <c r="I171" s="9"/>
+      <c r="J171" s="9"/>
+      <c r="K171" s="9"/>
+      <c r="L171" s="9"/>
+      <c r="M171" s="9"/>
+      <c r="N171" s="9"/>
+      <c r="O171" s="9"/>
+      <c r="P171" s="9"/>
+      <c r="Q171" s="9"/>
+      <c r="R171" s="9"/>
+      <c r="S171" s="21"/>
+    </row>
+    <row r="172" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A172" s="20"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
+      <c r="G172" s="9"/>
+      <c r="H172" s="9"/>
+      <c r="I172" s="9"/>
+      <c r="J172" s="9"/>
+      <c r="K172" s="9"/>
+      <c r="L172" s="9"/>
+      <c r="M172" s="9"/>
+      <c r="N172" s="9"/>
+      <c r="O172" s="9"/>
+      <c r="P172" s="9"/>
+      <c r="Q172" s="9"/>
+      <c r="R172" s="9"/>
+      <c r="S172" s="21"/>
+    </row>
+    <row r="173" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A173" s="20"/>
+      <c r="B173" s="9"/>
+      <c r="C173" s="9"/>
+      <c r="D173" s="9"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="9"/>
+      <c r="G173" s="9"/>
+      <c r="H173" s="9"/>
+      <c r="I173" s="9"/>
+      <c r="J173" s="9"/>
+      <c r="K173" s="9"/>
+      <c r="L173" s="9"/>
+      <c r="M173" s="9"/>
+      <c r="N173" s="9"/>
+      <c r="O173" s="9"/>
+      <c r="P173" s="9"/>
+      <c r="Q173" s="9"/>
+      <c r="R173" s="9"/>
+      <c r="S173" s="21"/>
+    </row>
+    <row r="174" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A174" s="20"/>
+      <c r="B174" s="9"/>
+      <c r="C174" s="9"/>
+      <c r="D174" s="9"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="9"/>
+      <c r="H174" s="9"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="9"/>
+      <c r="K174" s="9"/>
+      <c r="L174" s="9"/>
+      <c r="M174" s="9"/>
+      <c r="N174" s="9"/>
+      <c r="O174" s="9"/>
+      <c r="P174" s="9"/>
+      <c r="Q174" s="9"/>
+      <c r="R174" s="9"/>
+      <c r="S174" s="21"/>
+    </row>
+    <row r="175" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A175" s="20"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="9"/>
+      <c r="H175" s="9"/>
+      <c r="I175" s="9"/>
+      <c r="J175" s="9"/>
+      <c r="K175" s="9"/>
+      <c r="L175" s="9"/>
+      <c r="M175" s="9"/>
+      <c r="N175" s="9"/>
+      <c r="O175" s="9"/>
+      <c r="P175" s="9"/>
+      <c r="Q175" s="9"/>
+      <c r="R175" s="9"/>
+      <c r="S175" s="21"/>
+    </row>
+    <row r="176" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A176" s="20"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="9"/>
+      <c r="D176" s="9"/>
+      <c r="E176" s="9"/>
+      <c r="F176" s="9"/>
+      <c r="G176" s="9"/>
+      <c r="H176" s="9"/>
+      <c r="I176" s="9"/>
+      <c r="J176" s="9"/>
+      <c r="K176" s="9"/>
+      <c r="L176" s="9"/>
+      <c r="M176" s="9"/>
+      <c r="N176" s="9"/>
+      <c r="O176" s="9"/>
+      <c r="P176" s="9"/>
+      <c r="Q176" s="9"/>
+      <c r="R176" s="9"/>
+      <c r="S176" s="21"/>
+    </row>
+    <row r="177" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A177" s="20"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="9"/>
+      <c r="D177" s="9"/>
+      <c r="E177" s="9"/>
+      <c r="F177" s="9"/>
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+      <c r="I177" s="9"/>
+      <c r="J177" s="9"/>
+      <c r="K177" s="9"/>
+      <c r="L177" s="9"/>
+      <c r="M177" s="9"/>
+      <c r="N177" s="9"/>
+      <c r="O177" s="9"/>
+      <c r="P177" s="9"/>
+      <c r="Q177" s="9"/>
+      <c r="R177" s="9"/>
+      <c r="S177" s="21"/>
+    </row>
+    <row r="178" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A178" s="20"/>
+      <c r="B178" s="9"/>
+      <c r="C178" s="9"/>
+      <c r="D178" s="9"/>
+      <c r="E178" s="9"/>
+      <c r="F178" s="9"/>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="9"/>
+      <c r="K178" s="9"/>
+      <c r="L178" s="9"/>
+      <c r="M178" s="9"/>
+      <c r="N178" s="9"/>
+      <c r="O178" s="9"/>
+      <c r="P178" s="9"/>
+      <c r="Q178" s="9"/>
+      <c r="R178" s="9"/>
+      <c r="S178" s="21"/>
+    </row>
+    <row r="179" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A179" s="20"/>
+      <c r="B179" s="9"/>
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+      <c r="I179" s="9"/>
+      <c r="J179" s="9"/>
+      <c r="K179" s="9"/>
+      <c r="L179" s="9"/>
+      <c r="M179" s="9"/>
+      <c r="N179" s="9"/>
+      <c r="O179" s="9"/>
+      <c r="P179" s="9"/>
+      <c r="Q179" s="9"/>
+      <c r="R179" s="9"/>
+      <c r="S179" s="21"/>
+    </row>
+    <row r="180" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A180" s="20"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="9"/>
+      <c r="D180" s="9"/>
+      <c r="E180" s="9"/>
+      <c r="F180" s="9"/>
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+      <c r="I180" s="9"/>
+      <c r="J180" s="9"/>
+      <c r="K180" s="9"/>
+      <c r="L180" s="9"/>
+      <c r="M180" s="9"/>
+      <c r="N180" s="9"/>
+      <c r="O180" s="9"/>
+      <c r="P180" s="9"/>
+      <c r="Q180" s="9"/>
+      <c r="R180" s="9"/>
+      <c r="S180" s="21"/>
+    </row>
+    <row r="181" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A181" s="20"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="9"/>
+      <c r="E181" s="9"/>
+      <c r="F181" s="9"/>
+      <c r="G181" s="9"/>
+      <c r="H181" s="9"/>
+      <c r="I181" s="9"/>
+      <c r="J181" s="9"/>
+      <c r="K181" s="9"/>
+      <c r="L181" s="9"/>
+      <c r="M181" s="9"/>
+      <c r="N181" s="9"/>
+      <c r="O181" s="9"/>
+      <c r="P181" s="9"/>
+      <c r="Q181" s="9"/>
+      <c r="R181" s="9"/>
+      <c r="S181" s="21"/>
+    </row>
+    <row r="182" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A182" s="20"/>
+      <c r="B182" s="9"/>
+      <c r="C182" s="9"/>
+      <c r="D182" s="9"/>
+      <c r="E182" s="9"/>
+      <c r="F182" s="9"/>
+      <c r="G182" s="9"/>
+      <c r="H182" s="9"/>
+      <c r="I182" s="9"/>
+      <c r="J182" s="9"/>
+      <c r="K182" s="9"/>
+      <c r="L182" s="9"/>
+      <c r="M182" s="9"/>
+      <c r="N182" s="9"/>
+      <c r="O182" s="9"/>
+      <c r="P182" s="9"/>
+      <c r="Q182" s="9"/>
+      <c r="R182" s="9"/>
+      <c r="S182" s="21"/>
+    </row>
+    <row r="183" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A183" s="20"/>
+      <c r="B183" s="9"/>
+      <c r="C183" s="9"/>
+      <c r="D183" s="9"/>
+      <c r="E183" s="9"/>
+      <c r="F183" s="9"/>
+      <c r="G183" s="9"/>
+      <c r="H183" s="9"/>
+      <c r="I183" s="9"/>
+      <c r="J183" s="9"/>
+      <c r="K183" s="9"/>
+      <c r="L183" s="9"/>
+      <c r="M183" s="9"/>
+      <c r="N183" s="9"/>
+      <c r="O183" s="9"/>
+      <c r="P183" s="9"/>
+      <c r="Q183" s="9"/>
+      <c r="R183" s="9"/>
+      <c r="S183" s="21"/>
+    </row>
+    <row r="184" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A184" s="20"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="9"/>
+      <c r="E184" s="9"/>
+      <c r="F184" s="9"/>
+      <c r="G184" s="9"/>
+      <c r="H184" s="9"/>
+      <c r="I184" s="9"/>
+      <c r="J184" s="9"/>
+      <c r="K184" s="9"/>
+      <c r="L184" s="9"/>
+      <c r="M184" s="9"/>
+      <c r="N184" s="9"/>
+      <c r="O184" s="9"/>
+      <c r="P184" s="9"/>
+      <c r="Q184" s="9"/>
+      <c r="R184" s="9"/>
+      <c r="S184" s="21"/>
+    </row>
+    <row r="185" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A185" s="20"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="9"/>
+      <c r="D185" s="9"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="9"/>
+      <c r="G185" s="9"/>
+      <c r="H185" s="9"/>
+      <c r="I185" s="9"/>
+      <c r="J185" s="9"/>
+      <c r="K185" s="9"/>
+      <c r="L185" s="9"/>
+      <c r="M185" s="9"/>
+      <c r="N185" s="9"/>
+      <c r="O185" s="9"/>
+      <c r="P185" s="9"/>
+      <c r="Q185" s="9"/>
+      <c r="R185" s="9"/>
+      <c r="S185" s="21"/>
+    </row>
+    <row r="186" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A186" s="20"/>
+      <c r="B186" s="9"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="9"/>
+      <c r="E186" s="9"/>
+      <c r="F186" s="9"/>
+      <c r="G186" s="9"/>
+      <c r="H186" s="9"/>
+      <c r="I186" s="9"/>
+      <c r="J186" s="9"/>
+      <c r="K186" s="9"/>
+      <c r="L186" s="9"/>
+      <c r="M186" s="9"/>
+      <c r="N186" s="9"/>
+      <c r="O186" s="9"/>
+      <c r="P186" s="9"/>
+      <c r="Q186" s="9"/>
+      <c r="R186" s="9"/>
+      <c r="S186" s="21"/>
+    </row>
+    <row r="187" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A187" s="20"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="9"/>
+      <c r="E187" s="9"/>
+      <c r="F187" s="9"/>
+      <c r="G187" s="9"/>
+      <c r="H187" s="9"/>
+      <c r="I187" s="9"/>
+      <c r="J187" s="9"/>
+      <c r="K187" s="9"/>
+      <c r="L187" s="9"/>
+      <c r="M187" s="9"/>
+      <c r="N187" s="9"/>
+      <c r="O187" s="9"/>
+      <c r="P187" s="9"/>
+      <c r="Q187" s="9"/>
+      <c r="R187" s="9"/>
+      <c r="S187" s="21"/>
+    </row>
+    <row r="188" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A188" s="20"/>
+      <c r="B188" s="9"/>
+      <c r="C188" s="9"/>
+      <c r="D188" s="9"/>
+      <c r="E188" s="9"/>
+      <c r="F188" s="9"/>
+      <c r="G188" s="9"/>
+      <c r="H188" s="9"/>
+      <c r="I188" s="9"/>
+      <c r="J188" s="9"/>
+      <c r="K188" s="9"/>
+      <c r="L188" s="9"/>
+      <c r="M188" s="9"/>
+      <c r="N188" s="9"/>
+      <c r="O188" s="9"/>
+      <c r="P188" s="9"/>
+      <c r="Q188" s="9"/>
+      <c r="R188" s="9"/>
+      <c r="S188" s="21"/>
+    </row>
+    <row r="189" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A189" s="20"/>
+      <c r="B189" s="9"/>
+      <c r="C189" s="9"/>
+      <c r="D189" s="9"/>
+      <c r="E189" s="9"/>
+      <c r="F189" s="9"/>
+      <c r="G189" s="9"/>
+      <c r="H189" s="9"/>
+      <c r="I189" s="9"/>
+      <c r="J189" s="9"/>
+      <c r="K189" s="9"/>
+      <c r="L189" s="9"/>
+      <c r="M189" s="9"/>
+      <c r="N189" s="9"/>
+      <c r="O189" s="9"/>
+      <c r="P189" s="9"/>
+      <c r="Q189" s="9"/>
+      <c r="R189" s="9"/>
+      <c r="S189" s="21"/>
+    </row>
+    <row r="190" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A190" s="20"/>
+      <c r="B190" s="9"/>
+      <c r="C190" s="9"/>
+      <c r="D190" s="9"/>
+      <c r="E190" s="9"/>
+      <c r="F190" s="9"/>
+      <c r="G190" s="9"/>
+      <c r="H190" s="9"/>
+      <c r="I190" s="9"/>
+      <c r="J190" s="9"/>
+      <c r="K190" s="9"/>
+      <c r="L190" s="9"/>
+      <c r="M190" s="9"/>
+      <c r="N190" s="9"/>
+      <c r="O190" s="9"/>
+      <c r="P190" s="9"/>
+      <c r="Q190" s="9"/>
+      <c r="R190" s="9"/>
+      <c r="S190" s="21"/>
+    </row>
+    <row r="191" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A191" s="20"/>
+      <c r="B191" s="9"/>
+      <c r="C191" s="9"/>
+      <c r="D191" s="9"/>
+      <c r="E191" s="9"/>
+      <c r="F191" s="9"/>
+      <c r="G191" s="9"/>
+      <c r="H191" s="9"/>
+      <c r="I191" s="9"/>
+      <c r="J191" s="9"/>
+      <c r="K191" s="9"/>
+      <c r="L191" s="9"/>
+      <c r="M191" s="9"/>
+      <c r="N191" s="9"/>
+      <c r="O191" s="9"/>
+      <c r="P191" s="9"/>
+      <c r="Q191" s="9"/>
+      <c r="R191" s="9"/>
+      <c r="S191" s="21"/>
+    </row>
+    <row r="192" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A192" s="20"/>
+      <c r="B192" s="9"/>
+      <c r="C192" s="9"/>
+      <c r="D192" s="9"/>
+      <c r="E192" s="9"/>
+      <c r="F192" s="9"/>
+      <c r="G192" s="9"/>
+      <c r="H192" s="9"/>
+      <c r="I192" s="9"/>
+      <c r="J192" s="9"/>
+      <c r="K192" s="9"/>
+      <c r="L192" s="9"/>
+      <c r="M192" s="9"/>
+      <c r="N192" s="9"/>
+      <c r="O192" s="9"/>
+      <c r="P192" s="9"/>
+      <c r="Q192" s="9"/>
+      <c r="R192" s="9"/>
+      <c r="S192" s="21"/>
+    </row>
+    <row r="193" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A193" s="20"/>
+      <c r="B193" s="9"/>
+      <c r="C193" s="9"/>
+      <c r="D193" s="9"/>
+      <c r="E193" s="9"/>
+      <c r="F193" s="9"/>
+      <c r="G193" s="9"/>
+      <c r="H193" s="9"/>
+      <c r="I193" s="9"/>
+      <c r="J193" s="9"/>
+      <c r="K193" s="9"/>
+      <c r="L193" s="9"/>
+      <c r="M193" s="9"/>
+      <c r="N193" s="9"/>
+      <c r="O193" s="9"/>
+      <c r="P193" s="9"/>
+      <c r="Q193" s="9"/>
+      <c r="R193" s="9"/>
+      <c r="S193" s="21"/>
+    </row>
+    <row r="194" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A194" s="20"/>
+      <c r="B194" s="9"/>
+      <c r="C194" s="9"/>
+      <c r="D194" s="9"/>
+      <c r="E194" s="9"/>
+      <c r="F194" s="9"/>
+      <c r="G194" s="9"/>
+      <c r="H194" s="9"/>
+      <c r="I194" s="9"/>
+      <c r="J194" s="9"/>
+      <c r="K194" s="9"/>
+      <c r="L194" s="9"/>
+      <c r="M194" s="9"/>
+      <c r="N194" s="9"/>
+      <c r="O194" s="9"/>
+      <c r="P194" s="9"/>
+      <c r="Q194" s="9"/>
+      <c r="R194" s="9"/>
+      <c r="S194" s="21"/>
+    </row>
+    <row r="195" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A195" s="20"/>
+      <c r="B195" s="9"/>
+      <c r="C195" s="9"/>
+      <c r="D195" s="9"/>
+      <c r="E195" s="9"/>
+      <c r="F195" s="9"/>
+      <c r="G195" s="9"/>
+      <c r="H195" s="9"/>
+      <c r="I195" s="9"/>
+      <c r="J195" s="9"/>
+      <c r="K195" s="9"/>
+      <c r="L195" s="9"/>
+      <c r="M195" s="9"/>
+      <c r="N195" s="9"/>
+      <c r="O195" s="9"/>
+      <c r="P195" s="9"/>
+      <c r="Q195" s="9"/>
+      <c r="R195" s="9"/>
+      <c r="S195" s="21"/>
+    </row>
+    <row r="196" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A196" s="22"/>
+      <c r="B196" s="23"/>
+      <c r="C196" s="23"/>
+      <c r="D196" s="23"/>
+      <c r="E196" s="23"/>
+      <c r="F196" s="23"/>
+      <c r="G196" s="23"/>
+      <c r="H196" s="23"/>
+      <c r="I196" s="23"/>
+      <c r="J196" s="23"/>
+      <c r="K196" s="23"/>
+      <c r="L196" s="23"/>
+      <c r="M196" s="23"/>
+      <c r="N196" s="23"/>
+      <c r="O196" s="23"/>
+      <c r="P196" s="23"/>
+      <c r="Q196" s="23"/>
+      <c r="R196" s="23"/>
+      <c r="S196" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Convert database booleans to boolean literals in the JSON
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392439E2-B7FC-4132-BDFC-F26707EED9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0F09C5-C3CC-4FF8-BD99-A5F4FD30F5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="table data gateway class" sheetId="5" r:id="rId5"/>
     <sheet name="Show a list of all records" sheetId="6" r:id="rId6"/>
     <sheet name="prevent numeric converted toStr" sheetId="7" r:id="rId7"/>
+    <sheet name="boolean literals in the JSON" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="204">
   <si>
     <t>構成</t>
   </si>
@@ -745,6 +746,61 @@
   </si>
   <si>
     <t>https://www.php.net/manual/en/pdo.setattribute.php</t>
+  </si>
+  <si>
+    <t>Convert database booleans to boolean literals in the JSON</t>
+  </si>
+  <si>
+    <t>api hiện tại tra về giá trị của is_completed là 1 hoặc 0 mặc dù trong DB trường này định được định nghĩa là boolean</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    is_completed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BOOLEAN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> NOT NULL DEFAULT FALSE,</t>
+    </r>
+  </si>
+  <si>
+    <t>Thực thế thì đối với mysql boolean được quy về kiểu tinyint(1) với 0 tương ứng với false và 1 tương ứng với true</t>
+  </si>
+  <si>
+    <t>Tuy nhiên thì các giá trị boolean thì trong json có thể lưu ở dạng (true/false) nên sau khi query từ DB ra thì mình có thể encode các giá trị is_completed sang boolean(true/false)</t>
+  </si>
+  <si>
+    <t>        $data = [];</t>
+  </si>
+  <si>
+    <t>        while ($row = $stmt-&gt;fetch(PDO::FETCH_ASSOC)) {</t>
+  </si>
+  <si>
+    <t>            $row['is_completed'] = (bool) $row['is_completed'];</t>
+  </si>
+  <si>
+    <t>            $data[] = $row;</t>
+  </si>
+  <si>
+    <t>        return $data;</t>
+  </si>
+  <si>
+    <t>encode các giá trị is_completed sang boolean(true/false)</t>
   </si>
 </sst>
 </file>
@@ -2805,6 +2861,511 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A473587A-104D-428D-C08F-3CEEB524E2A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="971550" y="1504950"/>
+          <a:ext cx="1266825" cy="981075"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>133130</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D4080AC-E364-450B-6D50-F3E1BA88388C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="2724150"/>
+          <a:ext cx="11125200" cy="4076480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>370393</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>47121</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F232FB4-3AD9-6FDD-489D-FB4B2697DE70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="857250" y="7067550"/>
+          <a:ext cx="8657143" cy="4028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D85BB9E4-79CB-5D93-28DA-00FB40DA985C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3905250" y="2657475"/>
+          <a:ext cx="323850" cy="1085850"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8311FE3-731D-A225-9854-9705197ADDC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3895725" y="2667000"/>
+          <a:ext cx="914400" cy="6096000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>152085</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5462B31-D4C1-F086-47C2-C0447E6C8F94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="990600" y="11963400"/>
+          <a:ext cx="7772400" cy="5524185"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Arrow Connector 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEDE0BCF-86B2-3BE2-786C-8F5B270CECA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4410075" y="11772900"/>
+          <a:ext cx="104775" cy="3667125"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFEC2AF3-06C4-0427-D0ED-C81135B6BA1B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5591175" y="11782425"/>
+          <a:ext cx="2162175" cy="16259175"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>398802</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>27938</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E3EE222-DB11-898A-8BC2-2D8F3C9321AF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="781050" y="30365700"/>
+          <a:ext cx="9980952" cy="5095238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Arrow Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B64DFFA-7F3B-CD04-122A-64962556C8CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3162300" y="28174950"/>
+          <a:ext cx="5248275" cy="5200650"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -13324,8 +13885,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E626A40E-2901-4376-94B0-2A64A7359002}">
   <dimension ref="A2:T196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="G203" sqref="G203"/>
+    <sheetView topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104:L128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16613,4 +17174,3101 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3446F05F-C5AC-4C6E-8FE9-52F1D7A4A68C}">
+  <dimension ref="A2:T188"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="5"/>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="5"/>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="5"/>
+    </row>
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="5"/>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="5"/>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="5"/>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="5"/>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="5"/>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="5"/>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="5"/>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="5"/>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
+      <c r="T23" s="5"/>
+    </row>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="5"/>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="5"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="5"/>
+    </row>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="5"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="5"/>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="5"/>
+    </row>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="5"/>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="5"/>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="5"/>
+    </row>
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="9"/>
+      <c r="M33" s="9"/>
+      <c r="N33" s="9"/>
+      <c r="O33" s="9"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="9"/>
+      <c r="R33" s="9"/>
+      <c r="S33" s="9"/>
+      <c r="T33" s="5"/>
+    </row>
+    <row r="34" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B34" s="4"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="9"/>
+      <c r="N34" s="9"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="9"/>
+      <c r="Q34" s="9"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="9"/>
+      <c r="T34" s="5"/>
+    </row>
+    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="5"/>
+    </row>
+    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="5"/>
+    </row>
+    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
+      <c r="L37" s="9"/>
+      <c r="M37" s="9"/>
+      <c r="N37" s="9"/>
+      <c r="O37" s="9"/>
+      <c r="P37" s="9"/>
+      <c r="Q37" s="9"/>
+      <c r="R37" s="9"/>
+      <c r="S37" s="9"/>
+      <c r="T37" s="5"/>
+    </row>
+    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B38" s="4"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="5"/>
+    </row>
+    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="9"/>
+      <c r="N39" s="9"/>
+      <c r="O39" s="9"/>
+      <c r="P39" s="9"/>
+      <c r="Q39" s="9"/>
+      <c r="R39" s="9"/>
+      <c r="S39" s="9"/>
+      <c r="T39" s="5"/>
+    </row>
+    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B40" s="4"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="5"/>
+    </row>
+    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B41" s="4"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="5"/>
+    </row>
+    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="9"/>
+      <c r="N42" s="9"/>
+      <c r="O42" s="9"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="9"/>
+      <c r="R42" s="9"/>
+      <c r="S42" s="9"/>
+      <c r="T42" s="5"/>
+    </row>
+    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B43" s="4"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="5"/>
+    </row>
+    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="5"/>
+    </row>
+    <row r="45" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
+      <c r="L45" s="9"/>
+      <c r="M45" s="9"/>
+      <c r="N45" s="9"/>
+      <c r="O45" s="9"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="9"/>
+      <c r="R45" s="9"/>
+      <c r="S45" s="9"/>
+      <c r="T45" s="5"/>
+    </row>
+    <row r="46" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B46" s="4"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="5"/>
+    </row>
+    <row r="47" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B47" s="4"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="5"/>
+    </row>
+    <row r="48" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="9"/>
+      <c r="Q49" s="9"/>
+      <c r="R49" s="9"/>
+      <c r="S49" s="9"/>
+      <c r="T49" s="5"/>
+    </row>
+    <row r="50" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="9"/>
+      <c r="Q50" s="9"/>
+      <c r="R50" s="9"/>
+      <c r="S50" s="9"/>
+      <c r="T50" s="5"/>
+    </row>
+    <row r="51" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B51" s="4"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="5"/>
+    </row>
+    <row r="52" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="9"/>
+      <c r="Q52" s="9"/>
+      <c r="R52" s="9"/>
+      <c r="S52" s="9"/>
+      <c r="T52" s="5"/>
+    </row>
+    <row r="53" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
+      <c r="T53" s="5"/>
+    </row>
+    <row r="54" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="9"/>
+      <c r="S54" s="9"/>
+      <c r="T54" s="5"/>
+    </row>
+    <row r="55" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="9"/>
+      <c r="S55" s="9"/>
+      <c r="T55" s="5"/>
+    </row>
+    <row r="56" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="9"/>
+      <c r="Q56" s="9"/>
+      <c r="R56" s="9"/>
+      <c r="S56" s="9"/>
+      <c r="T56" s="5"/>
+    </row>
+    <row r="57" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B57" s="4"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="9"/>
+      <c r="R57" s="9"/>
+      <c r="S57" s="9"/>
+      <c r="T57" s="5"/>
+    </row>
+    <row r="58" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B58" s="4"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
+      <c r="Q58" s="9"/>
+      <c r="R58" s="9"/>
+      <c r="S58" s="9"/>
+      <c r="T58" s="5"/>
+    </row>
+    <row r="59" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="8"/>
+    </row>
+    <row r="62" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+      <c r="M62" s="2"/>
+      <c r="N62" s="2"/>
+      <c r="O62" s="2"/>
+      <c r="P62" s="2"/>
+      <c r="Q62" s="2"/>
+      <c r="R62" s="3"/>
+    </row>
+    <row r="63" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
+      <c r="L63" s="9"/>
+      <c r="M63" s="9"/>
+      <c r="N63" s="9"/>
+      <c r="O63" s="9"/>
+      <c r="P63" s="9"/>
+      <c r="Q63" s="9"/>
+      <c r="R63" s="5"/>
+    </row>
+    <row r="64" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="5"/>
+    </row>
+    <row r="65" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="5"/>
+    </row>
+    <row r="66" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B66" s="4"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
+      <c r="L66" s="9"/>
+      <c r="M66" s="9"/>
+      <c r="N66" s="9"/>
+      <c r="O66" s="9"/>
+      <c r="P66" s="9"/>
+      <c r="Q66" s="9"/>
+      <c r="R66" s="5"/>
+    </row>
+    <row r="67" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B67" s="4"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
+      <c r="L67" s="9"/>
+      <c r="M67" s="9"/>
+      <c r="N67" s="9"/>
+      <c r="O67" s="9"/>
+      <c r="P67" s="9"/>
+      <c r="Q67" s="9"/>
+      <c r="R67" s="5"/>
+    </row>
+    <row r="68" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="5"/>
+    </row>
+    <row r="69" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="9"/>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
+      <c r="L69" s="9"/>
+      <c r="M69" s="9"/>
+      <c r="N69" s="9"/>
+      <c r="O69" s="9"/>
+      <c r="P69" s="9"/>
+      <c r="Q69" s="9"/>
+      <c r="R69" s="5"/>
+    </row>
+    <row r="70" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+      <c r="O70" s="9"/>
+      <c r="P70" s="9"/>
+      <c r="Q70" s="9"/>
+      <c r="R70" s="5"/>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
+      <c r="O71" s="9"/>
+      <c r="P71" s="9"/>
+      <c r="Q71" s="9"/>
+      <c r="R71" s="5"/>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B72" s="4"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
+      <c r="O72" s="9"/>
+      <c r="P72" s="9"/>
+      <c r="Q72" s="9"/>
+      <c r="R72" s="5"/>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B73" s="4"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="5"/>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
+      <c r="O74" s="9"/>
+      <c r="P74" s="9"/>
+      <c r="Q74" s="9"/>
+      <c r="R74" s="5"/>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B75" s="4"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
+      <c r="O75" s="9"/>
+      <c r="P75" s="9"/>
+      <c r="Q75" s="9"/>
+      <c r="R75" s="5"/>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B76" s="4"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
+      <c r="O76" s="9"/>
+      <c r="P76" s="9"/>
+      <c r="Q76" s="9"/>
+      <c r="R76" s="5"/>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
+      <c r="O77" s="9"/>
+      <c r="P77" s="9"/>
+      <c r="Q77" s="9"/>
+      <c r="R77" s="5"/>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
+      <c r="O78" s="9"/>
+      <c r="P78" s="9"/>
+      <c r="Q78" s="9"/>
+      <c r="R78" s="5"/>
+    </row>
+    <row r="79" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
+      <c r="O79" s="9"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="9"/>
+      <c r="R79" s="5"/>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B80" s="4"/>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
+      <c r="O80" s="9"/>
+      <c r="P80" s="9"/>
+      <c r="Q80" s="9"/>
+      <c r="R80" s="5"/>
+    </row>
+    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B81" s="4"/>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="9"/>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
+      <c r="L81" s="9"/>
+      <c r="M81" s="9"/>
+      <c r="N81" s="9"/>
+      <c r="O81" s="9"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="9"/>
+      <c r="R81" s="5"/>
+    </row>
+    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="9"/>
+      <c r="N82" s="9"/>
+      <c r="O82" s="9"/>
+      <c r="P82" s="9"/>
+      <c r="Q82" s="9"/>
+      <c r="R82" s="5"/>
+    </row>
+    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="9"/>
+      <c r="J83" s="9"/>
+      <c r="K83" s="9"/>
+      <c r="L83" s="9"/>
+      <c r="M83" s="9"/>
+      <c r="N83" s="9"/>
+      <c r="O83" s="9"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="9"/>
+      <c r="R83" s="5"/>
+    </row>
+    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B84" s="4"/>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
+      <c r="O84" s="9"/>
+      <c r="P84" s="9"/>
+      <c r="Q84" s="9"/>
+      <c r="R84" s="5"/>
+    </row>
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
+      <c r="O85" s="9"/>
+      <c r="P85" s="9"/>
+      <c r="Q85" s="9"/>
+      <c r="R85" s="5"/>
+    </row>
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="9"/>
+      <c r="O86" s="9"/>
+      <c r="P86" s="9"/>
+      <c r="Q86" s="9"/>
+      <c r="R86" s="5"/>
+    </row>
+    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B87" s="4"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
+      <c r="O87" s="9"/>
+      <c r="P87" s="9"/>
+      <c r="Q87" s="9"/>
+      <c r="R87" s="5"/>
+    </row>
+    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
+      <c r="O88" s="9"/>
+      <c r="P88" s="9"/>
+      <c r="Q88" s="9"/>
+      <c r="R88" s="5"/>
+    </row>
+    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B89" s="4"/>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
+      <c r="O89" s="9"/>
+      <c r="P89" s="9"/>
+      <c r="Q89" s="9"/>
+      <c r="R89" s="5"/>
+    </row>
+    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B90" s="4"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="9"/>
+      <c r="P90" s="9"/>
+      <c r="Q90" s="9"/>
+      <c r="R90" s="5"/>
+    </row>
+    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="9"/>
+      <c r="P91" s="9"/>
+      <c r="Q91" s="9"/>
+      <c r="R91" s="5"/>
+    </row>
+    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B92" s="4"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="9"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="9"/>
+      <c r="P92" s="9"/>
+      <c r="Q92" s="9"/>
+      <c r="R92" s="5"/>
+    </row>
+    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B93" s="4"/>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="9"/>
+      <c r="O93" s="9"/>
+      <c r="P93" s="9"/>
+      <c r="Q93" s="9"/>
+      <c r="R93" s="5"/>
+    </row>
+    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B94" s="6"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="7"/>
+      <c r="I94" s="7"/>
+      <c r="J94" s="7"/>
+      <c r="K94" s="7"/>
+      <c r="L94" s="7"/>
+      <c r="M94" s="7"/>
+      <c r="N94" s="7"/>
+      <c r="O94" s="7"/>
+      <c r="P94" s="7"/>
+      <c r="Q94" s="7"/>
+      <c r="R94" s="8"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A97" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B97" s="32"/>
+      <c r="C97" s="32"/>
+      <c r="D97" s="32"/>
+      <c r="E97" s="32"/>
+      <c r="F97" s="32"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="32"/>
+      <c r="I97" s="32"/>
+      <c r="J97" s="32"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A98" s="32"/>
+      <c r="B98" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="34"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="34"/>
+      <c r="I98" s="34"/>
+      <c r="J98" s="35"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A99" s="32"/>
+      <c r="B99" s="36"/>
+      <c r="C99" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D99" s="11"/>
+      <c r="E99" s="11"/>
+      <c r="F99" s="11"/>
+      <c r="G99" s="11"/>
+      <c r="H99" s="11"/>
+      <c r="I99" s="11"/>
+      <c r="J99" s="37"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A100" s="32"/>
+      <c r="B100" s="36"/>
+      <c r="C100" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="11"/>
+      <c r="E100" s="11"/>
+      <c r="F100" s="11"/>
+      <c r="G100" s="11"/>
+      <c r="H100" s="11"/>
+      <c r="I100" s="11"/>
+      <c r="J100" s="37"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A101" s="32"/>
+      <c r="B101" s="36"/>
+      <c r="C101" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" s="11"/>
+      <c r="E101" s="11"/>
+      <c r="F101" s="11"/>
+      <c r="G101" s="11"/>
+      <c r="H101" s="11"/>
+      <c r="I101" s="11"/>
+      <c r="J101" s="37"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A102" s="32"/>
+      <c r="B102" s="36"/>
+      <c r="C102" s="11"/>
+      <c r="D102" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E102" s="11"/>
+      <c r="F102" s="11"/>
+      <c r="G102" s="11"/>
+      <c r="H102" s="11"/>
+      <c r="I102" s="11"/>
+      <c r="J102" s="37"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A103" s="32"/>
+      <c r="B103" s="36"/>
+      <c r="C103" s="11"/>
+      <c r="D103" s="11"/>
+      <c r="E103" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F103" s="11"/>
+      <c r="G103" s="11"/>
+      <c r="H103" s="11"/>
+      <c r="I103" s="11"/>
+      <c r="J103" s="37"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A104" s="32"/>
+      <c r="B104" s="36"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="11"/>
+      <c r="E104" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F104" s="11"/>
+      <c r="G104" s="11"/>
+      <c r="H104" s="11"/>
+      <c r="I104" s="11"/>
+      <c r="J104" s="37"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A105" s="32"/>
+      <c r="B105" s="36"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E105" s="11"/>
+      <c r="F105" s="11"/>
+      <c r="G105" s="11"/>
+      <c r="H105" s="11"/>
+      <c r="I105" s="11"/>
+      <c r="J105" s="37"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A106" s="32"/>
+      <c r="B106" s="36"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" s="11"/>
+      <c r="F106" s="11"/>
+      <c r="G106" s="11"/>
+      <c r="H106" s="11"/>
+      <c r="I106" s="11"/>
+      <c r="J106" s="37"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A107" s="32"/>
+      <c r="B107" s="36"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" s="11"/>
+      <c r="F107" s="11"/>
+      <c r="G107" s="11"/>
+      <c r="H107" s="11"/>
+      <c r="I107" s="11"/>
+      <c r="J107" s="37"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A108" s="32"/>
+      <c r="B108" s="36"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="11"/>
+      <c r="E108" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" s="11"/>
+      <c r="G108" s="11"/>
+      <c r="H108" s="11"/>
+      <c r="I108" s="11"/>
+      <c r="J108" s="37"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A109" s="32"/>
+      <c r="B109" s="36"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="11"/>
+      <c r="E109" s="11"/>
+      <c r="F109" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="11"/>
+      <c r="H109" s="11"/>
+      <c r="I109" s="11"/>
+      <c r="J109" s="37"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A110" s="32"/>
+      <c r="B110" s="36"/>
+      <c r="C110" s="11"/>
+      <c r="D110" s="11"/>
+      <c r="E110" s="11"/>
+      <c r="F110" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G110" s="11"/>
+      <c r="H110" s="11"/>
+      <c r="I110" s="11"/>
+      <c r="J110" s="37"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A111" s="32"/>
+      <c r="B111" s="36"/>
+      <c r="C111" s="11"/>
+      <c r="D111" s="11"/>
+      <c r="E111" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F111" s="11"/>
+      <c r="G111" s="11"/>
+      <c r="H111" s="11"/>
+      <c r="I111" s="11"/>
+      <c r="J111" s="37"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A112" s="32"/>
+      <c r="B112" s="36"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+      <c r="E112" s="11"/>
+      <c r="F112" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G112" s="11"/>
+      <c r="H112" s="11"/>
+      <c r="I112" s="11"/>
+      <c r="J112" s="37"/>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" s="32"/>
+      <c r="B113" s="36"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+      <c r="E113" s="11"/>
+      <c r="F113" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G113" s="11"/>
+      <c r="H113" s="11"/>
+      <c r="I113" s="11"/>
+      <c r="J113" s="37"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" s="32"/>
+      <c r="B114" s="36"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="11"/>
+      <c r="E114" s="11"/>
+      <c r="F114" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G114" s="11"/>
+      <c r="H114" s="11"/>
+      <c r="I114" s="11"/>
+      <c r="J114" s="37"/>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" s="32"/>
+      <c r="B115" s="36"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="11"/>
+      <c r="E115" s="11"/>
+      <c r="F115" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G115" s="11"/>
+      <c r="H115" s="11"/>
+      <c r="I115" s="11"/>
+      <c r="J115" s="37"/>
+      <c r="K115" t="s">
+        <v>34</v>
+      </c>
+      <c r="L115" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" s="32"/>
+      <c r="B116" s="36"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="11"/>
+      <c r="E116" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F116" s="11"/>
+      <c r="G116" s="11"/>
+      <c r="H116" s="11"/>
+      <c r="I116" s="11"/>
+      <c r="J116" s="37"/>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="32"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="11"/>
+      <c r="E117" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F117" s="11"/>
+      <c r="G117" s="11"/>
+      <c r="H117" s="11"/>
+      <c r="I117" s="11"/>
+      <c r="J117" s="37"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" s="32"/>
+      <c r="B118" s="36"/>
+      <c r="C118" s="11"/>
+      <c r="D118" s="11"/>
+      <c r="E118" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F118" s="11"/>
+      <c r="G118" s="11"/>
+      <c r="H118" s="11"/>
+      <c r="I118" s="11"/>
+      <c r="J118" s="37"/>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" s="32"/>
+      <c r="B119" s="36"/>
+      <c r="C119" s="11"/>
+      <c r="D119" s="11"/>
+      <c r="E119" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F119" s="11"/>
+      <c r="G119" s="11"/>
+      <c r="H119" s="11"/>
+      <c r="I119" s="11"/>
+      <c r="J119" s="37"/>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" s="32"/>
+      <c r="B120" s="36"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
+      <c r="E120" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F120" s="11"/>
+      <c r="G120" s="11"/>
+      <c r="H120" s="11"/>
+      <c r="I120" s="11"/>
+      <c r="J120" s="37"/>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" s="32"/>
+      <c r="B121" s="38"/>
+      <c r="C121" s="39"/>
+      <c r="D121" s="39"/>
+      <c r="E121" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F121" s="39"/>
+      <c r="G121" s="39"/>
+      <c r="H121" s="39"/>
+      <c r="I121" s="39"/>
+      <c r="J121" s="40"/>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B125" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125" s="2"/>
+      <c r="D125" s="2"/>
+      <c r="E125" s="2"/>
+      <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
+      <c r="H125" s="3"/>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B126" s="4"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="9"/>
+      <c r="H126" s="5"/>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+      <c r="H127" s="5"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="5"/>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+      <c r="H129" s="5"/>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="4"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9"/>
+      <c r="H130" s="5"/>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="5"/>
+    </row>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="5"/>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="5"/>
+    </row>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="5"/>
+    </row>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="4"/>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="5"/>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="5"/>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="H137" s="5"/>
+    </row>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="9"/>
+      <c r="H138" s="5"/>
+    </row>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+      <c r="H139" s="5"/>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="5"/>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="4"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="5"/>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C142" s="9"/>
+      <c r="D142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
+      <c r="G142" s="9"/>
+      <c r="H142" s="5"/>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="4"/>
+      <c r="C143" s="9"/>
+      <c r="D143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
+      <c r="G143" s="9"/>
+      <c r="H143" s="5"/>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="9"/>
+      <c r="H144" s="5"/>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B145" s="15"/>
+      <c r="C145" s="9"/>
+      <c r="D145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
+      <c r="G145" s="9"/>
+      <c r="H145" s="5"/>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B146" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="C146" s="9"/>
+      <c r="D146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
+      <c r="G146" s="9"/>
+      <c r="H146" s="5"/>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B147" s="15"/>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="5"/>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B148" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="5"/>
+      <c r="I148" t="s">
+        <v>34</v>
+      </c>
+      <c r="J148" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B149" s="15"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="5"/>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B150" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="5"/>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B151" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+      <c r="H151" s="5"/>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B152" s="15"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+      <c r="H152" s="5"/>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B153" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="H153" s="5"/>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B154" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+      <c r="H154" s="5"/>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B155" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C155" s="7"/>
+      <c r="D155" s="7"/>
+      <c r="E155" s="7"/>
+      <c r="F155" s="7"/>
+      <c r="G155" s="7"/>
+      <c r="H155" s="8"/>
+    </row>
+    <row r="157" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A158" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B158" s="18"/>
+      <c r="C158" s="18"/>
+      <c r="D158" s="18"/>
+      <c r="E158" s="18"/>
+      <c r="F158" s="18"/>
+      <c r="G158" s="18"/>
+      <c r="H158" s="18"/>
+      <c r="I158" s="18"/>
+      <c r="J158" s="18"/>
+      <c r="K158" s="18"/>
+      <c r="L158" s="18"/>
+      <c r="M158" s="18"/>
+      <c r="N158" s="18"/>
+      <c r="O158" s="18"/>
+      <c r="P158" s="18"/>
+      <c r="Q158" s="18"/>
+      <c r="R158" s="19"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A159" s="20"/>
+      <c r="B159" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="9"/>
+      <c r="H159" s="9"/>
+      <c r="I159" s="9"/>
+      <c r="J159" s="9"/>
+      <c r="K159" s="9"/>
+      <c r="L159" s="9"/>
+      <c r="M159" s="9"/>
+      <c r="N159" s="9"/>
+      <c r="O159" s="9"/>
+      <c r="P159" s="9"/>
+      <c r="Q159" s="9"/>
+      <c r="R159" s="21"/>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A160" s="20"/>
+      <c r="B160" s="9"/>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
+      <c r="G160" s="9"/>
+      <c r="H160" s="9"/>
+      <c r="I160" s="9"/>
+      <c r="J160" s="9"/>
+      <c r="K160" s="9"/>
+      <c r="L160" s="9"/>
+      <c r="M160" s="9"/>
+      <c r="N160" s="9"/>
+      <c r="O160" s="9"/>
+      <c r="P160" s="9"/>
+      <c r="Q160" s="9"/>
+      <c r="R160" s="21"/>
+    </row>
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A161" s="20"/>
+      <c r="B161" s="9"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="9"/>
+      <c r="H161" s="9"/>
+      <c r="I161" s="9"/>
+      <c r="J161" s="9"/>
+      <c r="K161" s="9"/>
+      <c r="L161" s="9"/>
+      <c r="M161" s="9"/>
+      <c r="N161" s="9"/>
+      <c r="O161" s="9"/>
+      <c r="P161" s="9"/>
+      <c r="Q161" s="9"/>
+      <c r="R161" s="21"/>
+    </row>
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A162" s="20"/>
+      <c r="B162" s="9"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="9"/>
+      <c r="J162" s="9"/>
+      <c r="K162" s="9"/>
+      <c r="L162" s="9"/>
+      <c r="M162" s="9"/>
+      <c r="N162" s="9"/>
+      <c r="O162" s="9"/>
+      <c r="P162" s="9"/>
+      <c r="Q162" s="9"/>
+      <c r="R162" s="21"/>
+    </row>
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A163" s="20"/>
+      <c r="B163" s="9"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
+      <c r="H163" s="9"/>
+      <c r="I163" s="9"/>
+      <c r="J163" s="9"/>
+      <c r="K163" s="9"/>
+      <c r="L163" s="9"/>
+      <c r="M163" s="9"/>
+      <c r="N163" s="9"/>
+      <c r="O163" s="9"/>
+      <c r="P163" s="9"/>
+      <c r="Q163" s="9"/>
+      <c r="R163" s="21"/>
+    </row>
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A164" s="20"/>
+      <c r="B164" s="9"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
+      <c r="G164" s="9"/>
+      <c r="H164" s="9"/>
+      <c r="I164" s="9"/>
+      <c r="J164" s="9"/>
+      <c r="K164" s="9"/>
+      <c r="L164" s="9"/>
+      <c r="M164" s="9"/>
+      <c r="N164" s="9"/>
+      <c r="O164" s="9"/>
+      <c r="P164" s="9"/>
+      <c r="Q164" s="9"/>
+      <c r="R164" s="21"/>
+    </row>
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A165" s="20"/>
+      <c r="B165" s="9"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
+      <c r="G165" s="9"/>
+      <c r="H165" s="9"/>
+      <c r="I165" s="9"/>
+      <c r="J165" s="9"/>
+      <c r="K165" s="9"/>
+      <c r="L165" s="9"/>
+      <c r="M165" s="9"/>
+      <c r="N165" s="9"/>
+      <c r="O165" s="9"/>
+      <c r="P165" s="9"/>
+      <c r="Q165" s="9"/>
+      <c r="R165" s="21"/>
+    </row>
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A166" s="20"/>
+      <c r="B166" s="9"/>
+      <c r="C166" s="9"/>
+      <c r="D166" s="9"/>
+      <c r="E166" s="9"/>
+      <c r="F166" s="9"/>
+      <c r="G166" s="9"/>
+      <c r="H166" s="9"/>
+      <c r="I166" s="9"/>
+      <c r="J166" s="9"/>
+      <c r="K166" s="9"/>
+      <c r="L166" s="9"/>
+      <c r="M166" s="9"/>
+      <c r="N166" s="9"/>
+      <c r="O166" s="9"/>
+      <c r="P166" s="9"/>
+      <c r="Q166" s="9"/>
+      <c r="R166" s="21"/>
+    </row>
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A167" s="20"/>
+      <c r="B167" s="9"/>
+      <c r="C167" s="9"/>
+      <c r="D167" s="9"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
+      <c r="G167" s="9"/>
+      <c r="H167" s="9"/>
+      <c r="I167" s="9"/>
+      <c r="J167" s="9"/>
+      <c r="K167" s="9"/>
+      <c r="L167" s="9"/>
+      <c r="M167" s="9"/>
+      <c r="N167" s="9"/>
+      <c r="O167" s="9"/>
+      <c r="P167" s="9"/>
+      <c r="Q167" s="9"/>
+      <c r="R167" s="21"/>
+    </row>
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A168" s="20"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="9"/>
+      <c r="D168" s="9"/>
+      <c r="E168" s="9"/>
+      <c r="F168" s="9"/>
+      <c r="G168" s="9"/>
+      <c r="H168" s="9"/>
+      <c r="I168" s="9"/>
+      <c r="J168" s="9"/>
+      <c r="K168" s="9"/>
+      <c r="L168" s="9"/>
+      <c r="M168" s="9"/>
+      <c r="N168" s="9"/>
+      <c r="O168" s="9"/>
+      <c r="P168" s="9"/>
+      <c r="Q168" s="9"/>
+      <c r="R168" s="21"/>
+    </row>
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A169" s="20"/>
+      <c r="B169" s="9"/>
+      <c r="C169" s="9"/>
+      <c r="D169" s="9"/>
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
+      <c r="G169" s="9"/>
+      <c r="H169" s="9"/>
+      <c r="I169" s="9"/>
+      <c r="J169" s="9"/>
+      <c r="K169" s="9"/>
+      <c r="L169" s="9"/>
+      <c r="M169" s="9"/>
+      <c r="N169" s="9"/>
+      <c r="O169" s="9"/>
+      <c r="P169" s="9"/>
+      <c r="Q169" s="9"/>
+      <c r="R169" s="21"/>
+    </row>
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A170" s="20"/>
+      <c r="B170" s="9"/>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
+      <c r="G170" s="9"/>
+      <c r="H170" s="9"/>
+      <c r="I170" s="9"/>
+      <c r="J170" s="9"/>
+      <c r="K170" s="9"/>
+      <c r="L170" s="9"/>
+      <c r="M170" s="9"/>
+      <c r="N170" s="9"/>
+      <c r="O170" s="9"/>
+      <c r="P170" s="9"/>
+      <c r="Q170" s="9"/>
+      <c r="R170" s="21"/>
+    </row>
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A171" s="20"/>
+      <c r="B171" s="9"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
+      <c r="G171" s="9"/>
+      <c r="H171" s="9"/>
+      <c r="I171" s="9"/>
+      <c r="J171" s="9"/>
+      <c r="K171" s="9"/>
+      <c r="L171" s="9"/>
+      <c r="M171" s="9"/>
+      <c r="N171" s="9"/>
+      <c r="O171" s="9"/>
+      <c r="P171" s="9"/>
+      <c r="Q171" s="9"/>
+      <c r="R171" s="21"/>
+    </row>
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A172" s="20"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
+      <c r="G172" s="9"/>
+      <c r="H172" s="9"/>
+      <c r="I172" s="9"/>
+      <c r="J172" s="9"/>
+      <c r="K172" s="9"/>
+      <c r="L172" s="9"/>
+      <c r="M172" s="9"/>
+      <c r="N172" s="9"/>
+      <c r="O172" s="9"/>
+      <c r="P172" s="9"/>
+      <c r="Q172" s="9"/>
+      <c r="R172" s="21"/>
+    </row>
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A173" s="20"/>
+      <c r="B173" s="9"/>
+      <c r="C173" s="9"/>
+      <c r="D173" s="9"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="9"/>
+      <c r="G173" s="9"/>
+      <c r="H173" s="9"/>
+      <c r="I173" s="9"/>
+      <c r="J173" s="9"/>
+      <c r="K173" s="9"/>
+      <c r="L173" s="9"/>
+      <c r="M173" s="9"/>
+      <c r="N173" s="9"/>
+      <c r="O173" s="9"/>
+      <c r="P173" s="9"/>
+      <c r="Q173" s="9"/>
+      <c r="R173" s="21"/>
+    </row>
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A174" s="20"/>
+      <c r="B174" s="9"/>
+      <c r="C174" s="9"/>
+      <c r="D174" s="9"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="9"/>
+      <c r="H174" s="9"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="9"/>
+      <c r="K174" s="9"/>
+      <c r="L174" s="9"/>
+      <c r="M174" s="9"/>
+      <c r="N174" s="9"/>
+      <c r="O174" s="9"/>
+      <c r="P174" s="9"/>
+      <c r="Q174" s="9"/>
+      <c r="R174" s="21"/>
+    </row>
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A175" s="20"/>
+      <c r="B175" s="9"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="9"/>
+      <c r="H175" s="9"/>
+      <c r="I175" s="9"/>
+      <c r="J175" s="9"/>
+      <c r="K175" s="9"/>
+      <c r="L175" s="9"/>
+      <c r="M175" s="9"/>
+      <c r="N175" s="9"/>
+      <c r="O175" s="9"/>
+      <c r="P175" s="9"/>
+      <c r="Q175" s="9"/>
+      <c r="R175" s="21"/>
+    </row>
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A176" s="20"/>
+      <c r="B176" s="9"/>
+      <c r="C176" s="9"/>
+      <c r="D176" s="9"/>
+      <c r="E176" s="9"/>
+      <c r="F176" s="9"/>
+      <c r="G176" s="9"/>
+      <c r="H176" s="9"/>
+      <c r="I176" s="9"/>
+      <c r="J176" s="9"/>
+      <c r="K176" s="9"/>
+      <c r="L176" s="9"/>
+      <c r="M176" s="9"/>
+      <c r="N176" s="9"/>
+      <c r="O176" s="9"/>
+      <c r="P176" s="9"/>
+      <c r="Q176" s="9"/>
+      <c r="R176" s="21"/>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A177" s="20"/>
+      <c r="B177" s="9"/>
+      <c r="C177" s="9"/>
+      <c r="D177" s="9"/>
+      <c r="E177" s="9"/>
+      <c r="F177" s="9"/>
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+      <c r="I177" s="9"/>
+      <c r="J177" s="9"/>
+      <c r="K177" s="9"/>
+      <c r="L177" s="9"/>
+      <c r="M177" s="9"/>
+      <c r="N177" s="9"/>
+      <c r="O177" s="9"/>
+      <c r="P177" s="9"/>
+      <c r="Q177" s="9"/>
+      <c r="R177" s="21"/>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A178" s="20"/>
+      <c r="B178" s="9"/>
+      <c r="C178" s="9"/>
+      <c r="D178" s="9"/>
+      <c r="E178" s="9"/>
+      <c r="F178" s="9"/>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="9"/>
+      <c r="K178" s="9"/>
+      <c r="L178" s="9"/>
+      <c r="M178" s="9"/>
+      <c r="N178" s="9"/>
+      <c r="O178" s="9"/>
+      <c r="P178" s="9"/>
+      <c r="Q178" s="9"/>
+      <c r="R178" s="21"/>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A179" s="20"/>
+      <c r="B179" s="9"/>
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+      <c r="I179" s="9"/>
+      <c r="J179" s="9"/>
+      <c r="K179" s="9"/>
+      <c r="L179" s="9"/>
+      <c r="M179" s="9"/>
+      <c r="N179" s="9"/>
+      <c r="O179" s="9"/>
+      <c r="P179" s="9"/>
+      <c r="Q179" s="9"/>
+      <c r="R179" s="21"/>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A180" s="20"/>
+      <c r="B180" s="9"/>
+      <c r="C180" s="9"/>
+      <c r="D180" s="9"/>
+      <c r="E180" s="9"/>
+      <c r="F180" s="9"/>
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+      <c r="I180" s="9"/>
+      <c r="J180" s="9"/>
+      <c r="K180" s="9"/>
+      <c r="L180" s="9"/>
+      <c r="M180" s="9"/>
+      <c r="N180" s="9"/>
+      <c r="O180" s="9"/>
+      <c r="P180" s="9"/>
+      <c r="Q180" s="9"/>
+      <c r="R180" s="21"/>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A181" s="20"/>
+      <c r="B181" s="9"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="9"/>
+      <c r="E181" s="9"/>
+      <c r="F181" s="9"/>
+      <c r="G181" s="9"/>
+      <c r="H181" s="9"/>
+      <c r="I181" s="9"/>
+      <c r="J181" s="9"/>
+      <c r="K181" s="9"/>
+      <c r="L181" s="9"/>
+      <c r="M181" s="9"/>
+      <c r="N181" s="9"/>
+      <c r="O181" s="9"/>
+      <c r="P181" s="9"/>
+      <c r="Q181" s="9"/>
+      <c r="R181" s="21"/>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A182" s="20"/>
+      <c r="B182" s="9"/>
+      <c r="C182" s="9"/>
+      <c r="D182" s="9"/>
+      <c r="E182" s="9"/>
+      <c r="F182" s="9"/>
+      <c r="G182" s="9"/>
+      <c r="H182" s="9"/>
+      <c r="I182" s="9"/>
+      <c r="J182" s="9"/>
+      <c r="K182" s="9"/>
+      <c r="L182" s="9"/>
+      <c r="M182" s="9"/>
+      <c r="N182" s="9"/>
+      <c r="O182" s="9"/>
+      <c r="P182" s="9"/>
+      <c r="Q182" s="9"/>
+      <c r="R182" s="21"/>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A183" s="20"/>
+      <c r="B183" s="9"/>
+      <c r="C183" s="9"/>
+      <c r="D183" s="9"/>
+      <c r="E183" s="9"/>
+      <c r="F183" s="9"/>
+      <c r="G183" s="9"/>
+      <c r="H183" s="9"/>
+      <c r="I183" s="9"/>
+      <c r="J183" s="9"/>
+      <c r="K183" s="9"/>
+      <c r="L183" s="9"/>
+      <c r="M183" s="9"/>
+      <c r="N183" s="9"/>
+      <c r="O183" s="9"/>
+      <c r="P183" s="9"/>
+      <c r="Q183" s="9"/>
+      <c r="R183" s="21"/>
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A184" s="20"/>
+      <c r="B184" s="9"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="9"/>
+      <c r="E184" s="9"/>
+      <c r="F184" s="9"/>
+      <c r="G184" s="9"/>
+      <c r="H184" s="9"/>
+      <c r="I184" s="9"/>
+      <c r="J184" s="9"/>
+      <c r="K184" s="9"/>
+      <c r="L184" s="9"/>
+      <c r="M184" s="9"/>
+      <c r="N184" s="9"/>
+      <c r="O184" s="9"/>
+      <c r="P184" s="9"/>
+      <c r="Q184" s="9"/>
+      <c r="R184" s="21"/>
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A185" s="20"/>
+      <c r="B185" s="9"/>
+      <c r="C185" s="9"/>
+      <c r="D185" s="9"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="9"/>
+      <c r="G185" s="9"/>
+      <c r="H185" s="9"/>
+      <c r="I185" s="9"/>
+      <c r="J185" s="9"/>
+      <c r="K185" s="9"/>
+      <c r="L185" s="9"/>
+      <c r="M185" s="9"/>
+      <c r="N185" s="9"/>
+      <c r="O185" s="9"/>
+      <c r="P185" s="9"/>
+      <c r="Q185" s="9"/>
+      <c r="R185" s="21"/>
+    </row>
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A186" s="20"/>
+      <c r="B186" s="9"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="9"/>
+      <c r="E186" s="9"/>
+      <c r="F186" s="9"/>
+      <c r="G186" s="9"/>
+      <c r="H186" s="9"/>
+      <c r="I186" s="9"/>
+      <c r="J186" s="9"/>
+      <c r="K186" s="9"/>
+      <c r="L186" s="9"/>
+      <c r="M186" s="9"/>
+      <c r="N186" s="9"/>
+      <c r="O186" s="9"/>
+      <c r="P186" s="9"/>
+      <c r="Q186" s="9"/>
+      <c r="R186" s="21"/>
+    </row>
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A187" s="20"/>
+      <c r="B187" s="9"/>
+      <c r="C187" s="9"/>
+      <c r="D187" s="9"/>
+      <c r="E187" s="9"/>
+      <c r="F187" s="9"/>
+      <c r="G187" s="9"/>
+      <c r="H187" s="9"/>
+      <c r="I187" s="9"/>
+      <c r="J187" s="9"/>
+      <c r="K187" s="9"/>
+      <c r="L187" s="9"/>
+      <c r="M187" s="9"/>
+      <c r="N187" s="9"/>
+      <c r="O187" s="9"/>
+      <c r="P187" s="9"/>
+      <c r="Q187" s="9"/>
+      <c r="R187" s="21"/>
+    </row>
+    <row r="188" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A188" s="22"/>
+      <c r="B188" s="23"/>
+      <c r="C188" s="23"/>
+      <c r="D188" s="23"/>
+      <c r="E188" s="23"/>
+      <c r="F188" s="23"/>
+      <c r="G188" s="23"/>
+      <c r="H188" s="23"/>
+      <c r="I188" s="23"/>
+      <c r="J188" s="23"/>
+      <c r="K188" s="23"/>
+      <c r="L188" s="23"/>
+      <c r="M188" s="23"/>
+      <c r="N188" s="23"/>
+      <c r="O188" s="23"/>
+      <c r="P188" s="23"/>
+      <c r="Q188" s="23"/>
+      <c r="R188" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Show an individual record
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0F09C5-C3CC-4FF8-BD99-A5F4FD30F5D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD75334-8DA4-4DEB-B180-F68F8E554A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Show a list of all records" sheetId="6" r:id="rId6"/>
     <sheet name="prevent numeric converted toStr" sheetId="7" r:id="rId7"/>
     <sheet name="boolean literals in the JSON" sheetId="8" r:id="rId8"/>
+    <sheet name="Show an individual record" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="221">
   <si>
     <t>構成</t>
   </si>
@@ -802,6 +803,57 @@
   <si>
     <t>encode các giá trị is_completed sang boolean(true/false)</t>
   </si>
+  <si>
+    <t>    public function get(string $id): array</t>
+  </si>
+  <si>
+    <t>                WHERE id = :id";</t>
+  </si>
+  <si>
+    <t>        $stmt = $this-&gt;conn-&gt;prepare($sql);</t>
+  </si>
+  <si>
+    <t>        $stmt-&gt;bindValue(":id", $id, PDO::PARAM_INT);</t>
+  </si>
+  <si>
+    <t>        $stmt-&gt;execute();</t>
+  </si>
+  <si>
+    <t>        $data = $stmt-&gt;fetch(PDO::FETCH_ASSOC);</t>
+  </si>
+  <si>
+    <t>        if ($data !== false) {</t>
+  </si>
+  <si>
+    <t>            $data['is_completed'] = (bool) $data['is_completed'];</t>
+  </si>
+  <si>
+    <t>            return [];</t>
+  </si>
+  <si>
+    <t>Sử dụng placeholder :id để tránh SQL injection</t>
+  </si>
+  <si>
+    <t>Dùng phương thức bindValue() để replace id placeholder</t>
+  </si>
+  <si>
+    <t>Kết quả trả về dạng mảng nếu có kết quả, còn ko có kết quả thì trả về false</t>
+  </si>
+  <si>
+    <t>                    echo json_encode($this-&gt;gateway-&gt;get($id));</t>
+  </si>
+  <si>
+    <t>Có kết quả trả về</t>
+  </si>
+  <si>
+    <t>http://localhost/api/tasks/1</t>
+  </si>
+  <si>
+    <t>Không có kết quả trả về</t>
+  </si>
+  <si>
+    <t>http://localhost/api/tasks/111</t>
+  </si>
 </sst>
 </file>
 
@@ -1021,7 +1073,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1063,6 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3366,6 +3419,258 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9AF5936-2D62-B801-5DB3-1F44D62A8BEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1952625" y="12734925"/>
+          <a:ext cx="161925" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{739CE14C-A08F-97CD-EB9D-2C476A01FA01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1276350" y="14277975"/>
+          <a:ext cx="8286750" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4283782C-2256-A7A5-64BD-C91D3AC792DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1771650" y="11972925"/>
+          <a:ext cx="1647825" cy="10782300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>474989</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>123465</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{605DFC77-0E2F-B572-200C-48337CA88783}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752475" y="32489775"/>
+          <a:ext cx="10085714" cy="2876190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>484515</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>9112</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCA71CF5-1D64-CA58-FB69-1FBE90C18449}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="28136850"/>
+          <a:ext cx="10076190" cy="3304762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -11696,8 +12001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF5B913-A637-422C-8D40-BE71A2590EEF}">
   <dimension ref="A4:X157"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="H66" sqref="H66:J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17180,8 +17485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3446F05F-C5AC-4C6E-8FE9-52F1D7A4A68C}">
   <dimension ref="A2:T188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20271,4 +20576,2365 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAAD77A-9F44-48F8-9088-AEEE6B84E767}">
+  <dimension ref="A4:R187"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="A167" sqref="A167"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="35"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="32"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="37"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="37"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="37"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="37"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="37"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="37"/>
+      <c r="K21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="37"/>
+      <c r="K22" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="37"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="37"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="37"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="37"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="37"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="40"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="5"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="5"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="5"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="5"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="4"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="5"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="5"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="5"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="5"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="5"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="4"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="5"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="5"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="5"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="5"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="5"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="4"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="5"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="5"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="5"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="4"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="5"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="5"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="5"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="5"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="5"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B65" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="5"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B66" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="5"/>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B67" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="5"/>
+      <c r="I67" t="s">
+        <v>34</v>
+      </c>
+      <c r="J67" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B68" s="15"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="5"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B69" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="5"/>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B70" s="15"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B71" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="5"/>
+      <c r="I71" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B72" s="15"/>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="5"/>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B73" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="5"/>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B74" s="15"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="5"/>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B75" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="5"/>
+      <c r="I75" t="s">
+        <v>34</v>
+      </c>
+      <c r="J75" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B76" s="15"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="5"/>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B77" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="5"/>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B78" s="15"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="5"/>
+    </row>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B79" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="5"/>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="5"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="5"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="5"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="15"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="5"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="5"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="5"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="8"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
+      <c r="H90" s="2"/>
+      <c r="I90" s="3"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="4"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="4"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="4"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
+      <c r="G100" s="9"/>
+      <c r="H100" s="9"/>
+      <c r="I100" s="5"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C101" s="9"/>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="5"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C102" s="9"/>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
+      <c r="G102" s="9"/>
+      <c r="H102" s="9"/>
+      <c r="I102" s="5"/>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="9"/>
+      <c r="H103" s="9"/>
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="4"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="5"/>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="4"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="5"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+      <c r="I108" s="5"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="4"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="9"/>
+      <c r="H109" s="9"/>
+      <c r="I109" s="5"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="5"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
+      <c r="I111" s="5"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="4"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="5"/>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="9"/>
+      <c r="H113" s="9"/>
+      <c r="I113" s="5"/>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="9"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="5"/>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="5"/>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="4"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="5"/>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="5"/>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="4"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="5"/>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="5"/>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B120" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="5"/>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B121" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="9"/>
+      <c r="H121" s="9"/>
+      <c r="I121" s="5"/>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="4"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
+      <c r="G122" s="9"/>
+      <c r="H122" s="9"/>
+      <c r="I122" s="5"/>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B123" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C123" s="9"/>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="5"/>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B124" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="9"/>
+      <c r="H124" s="9"/>
+      <c r="I124" s="5"/>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B125" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C125" s="9"/>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
+      <c r="G125" s="9"/>
+      <c r="H125" s="9"/>
+      <c r="I125" s="5"/>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B126" s="4"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
+      <c r="G126" s="9"/>
+      <c r="H126" s="9"/>
+      <c r="I126" s="5"/>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C127" s="9"/>
+      <c r="D127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
+      <c r="G127" s="9"/>
+      <c r="H127" s="9"/>
+      <c r="I127" s="5"/>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C128" s="9"/>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
+      <c r="G128" s="9"/>
+      <c r="H128" s="9"/>
+      <c r="I128" s="5"/>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
+      <c r="G129" s="9"/>
+      <c r="H129" s="9"/>
+      <c r="I129" s="5"/>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B130" s="4"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
+      <c r="G130" s="9"/>
+      <c r="H130" s="9"/>
+      <c r="I130" s="5"/>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C131" s="9"/>
+      <c r="D131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
+      <c r="G131" s="9"/>
+      <c r="H131" s="9"/>
+      <c r="I131" s="5"/>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C132" s="9"/>
+      <c r="D132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
+      <c r="G132" s="9"/>
+      <c r="H132" s="9"/>
+      <c r="I132" s="5"/>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="5"/>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B134" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C134" s="9"/>
+      <c r="D134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="5"/>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C135" s="9"/>
+      <c r="D135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
+      <c r="G135" s="9"/>
+      <c r="H135" s="9"/>
+      <c r="I135" s="5"/>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B136" s="4"/>
+      <c r="C136" s="9"/>
+      <c r="D136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
+      <c r="G136" s="9"/>
+      <c r="H136" s="9"/>
+      <c r="I136" s="5"/>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C137" s="9"/>
+      <c r="D137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
+      <c r="G137" s="9"/>
+      <c r="H137" s="9"/>
+      <c r="I137" s="5"/>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="9"/>
+      <c r="H138" s="9"/>
+      <c r="I138" s="5"/>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+      <c r="H139" s="9"/>
+      <c r="I139" s="5"/>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="5"/>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="9"/>
+      <c r="H141" s="9"/>
+      <c r="I141" s="5"/>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B142" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C142" s="7"/>
+      <c r="D142" s="7"/>
+      <c r="E142" s="7"/>
+      <c r="F142" s="7"/>
+      <c r="G142" s="7"/>
+      <c r="H142" s="7"/>
+      <c r="I142" s="8"/>
+    </row>
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A145" s="41" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B146" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+      <c r="H146" s="2"/>
+      <c r="I146" s="2"/>
+      <c r="J146" s="2"/>
+      <c r="K146" s="2"/>
+      <c r="L146" s="2"/>
+      <c r="M146" s="2"/>
+      <c r="N146" s="2"/>
+      <c r="O146" s="2"/>
+      <c r="P146" s="2"/>
+      <c r="Q146" s="2"/>
+      <c r="R146" s="3"/>
+    </row>
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B147" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="C147" s="9"/>
+      <c r="D147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
+      <c r="G147" s="9"/>
+      <c r="H147" s="9"/>
+      <c r="I147" s="9"/>
+      <c r="J147" s="9"/>
+      <c r="K147" s="9"/>
+      <c r="L147" s="9"/>
+      <c r="M147" s="9"/>
+      <c r="N147" s="9"/>
+      <c r="O147" s="9"/>
+      <c r="P147" s="9"/>
+      <c r="Q147" s="9"/>
+      <c r="R147" s="5"/>
+    </row>
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B148" s="4"/>
+      <c r="C148" s="9"/>
+      <c r="D148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
+      <c r="G148" s="9"/>
+      <c r="H148" s="9"/>
+      <c r="I148" s="9"/>
+      <c r="J148" s="9"/>
+      <c r="K148" s="9"/>
+      <c r="L148" s="9"/>
+      <c r="M148" s="9"/>
+      <c r="N148" s="9"/>
+      <c r="O148" s="9"/>
+      <c r="P148" s="9"/>
+      <c r="Q148" s="9"/>
+      <c r="R148" s="5"/>
+    </row>
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B149" s="4"/>
+      <c r="C149" s="9"/>
+      <c r="D149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
+      <c r="G149" s="9"/>
+      <c r="H149" s="9"/>
+      <c r="I149" s="9"/>
+      <c r="J149" s="9"/>
+      <c r="K149" s="9"/>
+      <c r="L149" s="9"/>
+      <c r="M149" s="9"/>
+      <c r="N149" s="9"/>
+      <c r="O149" s="9"/>
+      <c r="P149" s="9"/>
+      <c r="Q149" s="9"/>
+      <c r="R149" s="5"/>
+    </row>
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B150" s="4"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="9"/>
+      <c r="H150" s="9"/>
+      <c r="I150" s="9"/>
+      <c r="J150" s="9"/>
+      <c r="K150" s="9"/>
+      <c r="L150" s="9"/>
+      <c r="M150" s="9"/>
+      <c r="N150" s="9"/>
+      <c r="O150" s="9"/>
+      <c r="P150" s="9"/>
+      <c r="Q150" s="9"/>
+      <c r="R150" s="5"/>
+    </row>
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B151" s="4"/>
+      <c r="C151" s="9"/>
+      <c r="D151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
+      <c r="G151" s="9"/>
+      <c r="H151" s="9"/>
+      <c r="I151" s="9"/>
+      <c r="J151" s="9"/>
+      <c r="K151" s="9"/>
+      <c r="L151" s="9"/>
+      <c r="M151" s="9"/>
+      <c r="N151" s="9"/>
+      <c r="O151" s="9"/>
+      <c r="P151" s="9"/>
+      <c r="Q151" s="9"/>
+      <c r="R151" s="5"/>
+    </row>
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B152" s="4"/>
+      <c r="C152" s="9"/>
+      <c r="D152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
+      <c r="G152" s="9"/>
+      <c r="H152" s="9"/>
+      <c r="I152" s="9"/>
+      <c r="J152" s="9"/>
+      <c r="K152" s="9"/>
+      <c r="L152" s="9"/>
+      <c r="M152" s="9"/>
+      <c r="N152" s="9"/>
+      <c r="O152" s="9"/>
+      <c r="P152" s="9"/>
+      <c r="Q152" s="9"/>
+      <c r="R152" s="5"/>
+    </row>
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B153" s="4"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="9"/>
+      <c r="H153" s="9"/>
+      <c r="I153" s="9"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9"/>
+      <c r="L153" s="9"/>
+      <c r="M153" s="9"/>
+      <c r="N153" s="9"/>
+      <c r="O153" s="9"/>
+      <c r="P153" s="9"/>
+      <c r="Q153" s="9"/>
+      <c r="R153" s="5"/>
+    </row>
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B154" s="4"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="9"/>
+      <c r="J154" s="9"/>
+      <c r="K154" s="9"/>
+      <c r="L154" s="9"/>
+      <c r="M154" s="9"/>
+      <c r="N154" s="9"/>
+      <c r="O154" s="9"/>
+      <c r="P154" s="9"/>
+      <c r="Q154" s="9"/>
+      <c r="R154" s="5"/>
+    </row>
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B155" s="4"/>
+      <c r="C155" s="9"/>
+      <c r="D155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
+      <c r="G155" s="9"/>
+      <c r="H155" s="9"/>
+      <c r="I155" s="9"/>
+      <c r="J155" s="9"/>
+      <c r="K155" s="9"/>
+      <c r="L155" s="9"/>
+      <c r="M155" s="9"/>
+      <c r="N155" s="9"/>
+      <c r="O155" s="9"/>
+      <c r="P155" s="9"/>
+      <c r="Q155" s="9"/>
+      <c r="R155" s="5"/>
+    </row>
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B156" s="4"/>
+      <c r="C156" s="9"/>
+      <c r="D156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
+      <c r="G156" s="9"/>
+      <c r="H156" s="9"/>
+      <c r="I156" s="9"/>
+      <c r="J156" s="9"/>
+      <c r="K156" s="9"/>
+      <c r="L156" s="9"/>
+      <c r="M156" s="9"/>
+      <c r="N156" s="9"/>
+      <c r="O156" s="9"/>
+      <c r="P156" s="9"/>
+      <c r="Q156" s="9"/>
+      <c r="R156" s="5"/>
+    </row>
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B157" s="4"/>
+      <c r="C157" s="9"/>
+      <c r="D157" s="9"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
+      <c r="G157" s="9"/>
+      <c r="H157" s="9"/>
+      <c r="I157" s="9"/>
+      <c r="J157" s="9"/>
+      <c r="K157" s="9"/>
+      <c r="L157" s="9"/>
+      <c r="M157" s="9"/>
+      <c r="N157" s="9"/>
+      <c r="O157" s="9"/>
+      <c r="P157" s="9"/>
+      <c r="Q157" s="9"/>
+      <c r="R157" s="5"/>
+    </row>
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B158" s="4"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="9"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9"/>
+      <c r="G158" s="9"/>
+      <c r="H158" s="9"/>
+      <c r="I158" s="9"/>
+      <c r="J158" s="9"/>
+      <c r="K158" s="9"/>
+      <c r="L158" s="9"/>
+      <c r="M158" s="9"/>
+      <c r="N158" s="9"/>
+      <c r="O158" s="9"/>
+      <c r="P158" s="9"/>
+      <c r="Q158" s="9"/>
+      <c r="R158" s="5"/>
+    </row>
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B159" s="4"/>
+      <c r="C159" s="9"/>
+      <c r="D159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
+      <c r="G159" s="9"/>
+      <c r="H159" s="9"/>
+      <c r="I159" s="9"/>
+      <c r="J159" s="9"/>
+      <c r="K159" s="9"/>
+      <c r="L159" s="9"/>
+      <c r="M159" s="9"/>
+      <c r="N159" s="9"/>
+      <c r="O159" s="9"/>
+      <c r="P159" s="9"/>
+      <c r="Q159" s="9"/>
+      <c r="R159" s="5"/>
+    </row>
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B160" s="4"/>
+      <c r="C160" s="9"/>
+      <c r="D160" s="9"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
+      <c r="G160" s="9"/>
+      <c r="H160" s="9"/>
+      <c r="I160" s="9"/>
+      <c r="J160" s="9"/>
+      <c r="K160" s="9"/>
+      <c r="L160" s="9"/>
+      <c r="M160" s="9"/>
+      <c r="N160" s="9"/>
+      <c r="O160" s="9"/>
+      <c r="P160" s="9"/>
+      <c r="Q160" s="9"/>
+      <c r="R160" s="5"/>
+    </row>
+    <row r="161" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B161" s="4"/>
+      <c r="C161" s="9"/>
+      <c r="D161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
+      <c r="G161" s="9"/>
+      <c r="H161" s="9"/>
+      <c r="I161" s="9"/>
+      <c r="J161" s="9"/>
+      <c r="K161" s="9"/>
+      <c r="L161" s="9"/>
+      <c r="M161" s="9"/>
+      <c r="N161" s="9"/>
+      <c r="O161" s="9"/>
+      <c r="P161" s="9"/>
+      <c r="Q161" s="9"/>
+      <c r="R161" s="5"/>
+    </row>
+    <row r="162" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B162" s="4"/>
+      <c r="C162" s="9"/>
+      <c r="D162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
+      <c r="G162" s="9"/>
+      <c r="H162" s="9"/>
+      <c r="I162" s="9"/>
+      <c r="J162" s="9"/>
+      <c r="K162" s="9"/>
+      <c r="L162" s="9"/>
+      <c r="M162" s="9"/>
+      <c r="N162" s="9"/>
+      <c r="O162" s="9"/>
+      <c r="P162" s="9"/>
+      <c r="Q162" s="9"/>
+      <c r="R162" s="5"/>
+    </row>
+    <row r="163" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B163" s="4"/>
+      <c r="C163" s="9"/>
+      <c r="D163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
+      <c r="G163" s="9"/>
+      <c r="H163" s="9"/>
+      <c r="I163" s="9"/>
+      <c r="J163" s="9"/>
+      <c r="K163" s="9"/>
+      <c r="L163" s="9"/>
+      <c r="M163" s="9"/>
+      <c r="N163" s="9"/>
+      <c r="O163" s="9"/>
+      <c r="P163" s="9"/>
+      <c r="Q163" s="9"/>
+      <c r="R163" s="5"/>
+    </row>
+    <row r="164" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B164" s="4"/>
+      <c r="C164" s="9"/>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
+      <c r="G164" s="9"/>
+      <c r="H164" s="9"/>
+      <c r="I164" s="9"/>
+      <c r="J164" s="9"/>
+      <c r="K164" s="9"/>
+      <c r="L164" s="9"/>
+      <c r="M164" s="9"/>
+      <c r="N164" s="9"/>
+      <c r="O164" s="9"/>
+      <c r="P164" s="9"/>
+      <c r="Q164" s="9"/>
+      <c r="R164" s="5"/>
+    </row>
+    <row r="165" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B165" s="4"/>
+      <c r="C165" s="9"/>
+      <c r="D165" s="9"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
+      <c r="G165" s="9"/>
+      <c r="H165" s="9"/>
+      <c r="I165" s="9"/>
+      <c r="J165" s="9"/>
+      <c r="K165" s="9"/>
+      <c r="L165" s="9"/>
+      <c r="M165" s="9"/>
+      <c r="N165" s="9"/>
+      <c r="O165" s="9"/>
+      <c r="P165" s="9"/>
+      <c r="Q165" s="9"/>
+      <c r="R165" s="5"/>
+    </row>
+    <row r="166" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B166" s="6"/>
+      <c r="C166" s="7"/>
+      <c r="D166" s="7"/>
+      <c r="E166" s="7"/>
+      <c r="F166" s="7"/>
+      <c r="G166" s="7"/>
+      <c r="H166" s="7"/>
+      <c r="I166" s="7"/>
+      <c r="J166" s="7"/>
+      <c r="K166" s="7"/>
+      <c r="L166" s="7"/>
+      <c r="M166" s="7"/>
+      <c r="N166" s="7"/>
+      <c r="O166" s="7"/>
+      <c r="P166" s="7"/>
+      <c r="Q166" s="7"/>
+      <c r="R166" s="8"/>
+    </row>
+    <row r="169" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B169" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="C169" s="2"/>
+      <c r="D169" s="2"/>
+      <c r="E169" s="2"/>
+      <c r="F169" s="2"/>
+      <c r="G169" s="2"/>
+      <c r="H169" s="2"/>
+      <c r="I169" s="2"/>
+      <c r="J169" s="2"/>
+      <c r="K169" s="2"/>
+      <c r="L169" s="2"/>
+      <c r="M169" s="2"/>
+      <c r="N169" s="2"/>
+      <c r="O169" s="2"/>
+      <c r="P169" s="2"/>
+      <c r="Q169" s="2"/>
+      <c r="R169" s="3"/>
+    </row>
+    <row r="170" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B170" s="27" t="s">
+        <v>220</v>
+      </c>
+      <c r="C170" s="9"/>
+      <c r="D170" s="9"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
+      <c r="G170" s="9"/>
+      <c r="H170" s="9"/>
+      <c r="I170" s="9"/>
+      <c r="J170" s="9"/>
+      <c r="K170" s="9"/>
+      <c r="L170" s="9"/>
+      <c r="M170" s="9"/>
+      <c r="N170" s="9"/>
+      <c r="O170" s="9"/>
+      <c r="P170" s="9"/>
+      <c r="Q170" s="9"/>
+      <c r="R170" s="5"/>
+    </row>
+    <row r="171" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B171" s="4"/>
+      <c r="C171" s="9"/>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
+      <c r="G171" s="9"/>
+      <c r="H171" s="9"/>
+      <c r="I171" s="9"/>
+      <c r="J171" s="9"/>
+      <c r="K171" s="9"/>
+      <c r="L171" s="9"/>
+      <c r="M171" s="9"/>
+      <c r="N171" s="9"/>
+      <c r="O171" s="9"/>
+      <c r="P171" s="9"/>
+      <c r="Q171" s="9"/>
+      <c r="R171" s="5"/>
+    </row>
+    <row r="172" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B172" s="4"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="9"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
+      <c r="G172" s="9"/>
+      <c r="H172" s="9"/>
+      <c r="I172" s="9"/>
+      <c r="J172" s="9"/>
+      <c r="K172" s="9"/>
+      <c r="L172" s="9"/>
+      <c r="M172" s="9"/>
+      <c r="N172" s="9"/>
+      <c r="O172" s="9"/>
+      <c r="P172" s="9"/>
+      <c r="Q172" s="9"/>
+      <c r="R172" s="5"/>
+    </row>
+    <row r="173" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B173" s="4"/>
+      <c r="C173" s="9"/>
+      <c r="D173" s="9"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="9"/>
+      <c r="G173" s="9"/>
+      <c r="H173" s="9"/>
+      <c r="I173" s="9"/>
+      <c r="J173" s="9"/>
+      <c r="K173" s="9"/>
+      <c r="L173" s="9"/>
+      <c r="M173" s="9"/>
+      <c r="N173" s="9"/>
+      <c r="O173" s="9"/>
+      <c r="P173" s="9"/>
+      <c r="Q173" s="9"/>
+      <c r="R173" s="5"/>
+    </row>
+    <row r="174" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B174" s="4"/>
+      <c r="C174" s="9"/>
+      <c r="D174" s="9"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="9"/>
+      <c r="H174" s="9"/>
+      <c r="I174" s="9"/>
+      <c r="J174" s="9"/>
+      <c r="K174" s="9"/>
+      <c r="L174" s="9"/>
+      <c r="M174" s="9"/>
+      <c r="N174" s="9"/>
+      <c r="O174" s="9"/>
+      <c r="P174" s="9"/>
+      <c r="Q174" s="9"/>
+      <c r="R174" s="5"/>
+    </row>
+    <row r="175" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B175" s="4"/>
+      <c r="C175" s="9"/>
+      <c r="D175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="9"/>
+      <c r="H175" s="9"/>
+      <c r="I175" s="9"/>
+      <c r="J175" s="9"/>
+      <c r="K175" s="9"/>
+      <c r="L175" s="9"/>
+      <c r="M175" s="9"/>
+      <c r="N175" s="9"/>
+      <c r="O175" s="9"/>
+      <c r="P175" s="9"/>
+      <c r="Q175" s="9"/>
+      <c r="R175" s="5"/>
+    </row>
+    <row r="176" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B176" s="4"/>
+      <c r="C176" s="9"/>
+      <c r="D176" s="9"/>
+      <c r="E176" s="9"/>
+      <c r="F176" s="9"/>
+      <c r="G176" s="9"/>
+      <c r="H176" s="9"/>
+      <c r="I176" s="9"/>
+      <c r="J176" s="9"/>
+      <c r="K176" s="9"/>
+      <c r="L176" s="9"/>
+      <c r="M176" s="9"/>
+      <c r="N176" s="9"/>
+      <c r="O176" s="9"/>
+      <c r="P176" s="9"/>
+      <c r="Q176" s="9"/>
+      <c r="R176" s="5"/>
+    </row>
+    <row r="177" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B177" s="4"/>
+      <c r="C177" s="9"/>
+      <c r="D177" s="9"/>
+      <c r="E177" s="9"/>
+      <c r="F177" s="9"/>
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+      <c r="I177" s="9"/>
+      <c r="J177" s="9"/>
+      <c r="K177" s="9"/>
+      <c r="L177" s="9"/>
+      <c r="M177" s="9"/>
+      <c r="N177" s="9"/>
+      <c r="O177" s="9"/>
+      <c r="P177" s="9"/>
+      <c r="Q177" s="9"/>
+      <c r="R177" s="5"/>
+    </row>
+    <row r="178" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B178" s="4"/>
+      <c r="C178" s="9"/>
+      <c r="D178" s="9"/>
+      <c r="E178" s="9"/>
+      <c r="F178" s="9"/>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+      <c r="I178" s="9"/>
+      <c r="J178" s="9"/>
+      <c r="K178" s="9"/>
+      <c r="L178" s="9"/>
+      <c r="M178" s="9"/>
+      <c r="N178" s="9"/>
+      <c r="O178" s="9"/>
+      <c r="P178" s="9"/>
+      <c r="Q178" s="9"/>
+      <c r="R178" s="5"/>
+    </row>
+    <row r="179" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B179" s="4"/>
+      <c r="C179" s="9"/>
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+      <c r="I179" s="9"/>
+      <c r="J179" s="9"/>
+      <c r="K179" s="9"/>
+      <c r="L179" s="9"/>
+      <c r="M179" s="9"/>
+      <c r="N179" s="9"/>
+      <c r="O179" s="9"/>
+      <c r="P179" s="9"/>
+      <c r="Q179" s="9"/>
+      <c r="R179" s="5"/>
+    </row>
+    <row r="180" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B180" s="4"/>
+      <c r="C180" s="9"/>
+      <c r="D180" s="9"/>
+      <c r="E180" s="9"/>
+      <c r="F180" s="9"/>
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+      <c r="I180" s="9"/>
+      <c r="J180" s="9"/>
+      <c r="K180" s="9"/>
+      <c r="L180" s="9"/>
+      <c r="M180" s="9"/>
+      <c r="N180" s="9"/>
+      <c r="O180" s="9"/>
+      <c r="P180" s="9"/>
+      <c r="Q180" s="9"/>
+      <c r="R180" s="5"/>
+    </row>
+    <row r="181" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B181" s="4"/>
+      <c r="C181" s="9"/>
+      <c r="D181" s="9"/>
+      <c r="E181" s="9"/>
+      <c r="F181" s="9"/>
+      <c r="G181" s="9"/>
+      <c r="H181" s="9"/>
+      <c r="I181" s="9"/>
+      <c r="J181" s="9"/>
+      <c r="K181" s="9"/>
+      <c r="L181" s="9"/>
+      <c r="M181" s="9"/>
+      <c r="N181" s="9"/>
+      <c r="O181" s="9"/>
+      <c r="P181" s="9"/>
+      <c r="Q181" s="9"/>
+      <c r="R181" s="5"/>
+    </row>
+    <row r="182" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B182" s="4"/>
+      <c r="C182" s="9"/>
+      <c r="D182" s="9"/>
+      <c r="E182" s="9"/>
+      <c r="F182" s="9"/>
+      <c r="G182" s="9"/>
+      <c r="H182" s="9"/>
+      <c r="I182" s="9"/>
+      <c r="J182" s="9"/>
+      <c r="K182" s="9"/>
+      <c r="L182" s="9"/>
+      <c r="M182" s="9"/>
+      <c r="N182" s="9"/>
+      <c r="O182" s="9"/>
+      <c r="P182" s="9"/>
+      <c r="Q182" s="9"/>
+      <c r="R182" s="5"/>
+    </row>
+    <row r="183" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B183" s="4"/>
+      <c r="C183" s="9"/>
+      <c r="D183" s="9"/>
+      <c r="E183" s="9"/>
+      <c r="F183" s="9"/>
+      <c r="G183" s="9"/>
+      <c r="H183" s="9"/>
+      <c r="I183" s="9"/>
+      <c r="J183" s="9"/>
+      <c r="K183" s="9"/>
+      <c r="L183" s="9"/>
+      <c r="M183" s="9"/>
+      <c r="N183" s="9"/>
+      <c r="O183" s="9"/>
+      <c r="P183" s="9"/>
+      <c r="Q183" s="9"/>
+      <c r="R183" s="5"/>
+    </row>
+    <row r="184" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B184" s="4"/>
+      <c r="C184" s="9"/>
+      <c r="D184" s="9"/>
+      <c r="E184" s="9"/>
+      <c r="F184" s="9"/>
+      <c r="G184" s="9"/>
+      <c r="H184" s="9"/>
+      <c r="I184" s="9"/>
+      <c r="J184" s="9"/>
+      <c r="K184" s="9"/>
+      <c r="L184" s="9"/>
+      <c r="M184" s="9"/>
+      <c r="N184" s="9"/>
+      <c r="O184" s="9"/>
+      <c r="P184" s="9"/>
+      <c r="Q184" s="9"/>
+      <c r="R184" s="5"/>
+    </row>
+    <row r="185" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B185" s="4"/>
+      <c r="C185" s="9"/>
+      <c r="D185" s="9"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="9"/>
+      <c r="G185" s="9"/>
+      <c r="H185" s="9"/>
+      <c r="I185" s="9"/>
+      <c r="J185" s="9"/>
+      <c r="K185" s="9"/>
+      <c r="L185" s="9"/>
+      <c r="M185" s="9"/>
+      <c r="N185" s="9"/>
+      <c r="O185" s="9"/>
+      <c r="P185" s="9"/>
+      <c r="Q185" s="9"/>
+      <c r="R185" s="5"/>
+    </row>
+    <row r="186" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B186" s="4"/>
+      <c r="C186" s="9"/>
+      <c r="D186" s="9"/>
+      <c r="E186" s="9"/>
+      <c r="F186" s="9"/>
+      <c r="G186" s="9"/>
+      <c r="H186" s="9"/>
+      <c r="I186" s="9"/>
+      <c r="J186" s="9"/>
+      <c r="K186" s="9"/>
+      <c r="L186" s="9"/>
+      <c r="M186" s="9"/>
+      <c r="N186" s="9"/>
+      <c r="O186" s="9"/>
+      <c r="P186" s="9"/>
+      <c r="Q186" s="9"/>
+      <c r="R186" s="5"/>
+    </row>
+    <row r="187" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B187" s="6"/>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="7"/>
+      <c r="F187" s="7"/>
+      <c r="G187" s="7"/>
+      <c r="H187" s="7"/>
+      <c r="I187" s="7"/>
+      <c r="J187" s="7"/>
+      <c r="K187" s="7"/>
+      <c r="L187" s="7"/>
+      <c r="M187" s="7"/>
+      <c r="N187" s="7"/>
+      <c r="O187" s="7"/>
+      <c r="P187" s="7"/>
+      <c r="Q187" s="7"/>
+      <c r="R187" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Respond with 404 if the resource with the specified ID is not found
</commit_message>
<xml_diff>
--- a/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
+++ b/me/4.create-a-restful-api/2.create-a-database-and-retrieve-data-from-it.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\rest-api-php\me\4.create-a-restful-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD75334-8DA4-4DEB-B180-F68F8E554A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BF3310-F7A1-436C-9CDF-7C096873D18D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Create a new database" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="prevent numeric converted toStr" sheetId="7" r:id="rId7"/>
     <sheet name="boolean literals in the JSON" sheetId="8" r:id="rId8"/>
     <sheet name="Show an individual record" sheetId="9" r:id="rId9"/>
+    <sheet name="specified ID is not found" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="236">
   <si>
     <t>構成</t>
   </si>
@@ -854,6 +855,51 @@
   <si>
     <t>http://localhost/api/tasks/111</t>
   </si>
+  <si>
+    <t>Respond with 404 if the resource with the specified ID is not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trường hợp giá trị id ko tồn tại thì cần trả về status code là 404 và message trong response body </t>
+  </si>
+  <si>
+    <t>            $task = $this-&gt;gateway-&gt;get($id);</t>
+  </si>
+  <si>
+    <t>            if ($task === []) {</t>
+  </si>
+  <si>
+    <t>                $this-&gt;respondNotFound($id);</t>
+  </si>
+  <si>
+    <t>                return;</t>
+  </si>
+  <si>
+    <t>                    echo json_encode($task);</t>
+  </si>
+  <si>
+    <t>    private function respondNotFound(string $id): void</t>
+  </si>
+  <si>
+    <t>        http_response_code(404);</t>
+  </si>
+  <si>
+    <t>        echo json_encode(["message" =&gt; "Task with ID $id not found"]);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ngoài lấy thông tin của 1 phần tử ra thì sử hay xóa phần tử cũng đều phải kiểm tra có tồn tại hya không nên </t>
+  </si>
+  <si>
+    <t>mình sẽ kiểm tra ở ngay trong else và trước khi vào switch</t>
+  </si>
+  <si>
+    <t>Thực ra ko cần trả về nội dung cũng được nhưng trả về message thì tốt hơn</t>
+  </si>
+  <si>
+    <t>Nếu 404 xảy ra thì ko cần thực hiện các xử lý tiếp theo trong hàm này nữa</t>
+  </si>
+  <si>
+    <t>http://localhost/api/tasks/99</t>
+  </si>
 </sst>
 </file>
 
@@ -1177,6 +1223,267 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B917D04-BD61-B672-9594-A74E7F26ED83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1133475" y="11610975"/>
+          <a:ext cx="1304925" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9691E57-A694-D1AC-7224-11185941B4E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2286000" y="12344400"/>
+          <a:ext cx="66675" cy="5629275"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>436892</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>132982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6BBCD0D-19A5-1C9E-0C98-000DD718165C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="733425" y="19859625"/>
+          <a:ext cx="10066667" cy="2942857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8D72587-67D8-B685-466F-2F15F3AC67AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2381250" y="18430875"/>
+          <a:ext cx="6762750" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B08D01EF-361F-376B-7C42-81FF8FEE5C41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1809750" y="18678525"/>
+          <a:ext cx="552450" cy="3695700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4220,6 +4527,1569 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293D3563-0BF4-4AA7-956A-11624F19BF10}">
+  <dimension ref="A2:R121"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="M101" sqref="M101"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="32"/>
+      <c r="B7" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="35"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="32"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="37"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="32"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="37"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="32"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="37"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="32"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="37"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="32"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="37"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="32"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="32"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="37"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="32"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="37"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="32"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="37"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="32"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="37"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="32"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="37"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="32"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="37"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="32"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="37"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="32"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="37"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="32"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="37"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="32"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="37"/>
+      <c r="K23" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="37"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="32"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="37"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="32"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="37"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="32"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="37"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="37"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="32"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="37"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="32"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="40"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="4"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="4"/>
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B51" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="5"/>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="5"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="5"/>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="5"/>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="5"/>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B58" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B59" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B60" s="4"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B61" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" s="9"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B62" s="15"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B63" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="5"/>
+      <c r="J63" t="s">
+        <v>34</v>
+      </c>
+      <c r="K63" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B64" s="15"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="5"/>
+      <c r="K64" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B65" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B66" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="5"/>
+      <c r="J66" t="s">
+        <v>34</v>
+      </c>
+      <c r="K66" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B67" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B68" s="4"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B69" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B71" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="9"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B72" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B73" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B74" s="4"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
+      <c r="G74" s="9"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" s="9"/>
+      <c r="D75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
+      <c r="G75" s="9"/>
+      <c r="H75" s="9"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="9"/>
+      <c r="D78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+      <c r="H78" s="9"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C79" s="9"/>
+      <c r="D79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C80" s="9"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
+      <c r="G80" s="9"/>
+      <c r="H80" s="9"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81" s="9"/>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
+      <c r="G81" s="9"/>
+      <c r="H81" s="9"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B82" s="4"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C84" s="9"/>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
+      <c r="G84" s="9"/>
+      <c r="H84" s="9"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B86" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
+      <c r="G86" s="9"/>
+      <c r="H86" s="9"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C87" s="9"/>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
+      <c r="G87" s="9"/>
+      <c r="H87" s="9"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="4"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
+      <c r="G88" s="9"/>
+      <c r="H88" s="9"/>
+      <c r="I88" s="5"/>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="5"/>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C90" s="9"/>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="5"/>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C91" s="9"/>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
+      <c r="G91" s="9"/>
+      <c r="H91" s="9"/>
+      <c r="I91" s="5"/>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
+      <c r="G92" s="9"/>
+      <c r="H92" s="9"/>
+      <c r="I92" s="5"/>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C93" s="9"/>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
+      <c r="G93" s="9"/>
+      <c r="H93" s="9"/>
+      <c r="I93" s="5"/>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B94" s="4"/>
+      <c r="C94" s="9"/>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
+      <c r="G94" s="9"/>
+      <c r="H94" s="9"/>
+      <c r="I94" s="5"/>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C95" s="9"/>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
+      <c r="G95" s="9"/>
+      <c r="H95" s="9"/>
+      <c r="I95" s="5"/>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="5"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B97" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="9"/>
+      <c r="I97" s="5"/>
+    </row>
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B98" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="C98" s="9"/>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
+      <c r="G98" s="9"/>
+      <c r="H98" s="9"/>
+      <c r="I98" s="5"/>
+      <c r="J98" t="s">
+        <v>34</v>
+      </c>
+      <c r="K98" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B99" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
+      <c r="G99" s="9"/>
+      <c r="H99" s="9"/>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B100" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C100" s="7"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="7"/>
+      <c r="I100" s="8"/>
+    </row>
+    <row r="102" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A103" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="18"/>
+      <c r="F103" s="18"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="18"/>
+      <c r="I103" s="18"/>
+      <c r="J103" s="18"/>
+      <c r="K103" s="18"/>
+      <c r="L103" s="18"/>
+      <c r="M103" s="18"/>
+      <c r="N103" s="18"/>
+      <c r="O103" s="18"/>
+      <c r="P103" s="18"/>
+      <c r="Q103" s="18"/>
+      <c r="R103" s="19"/>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A104" s="20"/>
+      <c r="B104" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C104" s="9"/>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
+      <c r="G104" s="9"/>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
+      <c r="L104" s="9"/>
+      <c r="M104" s="9"/>
+      <c r="N104" s="9"/>
+      <c r="O104" s="9"/>
+      <c r="P104" s="9"/>
+      <c r="Q104" s="9"/>
+      <c r="R104" s="21"/>
+    </row>
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A105" s="20"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
+      <c r="G105" s="9"/>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="9"/>
+      <c r="M105" s="9"/>
+      <c r="N105" s="9"/>
+      <c r="O105" s="9"/>
+      <c r="P105" s="9"/>
+      <c r="Q105" s="9"/>
+      <c r="R105" s="21"/>
+    </row>
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A106" s="20"/>
+      <c r="B106" s="9"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
+      <c r="G106" s="9"/>
+      <c r="H106" s="9"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
+      <c r="L106" s="9"/>
+      <c r="M106" s="9"/>
+      <c r="N106" s="9"/>
+      <c r="O106" s="9"/>
+      <c r="P106" s="9"/>
+      <c r="Q106" s="9"/>
+      <c r="R106" s="21"/>
+    </row>
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A107" s="20"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
+      <c r="G107" s="9"/>
+      <c r="H107" s="9"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
+      <c r="L107" s="9"/>
+      <c r="M107" s="9"/>
+      <c r="N107" s="9"/>
+      <c r="O107" s="9"/>
+      <c r="P107" s="9"/>
+      <c r="Q107" s="9"/>
+      <c r="R107" s="21"/>
+    </row>
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A108" s="20"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
+      <c r="G108" s="9"/>
+      <c r="H108" s="9"/>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
+      <c r="L108" s="9"/>
+      <c r="M108" s="9"/>
+      <c r="N108" s="9"/>
+      <c r="O108" s="9"/>
+      <c r="P108" s="9"/>
+      <c r="Q108" s="9"/>
+      <c r="R108" s="21"/>
+    </row>
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A109" s="20"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="9"/>
+      <c r="H109" s="9"/>
+      <c r="I109" s="9"/>
+      <c r="J109" s="9"/>
+      <c r="K109" s="9"/>
+      <c r="L109" s="9"/>
+      <c r="M109" s="9"/>
+      <c r="N109" s="9"/>
+      <c r="O109" s="9"/>
+      <c r="P109" s="9"/>
+      <c r="Q109" s="9"/>
+      <c r="R109" s="21"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A110" s="20"/>
+      <c r="B110" s="9"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
+      <c r="G110" s="9"/>
+      <c r="H110" s="9"/>
+      <c r="I110" s="9"/>
+      <c r="J110" s="9"/>
+      <c r="K110" s="9"/>
+      <c r="L110" s="9"/>
+      <c r="M110" s="9"/>
+      <c r="N110" s="9"/>
+      <c r="O110" s="9"/>
+      <c r="P110" s="9"/>
+      <c r="Q110" s="9"/>
+      <c r="R110" s="21"/>
+    </row>
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A111" s="20"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
+      <c r="G111" s="9"/>
+      <c r="H111" s="9"/>
+      <c r="I111" s="9"/>
+      <c r="J111" s="9"/>
+      <c r="K111" s="9"/>
+      <c r="L111" s="9"/>
+      <c r="M111" s="9"/>
+      <c r="N111" s="9"/>
+      <c r="O111" s="9"/>
+      <c r="P111" s="9"/>
+      <c r="Q111" s="9"/>
+      <c r="R111" s="21"/>
+    </row>
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A112" s="20"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="9"/>
+      <c r="J112" s="9"/>
+      <c r="K112" s="9"/>
+      <c r="L112" s="9"/>
+      <c r="M112" s="9"/>
+      <c r="N112" s="9"/>
+      <c r="O112" s="9"/>
+      <c r="P112" s="9"/>
+      <c r="Q112" s="9"/>
+      <c r="R112" s="21"/>
+    </row>
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A113" s="20"/>
+      <c r="B113" s="9"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
+      <c r="G113" s="9"/>
+      <c r="H113" s="9"/>
+      <c r="I113" s="9"/>
+      <c r="J113" s="9"/>
+      <c r="K113" s="9"/>
+      <c r="L113" s="9"/>
+      <c r="M113" s="9"/>
+      <c r="N113" s="9"/>
+      <c r="O113" s="9"/>
+      <c r="P113" s="9"/>
+      <c r="Q113" s="9"/>
+      <c r="R113" s="21"/>
+    </row>
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A114" s="20"/>
+      <c r="B114" s="9"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
+      <c r="G114" s="9"/>
+      <c r="H114" s="9"/>
+      <c r="I114" s="9"/>
+      <c r="J114" s="9"/>
+      <c r="K114" s="9"/>
+      <c r="L114" s="9"/>
+      <c r="M114" s="9"/>
+      <c r="N114" s="9"/>
+      <c r="O114" s="9"/>
+      <c r="P114" s="9"/>
+      <c r="Q114" s="9"/>
+      <c r="R114" s="21"/>
+    </row>
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A115" s="20"/>
+      <c r="B115" s="9"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="9"/>
+      <c r="H115" s="9"/>
+      <c r="I115" s="9"/>
+      <c r="J115" s="9"/>
+      <c r="K115" s="9"/>
+      <c r="L115" s="9"/>
+      <c r="M115" s="9"/>
+      <c r="N115" s="9"/>
+      <c r="O115" s="9"/>
+      <c r="P115" s="9"/>
+      <c r="Q115" s="9"/>
+      <c r="R115" s="21"/>
+    </row>
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A116" s="20"/>
+      <c r="B116" s="9"/>
+      <c r="C116" s="9"/>
+      <c r="D116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
+      <c r="G116" s="9"/>
+      <c r="H116" s="9"/>
+      <c r="I116" s="9"/>
+      <c r="J116" s="9"/>
+      <c r="K116" s="9"/>
+      <c r="L116" s="9"/>
+      <c r="M116" s="9"/>
+      <c r="N116" s="9"/>
+      <c r="O116" s="9"/>
+      <c r="P116" s="9"/>
+      <c r="Q116" s="9"/>
+      <c r="R116" s="21"/>
+    </row>
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A117" s="20"/>
+      <c r="B117" s="9"/>
+      <c r="C117" s="9"/>
+      <c r="D117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
+      <c r="G117" s="9"/>
+      <c r="H117" s="9"/>
+      <c r="I117" s="9"/>
+      <c r="J117" s="9"/>
+      <c r="K117" s="9"/>
+      <c r="L117" s="9"/>
+      <c r="M117" s="9"/>
+      <c r="N117" s="9"/>
+      <c r="O117" s="9"/>
+      <c r="P117" s="9"/>
+      <c r="Q117" s="9"/>
+      <c r="R117" s="21"/>
+    </row>
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A118" s="20"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
+      <c r="G118" s="9"/>
+      <c r="H118" s="9"/>
+      <c r="I118" s="9"/>
+      <c r="J118" s="9"/>
+      <c r="K118" s="9"/>
+      <c r="L118" s="9"/>
+      <c r="M118" s="9"/>
+      <c r="N118" s="9"/>
+      <c r="O118" s="9"/>
+      <c r="P118" s="9"/>
+      <c r="Q118" s="9"/>
+      <c r="R118" s="21"/>
+    </row>
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A119" s="20"/>
+      <c r="B119" s="9"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
+      <c r="G119" s="9"/>
+      <c r="H119" s="9"/>
+      <c r="I119" s="9"/>
+      <c r="J119" s="9"/>
+      <c r="K119" s="9"/>
+      <c r="L119" s="9"/>
+      <c r="M119" s="9"/>
+      <c r="N119" s="9"/>
+      <c r="O119" s="9"/>
+      <c r="P119" s="9"/>
+      <c r="Q119" s="9"/>
+      <c r="R119" s="21"/>
+    </row>
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A120" s="20"/>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
+      <c r="G120" s="9"/>
+      <c r="H120" s="9"/>
+      <c r="I120" s="9"/>
+      <c r="J120" s="9"/>
+      <c r="K120" s="9"/>
+      <c r="L120" s="9"/>
+      <c r="M120" s="9"/>
+      <c r="N120" s="9"/>
+      <c r="O120" s="9"/>
+      <c r="P120" s="9"/>
+      <c r="Q120" s="9"/>
+      <c r="R120" s="21"/>
+    </row>
+    <row r="121" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="22"/>
+      <c r="B121" s="23"/>
+      <c r="C121" s="23"/>
+      <c r="D121" s="23"/>
+      <c r="E121" s="23"/>
+      <c r="F121" s="23"/>
+      <c r="G121" s="23"/>
+      <c r="H121" s="23"/>
+      <c r="I121" s="23"/>
+      <c r="J121" s="23"/>
+      <c r="K121" s="23"/>
+      <c r="L121" s="23"/>
+      <c r="M121" s="23"/>
+      <c r="N121" s="23"/>
+      <c r="O121" s="23"/>
+      <c r="P121" s="23"/>
+      <c r="Q121" s="23"/>
+      <c r="R121" s="24"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A6DC166-3C5B-44B6-AADB-1BB724337B91}">
   <dimension ref="A2:J35"/>
@@ -20582,8 +22452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EAAD77A-9F44-48F8-9088-AEEE6B84E767}">
   <dimension ref="A4:R187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>